<commit_message>
12/18/2018-19:04:31 -> NO COMMENT
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MeleeGame\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D727B0B-D58C-45EC-89BF-35CBA387E328}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moves" sheetId="1" r:id="rId1"/>
@@ -18,7 +24,7 @@
     <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet5" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -328,9 +334,6 @@
     <t>Staff (twohand)</t>
   </si>
   <si>
-    <t>Small Shield (Buckler, etc…)</t>
-  </si>
-  <si>
     <t>Offhand Only, Knockback 5ft on Hit</t>
   </si>
   <si>
@@ -408,11 +411,14 @@
   <si>
     <t>Composure</t>
   </si>
+  <si>
+    <t>Small Shield (Small Buckler, etc…)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -682,23 +688,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,6 +707,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,6 +799,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -840,7 +849,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,9 +882,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -908,6 +934,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1083,7 +1126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -1209,7 +1252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1765,10 +1808,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
@@ -1817,10 +1860,10 @@
         <f t="shared" ref="C2:C9" si="0">IF(B2&gt;10,ROUNDDOWN((B2-10)/2,0),ROUNDUP((B2-10)/2,0))</f>
         <v>0</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="43">
         <f>IF(($C2+$C3)&gt;0,$C2+$C3+10,10)</f>
         <v>11</v>
       </c>
@@ -1836,8 +1879,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
@@ -1850,10 +1893,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="43">
         <f>IF(($C4+$C5)&gt;0,$C4+$C5+10,10)</f>
         <v>13</v>
       </c>
@@ -1869,12 +1912,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <f>IF(($C5+$C6)&gt;0,$C5+$C6+10,10)</f>
         <v>14</v>
       </c>
@@ -1890,15 +1933,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="43">
         <f>IF(($C6+$C7)&gt;0,$C6+$C7+10,10)</f>
         <v>15</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="43"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -1911,12 +1954,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="G7" s="44">
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="43">
         <f>IF(($C7+$C8)&gt;0,$C7+$C8+10,10)</f>
         <v>16</v>
       </c>
@@ -1932,15 +1975,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="43">
         <f>IF(($C8+$C9)&gt;0,$C8+$C9+10,10)</f>
         <v>17</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
@@ -1953,11 +1996,16 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
@@ -1965,11 +2013,6 @@
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1981,7 +2024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3867,7 +3910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5753,7 +5796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8083,7 +8126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -9968,16 +10011,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="13"/>
@@ -10044,14 +10087,14 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="51">
         <f>2*C2+ROUND(2.5*E2,0)+ROUND(0.75*E3,0)+3*F2+2*F3+((G2-2)+(G3-2))+D2+D3</f>
         <v>10</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="51">
         <v>0</v>
       </c>
       <c r="D2" s="19">
@@ -10094,20 +10137,20 @@
         <f t="shared" ref="N2:N41" si="6">IF($E2=0, ROUNDUP(100/($H2/2),0), ROUNDUP((100-ROUNDUP(30/$E2,0)*$H2/2)/$H2,0)+ROUNDUP(30/$E2,0))</f>
         <v>200</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="48" t="s">
+      <c r="P2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="48" t="s">
+      <c r="Q2" s="52" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="23">
         <v>1</v>
       </c>
@@ -10148,19 +10191,19 @@
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="50">
+      <c r="B4" s="47">
         <f>2*C4+ROUND(2.5*E4,0)+ROUND(0.75*E5,0)+3*F4+2*F5+((G4-2)+(G5-2))+D4+D5</f>
         <v>22</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="48">
         <v>1</v>
       </c>
       <c r="D4" s="28">
@@ -10203,20 +10246,20 @@
         <f t="shared" si="6"/>
         <v>67</v>
       </c>
-      <c r="O4" s="52" t="s">
+      <c r="O4" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="52" t="s">
+      <c r="P4" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="52" t="s">
+      <c r="Q4" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="30">
         <v>2</v>
       </c>
@@ -10257,19 +10300,19 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
     </row>
     <row r="6" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="51">
         <f>2*C6+ROUND(2.5*E6,0)+ROUND(0.75*E7,0)+3*F6+2*F7+((G6-2)+(G7-2))+D6+D7</f>
         <v>28</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="51">
         <v>2</v>
       </c>
       <c r="D6" s="19">
@@ -10312,20 +10355,20 @@
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="48" t="s">
+      <c r="P6" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="48" t="s">
+      <c r="Q6" s="52" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="23">
         <v>3</v>
       </c>
@@ -10366,19 +10409,19 @@
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52"/>
+      <c r="Q7" s="52"/>
     </row>
     <row r="8" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="50">
+      <c r="B8" s="47">
         <f>2*C8+ROUND(2.5*E8,0)+ROUND(0.75*E9,0)+3*F8+2*F9+((G8-2)+(G9-2))+D8+D9</f>
         <v>28</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="48">
         <v>1</v>
       </c>
       <c r="D8" s="28">
@@ -10421,20 +10464,20 @@
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O8" s="52" t="s">
+      <c r="O8" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="P8" s="52" t="s">
+      <c r="P8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="Q8" s="52" t="s">
+      <c r="Q8" s="49" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="30">
         <v>2</v>
       </c>
@@ -10475,19 +10518,19 @@
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
     </row>
     <row r="10" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="51">
         <f>2*C10+ROUND(2.5*E10,0)+ROUND(0.75*E11,0)+3*F10+2*F11+((G10-2)+(G11-2))+D10+D11</f>
         <v>28</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="51">
         <v>1</v>
       </c>
       <c r="D10" s="19">
@@ -10530,20 +10573,20 @@
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O10" s="48" t="s">
+      <c r="O10" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="P10" s="48" t="s">
+      <c r="P10" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="Q10" s="48" t="s">
+      <c r="Q10" s="52" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="23">
         <v>2</v>
       </c>
@@ -10584,19 +10627,19 @@
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
     </row>
     <row r="12" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="50">
+      <c r="B12" s="47">
         <f>2*C12+ROUND(2.5*E12,0)+ROUND(0.75*E13,0)+3*F12+2*F13+((G12-2)+(G13-2))+D12+D13</f>
         <v>33</v>
       </c>
-      <c r="C12" s="51">
+      <c r="C12" s="48">
         <v>2</v>
       </c>
       <c r="D12" s="28">
@@ -10639,20 +10682,20 @@
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O12" s="52" t="s">
+      <c r="O12" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="P12" s="52" t="s">
+      <c r="P12" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q12" s="52" t="s">
+      <c r="Q12" s="49" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="30">
         <v>4</v>
       </c>
@@ -10693,19 +10736,19 @@
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="50">
+      <c r="B14" s="47">
         <f>2*C14+ROUND(2.5*E14,0)+ROUND(0.75*E15,0)+3*F14+2*F15+((G14-2)+(G15-2))+D14+D15</f>
         <v>41</v>
       </c>
-      <c r="C14" s="51">
+      <c r="C14" s="48">
         <v>3</v>
       </c>
       <c r="D14" s="28">
@@ -10748,14 +10791,14 @@
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="30">
         <v>5</v>
       </c>
@@ -10796,19 +10839,19 @@
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
     </row>
     <row r="16" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="51">
         <f>2*C16+ROUND(2.5*E16,0)+ROUND(0.75*E17,0)+3*F16+2*F17+((G16-2)+(G17-2))+D16+D17</f>
         <v>33</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="51">
         <v>1</v>
       </c>
       <c r="D16" s="19">
@@ -10851,20 +10894,20 @@
         <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="O16" s="48" t="s">
+      <c r="O16" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="48" t="s">
+      <c r="P16" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="Q16" s="48" t="s">
+      <c r="Q16" s="52" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="23">
         <v>2</v>
       </c>
@@ -10905,19 +10948,19 @@
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="51">
         <f>2*C18+ROUND(2.5*E18,0)+ROUND(0.75*E19,0)+3*F18+2*F19+((G18-2)+(G19-2))+D18+D19</f>
         <v>41</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="51">
         <v>2</v>
       </c>
       <c r="D18" s="19">
@@ -10960,14 +11003,14 @@
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="23">
         <v>3</v>
       </c>
@@ -11008,19 +11051,19 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
+      <c r="O19" s="52"/>
+      <c r="P19" s="52"/>
+      <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="47">
         <f>2*C20+ROUND(2.5*E20,0)+ROUND(0.75*E21,0)+3*F20+2*F21+((G20-2)+(G21-2))+D20+D21</f>
         <v>33</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="48">
         <v>1</v>
       </c>
       <c r="D20" s="28">
@@ -11063,20 +11106,20 @@
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="O20" s="52" t="s">
+      <c r="O20" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="P20" s="52" t="s">
+      <c r="P20" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q20" s="52" t="s">
+      <c r="Q20" s="49" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="30">
         <v>2</v>
       </c>
@@ -11117,19 +11160,19 @@
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="O21" s="52"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="52"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="A22" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="50">
+      <c r="B22" s="47">
         <f>2*C22+ROUND(2.5*E22,0)+ROUND(0.75*E23,0)+3*F22+2*F23+((G22-2)+(G23-2))+D22+D23</f>
         <v>42</v>
       </c>
-      <c r="C22" s="51">
+      <c r="C22" s="48">
         <v>2</v>
       </c>
       <c r="D22" s="28">
@@ -11172,14 +11215,14 @@
         <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="O22" s="52"/>
-      <c r="P22" s="52"/>
-      <c r="Q22" s="52"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="51"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="30">
         <v>4</v>
       </c>
@@ -11220,19 +11263,19 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
+      <c r="Q23" s="49"/>
     </row>
     <row r="24" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="47">
+      <c r="B24" s="51">
         <f>2*C24+ROUND(2.5*E24,0)+ROUND(0.75*E25,0)+3*F24+2*F25+((G24-2)+(G25-2))+D24+D25</f>
         <v>42</v>
       </c>
-      <c r="C24" s="47">
+      <c r="C24" s="51">
         <v>2</v>
       </c>
       <c r="D24" s="19">
@@ -11275,20 +11318,20 @@
         <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="O24" s="48" t="s">
+      <c r="O24" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="P24" s="48" t="s">
+      <c r="P24" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="Q24" s="48" t="s">
+      <c r="Q24" s="52" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="23">
         <v>5</v>
       </c>
@@ -11329,19 +11372,19 @@
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="O25" s="48"/>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
+      <c r="O25" s="52"/>
+      <c r="P25" s="52"/>
+      <c r="Q25" s="52"/>
     </row>
     <row r="26" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="50">
+      <c r="B26" s="47">
         <f>2*C26+ROUND(2.5*E26,0)+ROUND(0.75*E27,0)+3*F26+2*F27+((G26-2)+(G27-2))+D26+D27</f>
         <v>44</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="48">
         <v>1</v>
       </c>
       <c r="D26" s="28">
@@ -11384,20 +11427,20 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="O26" s="52" t="s">
+      <c r="O26" s="49" t="s">
         <v>81</v>
       </c>
       <c r="P26" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="Q26" s="52" t="s">
+      <c r="Q26" s="49" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="51"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="48"/>
       <c r="D27" s="30">
         <v>2</v>
       </c>
@@ -11438,19 +11481,19 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="O27" s="52"/>
+      <c r="O27" s="49"/>
       <c r="P27" s="53"/>
-      <c r="Q27" s="52"/>
+      <c r="Q27" s="49"/>
     </row>
     <row r="28" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="47">
+      <c r="B28" s="51">
         <f>2*C28+ROUND(2.5*E28,0)+ROUND(0.75*E29,0)+3*F28+2*F29+((G28-2)+(G29-2))+D28+D29</f>
         <v>43</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="51">
         <v>1</v>
       </c>
       <c r="D28" s="19">
@@ -11493,20 +11536,20 @@
         <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="O28" s="48" t="s">
+      <c r="O28" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="P28" s="48" t="s">
+      <c r="P28" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="Q28" s="48" t="s">
+      <c r="Q28" s="52" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="23">
         <v>4</v>
       </c>
@@ -11547,19 +11590,19 @@
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="O29" s="48"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
     </row>
     <row r="30" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="50">
+      <c r="B30" s="47">
         <f>2*C30+ROUND(2.5*E30,0)+ROUND(0.75*E31,0)+3*F30+2*F31+((G30-2)+(G31-2))+D30+D31</f>
         <v>24</v>
       </c>
-      <c r="C30" s="51">
+      <c r="C30" s="48">
         <v>1</v>
       </c>
       <c r="D30" s="28">
@@ -11602,20 +11645,20 @@
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="O30" s="52" t="s">
+      <c r="O30" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="P30" s="52" t="s">
+      <c r="P30" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="Q30" s="52" t="s">
+      <c r="Q30" s="49" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="30">
         <v>2</v>
       </c>
@@ -11656,19 +11699,19 @@
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="O31" s="52"/>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="52"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+      <c r="A32" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="B32" s="50">
+      <c r="B32" s="47">
         <f>2*C32+ROUND(2.5*E32,0)+ROUND(0.75*E33,0)+3*F32+2*F33+((G32-2)+(G33-2))+D32+D33</f>
         <v>34</v>
       </c>
-      <c r="C32" s="51">
+      <c r="C32" s="48">
         <v>3</v>
       </c>
       <c r="D32" s="28">
@@ -11711,14 +11754,14 @@
         <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="O32" s="52"/>
-      <c r="P32" s="52"/>
-      <c r="Q32" s="52"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="49"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="51"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="30">
         <v>4</v>
       </c>
@@ -11759,19 +11802,19 @@
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="O33" s="52"/>
-      <c r="P33" s="52"/>
-      <c r="Q33" s="52"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
     </row>
     <row r="34" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="47">
+      <c r="B34" s="51">
         <f>2*C34+ROUND(2.5*E34,0)+ROUND(0.75*E35,0)+3*F34+2*F35+((G34-2)+(G35-2))+D34+D35</f>
         <v>29</v>
       </c>
-      <c r="C34" s="47">
+      <c r="C34" s="51">
         <v>1</v>
       </c>
       <c r="D34" s="19">
@@ -11814,20 +11857,20 @@
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O34" s="48" t="s">
+      <c r="O34" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="P34" s="48" t="s">
+      <c r="P34" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="Q34" s="48" t="s">
+      <c r="Q34" s="52" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="23">
         <v>3</v>
       </c>
@@ -11868,19 +11911,19 @@
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="O35" s="48"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="47">
+      <c r="B36" s="51">
         <f>2*C36+ROUND(2.5*E36,0)+ROUND(0.75*E37,0)+3*F36+2*F37+((G36-2)+(G37-2))+D36+D37</f>
         <v>41</v>
       </c>
-      <c r="C36" s="47">
+      <c r="C36" s="51">
         <v>3</v>
       </c>
       <c r="D36" s="19">
@@ -11923,14 +11966,14 @@
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
+      <c r="A37" s="50"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
       <c r="D37" s="23">
         <v>5</v>
       </c>
@@ -11971,19 +12014,19 @@
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="O37" s="48"/>
-      <c r="P37" s="48"/>
-      <c r="Q37" s="48"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="52"/>
     </row>
     <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="50">
+      <c r="B38" s="47">
         <f>2*C38+ROUND(2.5*E38,0)+ROUND(0.75*E39,0)+3*F38+2*F39+((G38-2)+(G39-2))+D38+D39</f>
         <v>19</v>
       </c>
-      <c r="C38" s="51">
+      <c r="C38" s="48">
         <v>1</v>
       </c>
       <c r="D38" s="28">
@@ -12026,20 +12069,20 @@
         <f t="shared" si="6"/>
         <v>67</v>
       </c>
-      <c r="O38" s="52" t="s">
+      <c r="O38" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="P38" s="52" t="s">
+      <c r="P38" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q38" s="52" t="s">
+      <c r="Q38" s="49" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="51"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="48"/>
       <c r="D39" s="30">
         <v>2</v>
       </c>
@@ -12080,19 +12123,19 @@
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" s="49" t="s">
+      <c r="A40" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="50">
+      <c r="B40" s="47">
         <f>2*C40+ROUND(2.5*E40,0)+ROUND(0.75*E41,0)+3*F40+2*F41+((G40-2)+(G41-2))+D40+D41</f>
         <v>29</v>
       </c>
-      <c r="C40" s="51">
+      <c r="C40" s="48">
         <v>3</v>
       </c>
       <c r="D40" s="28">
@@ -12135,14 +12178,14 @@
         <f t="shared" si="6"/>
         <v>67</v>
       </c>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="51"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="30">
         <v>4</v>
       </c>
@@ -12183,13 +12226,13 @@
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
     </row>
     <row r="44" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="B44" s="18">
         <f>2*C44+ROUND(2.5*E44,0)+F44+((G44-2)+D44)</f>
@@ -12242,7 +12285,7 @@
         <v>66</v>
       </c>
       <c r="P44" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q44" s="35" t="s">
         <v>64</v>
@@ -12250,7 +12293,7 @@
     </row>
     <row r="45" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="26">
         <f>2*C45+ROUND(2.5*E45,0)+F45+((G45-2)+D45)</f>
@@ -12303,7 +12346,7 @@
         <v>66</v>
       </c>
       <c r="P45" s="38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q45" s="38" t="s">
         <v>64</v>
@@ -12311,7 +12354,7 @@
     </row>
     <row r="46" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" s="18">
         <f>2*C46+ROUND(2.5*E46,0)+F46+((G46-2)+D46)</f>
@@ -12364,7 +12407,7 @@
         <v>71</v>
       </c>
       <c r="P46" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q46" s="22" t="s">
         <v>64</v>
@@ -12372,24 +12415,75 @@
     </row>
   </sheetData>
   <mergeCells count="102">
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="O38:O41"/>
-    <mergeCell ref="P38:P41"/>
-    <mergeCell ref="Q38:Q41"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="O34:O37"/>
-    <mergeCell ref="P34:P37"/>
-    <mergeCell ref="Q34:Q37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="P12:P15"/>
+    <mergeCell ref="Q12:Q15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="O16:O19"/>
+    <mergeCell ref="P16:P19"/>
+    <mergeCell ref="Q16:Q19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="O20:O23"/>
+    <mergeCell ref="P20:P23"/>
+    <mergeCell ref="Q20:Q23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="Q26:Q27"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="C28:C29"/>
@@ -12405,75 +12499,24 @@
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="O20:O23"/>
-    <mergeCell ref="P20:P23"/>
-    <mergeCell ref="Q20:Q23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="O16:O19"/>
-    <mergeCell ref="P16:P19"/>
-    <mergeCell ref="Q16:Q19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="P12:P15"/>
-    <mergeCell ref="Q12:Q15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="O34:O37"/>
+    <mergeCell ref="P34:P37"/>
+    <mergeCell ref="Q34:Q37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="O38:O41"/>
+    <mergeCell ref="P38:P41"/>
+    <mergeCell ref="Q38:Q41"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -12485,11 +12528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12506,30 +12549,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="C1" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="D1" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>105</v>
-      </c>
-      <c r="G1" s="40" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="41">
         <v>10</v>
@@ -12538,21 +12581,21 @@
         <v>0</v>
       </c>
       <c r="D2" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>109</v>
-      </c>
       <c r="F2" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G2" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="42">
         <v>15</v>
@@ -12561,21 +12604,21 @@
         <v>0</v>
       </c>
       <c r="D3" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="42" t="s">
-        <v>109</v>
-      </c>
       <c r="F3" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="41">
         <v>20</v>
@@ -12584,21 +12627,21 @@
         <v>0</v>
       </c>
       <c r="D4" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>109</v>
-      </c>
       <c r="F4" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="42">
         <v>30</v>
@@ -12613,15 +12656,15 @@
         <v>66</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="41">
         <v>15</v>
@@ -12636,13 +12679,13 @@
         <v>66</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="41"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="42">
         <v>30</v>
@@ -12657,15 +12700,15 @@
         <v>66</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8" s="41">
         <v>20</v>
@@ -12680,15 +12723,15 @@
         <v>66</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="42">
         <v>30</v>
@@ -12700,18 +12743,18 @@
         <v>12</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="41">
         <v>40</v>
@@ -12723,18 +12766,18 @@
         <v>12</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B11" s="42">
         <v>50</v>
@@ -12746,18 +12789,18 @@
         <v>12</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" s="41">
         <v>60</v>
@@ -12769,13 +12812,13 @@
         <v>12</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -12789,7 +12832,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Weapons and Armor 5, progress. Now leading method
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Moves" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,8 +22,11 @@
     <sheet name="Armor Layering 3.0" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Weapons 4.0" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Armor 4.0" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Sheet2" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Sheet5" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Weapons 5.0" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Armor 5.0" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Weapon 5.0 (Table)" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Sheet2" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Sheet5" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="186">
   <si>
     <t xml:space="preserve">Moves</t>
   </si>
@@ -512,6 +515,108 @@
   <si>
     <t xml:space="preserve">Full Plate Mail Set</t>
   </si>
+  <si>
+    <t xml:space="preserve">Concentration cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concealable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide Overcoat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain Mail  Hauberk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Certain Backgrounds may allow starting with this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dice Numb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dice Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Lethal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Lethal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Lethal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Lethal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Pain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Lethal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pain Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lethal Threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club/Improvised Weapon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand Axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longsword (One Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longsword (Two Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WarHammer (One Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WarHammer (Two Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battle Axe (One Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battle Axe (Two Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Hammer</t>
+  </si>
 </sst>
 </file>
 
@@ -522,12 +627,11 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -546,10 +650,60 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -557,10 +711,28 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -569,8 +741,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFBCE4E5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFDCE6F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDCE6F2"/>
-        <bgColor rgb="FFBCE4E5"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -591,13 +805,34 @@
         <bgColor rgb="FFDCE6F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -741,7 +976,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -765,8 +1000,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -783,7 +1069,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,7 +1077,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -803,132 +1089,128 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -943,47 +1225,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -991,15 +1277,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1007,88 +1293,113 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1097,7 +1408,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFBCE4E5"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1107,13 +1418,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFBCE4E5"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1183,16 +1494,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="R1:S2 B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -1313,14 +1624,14 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="1" sqref="R1:S2 I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
@@ -3902,15 +4213,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="R1:S2 E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
@@ -4187,7 +4498,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="R1:S2 E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4196,7 +4507,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.7"/>
@@ -6666,15 +6977,15 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="R1:S2 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
@@ -8187,14 +8498,14 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="R1:S2 B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="11.99"/>
@@ -8465,401 +8776,1511 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="R1:S2 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="40.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="2" width="40.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="n">
+    <row r="1" s="2" customFormat="true" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="66" t="n">
+        <f aca="false">IF(C2="Light",E2,E2+$W$2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="49" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" s="49" t="n">
+        <f aca="false">H2+F2</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="49" t="n">
+        <f aca="false">H2*(I2/2)+F2</f>
+        <v>2.5</v>
+      </c>
+      <c r="L2" s="49" t="n">
+        <f aca="false">H2*I2+F2</f>
+        <v>5</v>
+      </c>
+      <c r="M2" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K2,0)</f>
+        <v>20</v>
+      </c>
+      <c r="N2" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K2,0)</f>
+        <v>40</v>
+      </c>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="70" t="n">
+        <f aca="false">IF(C3="Light",E3,E3+$W$2)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="71" t="n">
+        <f aca="false">H3+F3</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="71" t="n">
+        <f aca="false">H3*(I3/2)+F3</f>
+        <v>5</v>
+      </c>
+      <c r="L3" s="71" t="n">
+        <f aca="false">H3*I3+F3</f>
+        <v>10</v>
+      </c>
+      <c r="M3" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K3,0)</f>
+        <v>10</v>
+      </c>
+      <c r="N3" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K3,0)</f>
+        <v>20</v>
+      </c>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="66" t="n">
+        <f aca="false">IF(C4="Light",E4,E4+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G4" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J4" s="49" t="n">
+        <f aca="false">H4+F4</f>
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="K4" s="49" t="n">
+        <f aca="false">H4*(I4/2)+F4</f>
+        <v>6</v>
+      </c>
+      <c r="L4" s="49" t="n">
+        <f aca="false">H4*I4+F4</f>
+        <v>11</v>
+      </c>
+      <c r="M4" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K4,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N4" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K4,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="69" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="70" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="70" t="n">
+        <f aca="false">IF(C5="Light",E5,E5+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J5" s="71" t="n">
+        <f aca="false">H5+F5</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="71" t="n">
+        <f aca="false">H5*(I5/2)+F5</f>
+        <v>6</v>
+      </c>
+      <c r="L5" s="71" t="n">
+        <f aca="false">H5*I5+F5</f>
+        <v>11</v>
+      </c>
+      <c r="M5" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K5,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N5" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K5,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O5" s="71"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="66" t="n">
+        <f aca="false">IF(C6="Light",E6,E6+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" s="49" t="n">
+        <f aca="false">H6+F6</f>
+        <v>2</v>
+      </c>
+      <c r="K6" s="49" t="n">
+        <f aca="false">H6*(I6/2)+F6</f>
+        <v>6</v>
+      </c>
+      <c r="L6" s="49" t="n">
+        <f aca="false">H6*I6+F6</f>
+        <v>11</v>
+      </c>
+      <c r="M6" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K6,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N6" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K6,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="70" t="n">
+        <f aca="false">IF(C7="Light",E7,E7+$W$2)</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J7" s="71" t="n">
+        <f aca="false">H7+F7</f>
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="K7" s="71" t="n">
+        <f aca="false">H7*(I7/2)+F7</f>
+        <v>7</v>
+      </c>
+      <c r="L7" s="71" t="n">
+        <f aca="false">H7*I7+F7</f>
+        <v>12</v>
+      </c>
+      <c r="M7" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K7,0)</f>
+        <v>8</v>
+      </c>
+      <c r="N7" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K7,0)</f>
+        <v>15</v>
+      </c>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="65" t="n">
+        <v>10</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="66" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="66" t="n">
+        <f aca="false">IF(C8="Light",E8,E8+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J8" s="49" t="n">
+        <f aca="false">H8+F8</f>
+        <v>2</v>
+      </c>
+      <c r="K8" s="49" t="n">
+        <f aca="false">H8*(I8/2)+F8</f>
+        <v>6</v>
+      </c>
+      <c r="L8" s="49" t="n">
+        <f aca="false">H8*I8+F8</f>
+        <v>11</v>
+      </c>
+      <c r="M8" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K8,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N8" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K8,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="65" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="66" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" s="66" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="66" t="n">
+        <f aca="false">IF(C9="Light",E9,E9+$W$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J9" s="49" t="n">
+        <f aca="false">H9+F9</f>
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="K9" s="49" t="n">
+        <f aca="false">H9*(I9/2)+F9</f>
+        <v>8</v>
+      </c>
+      <c r="L9" s="49" t="n">
+        <f aca="false">H9*I9+F9</f>
+        <v>13</v>
+      </c>
+      <c r="M9" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K9,0)</f>
+        <v>7</v>
+      </c>
+      <c r="N9" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K9,0)</f>
+        <v>13</v>
+      </c>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="67"/>
+      <c r="R9" s="67"/>
+      <c r="S9" s="23"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="n">
+      <c r="C10" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="70" t="n">
+        <f aca="false">IF(C10="Light",E10,E10+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="70" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J10" s="71" t="n">
+        <f aca="false">H10+F10</f>
+        <v>2</v>
+      </c>
+      <c r="K10" s="71" t="n">
+        <f aca="false">H10*(I10/2)+F10</f>
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="n">
+      <c r="L10" s="71" t="n">
+        <f aca="false">H10*I10+F10</f>
+        <v>11</v>
+      </c>
+      <c r="M10" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K10,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N10" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K10,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="R10" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="69" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="70" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="70" t="n">
+        <f aca="false">IF(C11="Light",E11,E11+$W$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G11" s="70" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J11" s="71" t="n">
+        <f aca="false">H11+F11</f>
+        <v>4</v>
+      </c>
+      <c r="K11" s="71" t="n">
+        <f aca="false">H11*(I11/2)+F11</f>
+        <v>8</v>
+      </c>
+      <c r="L11" s="71" t="n">
+        <f aca="false">H11*I11+F11</f>
+        <v>13</v>
+      </c>
+      <c r="M11" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K11,0)</f>
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="n">
+      <c r="N11" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K11,0)</f>
+        <v>13</v>
+      </c>
+      <c r="O11" s="71"/>
+      <c r="P11" s="71"/>
+      <c r="Q11" s="72"/>
+      <c r="R11" s="72"/>
+      <c r="S11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C12" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="66" t="n">
+        <f aca="false">IF(C12="Light",E12,E12+$W$2)</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" s="49" t="n">
+        <f aca="false">H12+F12</f>
+        <v>3</v>
+      </c>
+      <c r="K12" s="49" t="n">
+        <f aca="false">H12*(I12/2)+F12</f>
+        <v>7</v>
+      </c>
+      <c r="L12" s="49" t="n">
+        <f aca="false">H12*I12+F12</f>
+        <v>12</v>
+      </c>
+      <c r="M12" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K12,0)</f>
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="n">
+      <c r="N12" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K12,0)</f>
+        <v>15</v>
+      </c>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="R12" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="S12" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="65" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="66" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" s="66" t="n">
+        <f aca="false">IF(C13="Light",E13,E13+$W$2)</f>
+        <v>4</v>
+      </c>
+      <c r="G13" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J13" s="49" t="n">
+        <f aca="false">H13+F13</f>
+        <v>5</v>
+      </c>
+      <c r="K13" s="49" t="n">
+        <f aca="false">H13*(I13/2)+F13</f>
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="L13" s="49" t="n">
+        <f aca="false">H13*I13+F13</f>
+        <v>14</v>
+      </c>
+      <c r="M13" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K13,0)</f>
+        <v>6</v>
+      </c>
+      <c r="N13" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K13,0)</f>
+        <v>12</v>
+      </c>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="23"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="69" t="n">
+        <v>15</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="70" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="70" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" s="70" t="n">
+        <f aca="false">IF(C14="Light",E14,E14+$W$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G14" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J14" s="71" t="n">
+        <f aca="false">H14+F14</f>
+        <v>4</v>
+      </c>
+      <c r="K14" s="71" t="n">
+        <f aca="false">H14*(I14/2)+F14</f>
+        <v>8</v>
+      </c>
+      <c r="L14" s="71" t="n">
+        <f aca="false">H14*I14+F14</f>
+        <v>13</v>
+      </c>
+      <c r="M14" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K14,0)</f>
+        <v>7</v>
+      </c>
+      <c r="N14" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K14,0)</f>
+        <v>13</v>
+      </c>
+      <c r="O14" s="71"/>
+      <c r="P14" s="71"/>
+      <c r="Q14" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="R14" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="66" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="66" t="n">
+        <f aca="false">IF(C15="Light",E15,E15+$W$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G15" s="66" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="H15" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" s="49" t="n">
+        <f aca="false">H15+F15</f>
+        <v>4</v>
+      </c>
+      <c r="K15" s="49" t="n">
+        <f aca="false">H15*(I15/2)+F15</f>
+        <v>8</v>
+      </c>
+      <c r="L15" s="49" t="n">
+        <f aca="false">H15*I15+F15</f>
+        <v>13</v>
+      </c>
+      <c r="M15" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K15,0)</f>
+        <v>7</v>
+      </c>
+      <c r="N15" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K15,0)</f>
+        <v>13</v>
+      </c>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="70" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="70" t="n">
+        <f aca="false">IF(C16="Light",E16,E16+$W$2)</f>
+        <v>4</v>
+      </c>
+      <c r="G16" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J16" s="71" t="n">
+        <f aca="false">H16+F16</f>
+        <v>5</v>
+      </c>
+      <c r="K16" s="71" t="n">
+        <f aca="false">H16*(I16/2)+F16</f>
+        <v>9</v>
+      </c>
+      <c r="L16" s="71" t="n">
+        <f aca="false">H16*I16+F16</f>
+        <v>14</v>
+      </c>
+      <c r="M16" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K16,0)</f>
+        <v>6</v>
+      </c>
+      <c r="N16" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K16,0)</f>
+        <v>12</v>
+      </c>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="66" t="n">
+        <f aca="false">IF(C17="Light",E17,E17+$W$2)</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J17" s="49" t="n">
+        <f aca="false">H17+F17</f>
+        <v>2</v>
+      </c>
+      <c r="K17" s="49" t="n">
+        <f aca="false">H17*(I17/2)+F17</f>
+        <v>6</v>
+      </c>
+      <c r="L17" s="49" t="n">
+        <f aca="false">H17*I17+F17</f>
+        <v>11</v>
+      </c>
+      <c r="M17" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K17,0)</f>
+        <v>9</v>
+      </c>
+      <c r="N17" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K17,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="R17" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="S17" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="65" t="n">
+        <v>20</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="66" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="F18" s="66" t="n">
+        <f aca="false">IF(C18="Light",E18,E18+$W$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G18" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J18" s="49" t="n">
+        <f aca="false">H18+F18</f>
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="K18" s="49" t="n">
+        <f aca="false">H18*(I18/2)+F18</f>
+        <v>8</v>
+      </c>
+      <c r="L18" s="49" t="n">
+        <f aca="false">H18*I18+F18</f>
+        <v>13</v>
+      </c>
+      <c r="M18" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K18,0)</f>
+        <v>7</v>
+      </c>
+      <c r="N18" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K18,0)</f>
+        <v>13</v>
+      </c>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="23"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="69" t="n">
+        <v>15</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="70" t="n">
+        <v>4</v>
+      </c>
+      <c r="F19" s="70" t="n">
+        <f aca="false">IF(C19="Light",E19,E19+$W$2)</f>
+        <v>4</v>
+      </c>
+      <c r="G19" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="71" t="n">
+        <v>10</v>
+      </c>
+      <c r="J19" s="71" t="n">
+        <f aca="false">H19+F19</f>
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="K19" s="71" t="n">
+        <f aca="false">H19*(I19/2)+F19</f>
+        <v>9</v>
+      </c>
+      <c r="L19" s="71" t="n">
+        <f aca="false">H19*I19+F19</f>
+        <v>14</v>
+      </c>
+      <c r="M19" s="71" t="n">
+        <f aca="false">ROUNDUP(50/K19,0)</f>
         <v>6</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="N19" s="71" t="n">
+        <f aca="false">ROUNDUP(100/K19,0)</f>
+        <v>12</v>
+      </c>
+      <c r="O19" s="71"/>
+      <c r="P19" s="71"/>
+      <c r="Q19" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" s="72" t="s">
+        <v>78</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="65" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="66" t="n">
+        <f aca="false">IF(C20="Light",E20,E20+$W$2)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J20" s="49" t="n">
+        <f aca="false">H20+F20</f>
+        <v>1</v>
+      </c>
+      <c r="K20" s="49" t="n">
+        <f aca="false">H20*(I20/2)+F20</f>
+        <v>5</v>
+      </c>
+      <c r="L20" s="49" t="n">
+        <f aca="false">H20*I20+F20</f>
+        <v>10</v>
+      </c>
+      <c r="M20" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K20,0)</f>
+        <v>10</v>
+      </c>
+      <c r="N20" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K20,0)</f>
+        <v>20</v>
+      </c>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
+      <c r="Q20" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="R20" s="67" t="s">
+        <v>122</v>
+      </c>
+      <c r="S20" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="65" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="66" t="n">
+        <f aca="false">IF(C21="Light",E21,E21+$W$2)</f>
+        <v>2</v>
+      </c>
+      <c r="G21" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="J21" s="49" t="n">
+        <f aca="false">H21+F21</f>
+        <v>3</v>
+      </c>
+      <c r="K21" s="49" t="n">
+        <f aca="false">H21*(I21/2)+F21</f>
         <v>7</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="L21" s="49" t="n">
+        <f aca="false">H21*I21+F21</f>
+        <v>12</v>
+      </c>
+      <c r="M21" s="49" t="n">
+        <f aca="false">ROUNDUP(50/K21,0)</f>
         <v>8</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="N21" s="49" t="n">
+        <f aca="false">ROUNDUP(100/K21,0)</f>
+        <v>15</v>
+      </c>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="23"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="27" t="n">
+        <v>10</v>
+      </c>
+      <c r="J24" s="27" t="n">
+        <f aca="false">H24+F24</f>
+        <v>1</v>
+      </c>
+      <c r="K24" s="27" t="n">
+        <f aca="false">ROUNDUP(H24*(I24/2+0.5),0)</f>
+        <v>6</v>
+      </c>
+      <c r="L24" s="27" t="n">
+        <f aca="false">H24*I24</f>
+        <v>10</v>
+      </c>
+      <c r="M24" s="27" t="n">
+        <f aca="false">ROUNDUP(50/K24,0)</f>
         <v>9</v>
       </c>
-      <c r="J2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="N24" s="27" t="n">
+        <f aca="false">ROUNDUP(100/K24,0)</f>
+        <v>17</v>
+      </c>
+      <c r="O24" s="27" t="n">
+        <f aca="false">IF($F24=0, ROUNDUP(100/($K24/2),0), ROUNDUP((100-ROUNDUP(15/$F24,0)*$K24/2)/$K24,0)+ROUNDUP(15/$F24,0))</f>
+        <v>34</v>
+      </c>
+      <c r="P24" s="29" t="n">
+        <f aca="false">IF($F24=0, ROUNDUP(100/($K24/2),0), ROUNDUP((100-ROUNDUP(30/$F24,0)*$K24/2)/$K24,0)+ROUNDUP(30/$F24,0))</f>
+        <v>34</v>
+      </c>
+      <c r="Q24" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="R24" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="S24" s="30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="20" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="K11" s="0" t="n">
+      <c r="D25" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="32" t="n">
+        <f aca="false">H25+F25</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="32" t="n">
+        <f aca="false">ROUNDUP(H25*(I25/2+0.5),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="32" t="n">
+        <f aca="false">H25*I25</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="32" t="e">
+        <f aca="false">ROUNDUP(50/K25,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" s="32" t="e">
+        <f aca="false">ROUNDUP(100/K25,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" s="32" t="e">
+        <f aca="false">IF($F25=0, ROUNDUP(100/($K25/2),0), ROUNDUP((100-ROUNDUP(15/$F25,0)*$K25/2)/$K25,0)+ROUNDUP(15/$F25,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P25" s="32" t="e">
+        <f aca="false">IF($F25=0, ROUNDUP(100/($K25/2),0), ROUNDUP((100-ROUNDUP(30/$F25,0)*$K25/2)/$K25,0)+ROUNDUP(30/$F25,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q25" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="R25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="S25" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="11" t="n">
         <v>20</v>
       </c>
-    </row>
+      <c r="C26" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="11" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E26" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="35" t="n">
+        <f aca="false">H26+F26</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="35" t="n">
+        <f aca="false">ROUNDUP(H26*(I26/2+0.5),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="35" t="n">
+        <f aca="false">H26*I26</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="35" t="e">
+        <f aca="false">ROUNDUP(50/K26,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" s="35" t="e">
+        <f aca="false">ROUNDUP(100/K26,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" s="35" t="e">
+        <f aca="false">IF($F26=0, ROUNDUP(100/($K26/2),0), ROUNDUP((100-ROUNDUP(15/$F26,0)*$K26/2)/$K26,0)+ROUNDUP(15/$F26,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P26" s="35" t="e">
+        <f aca="false">IF($F26=0, ROUNDUP(100/($K26/2),0), ROUNDUP((100-ROUNDUP(30/$F26,0)*$K26/2)/$K26,0)+ROUNDUP(30/$F26,0))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="R26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="S26" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="R12:R13"/>
+    <mergeCell ref="S12:S13"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="R17:R18"/>
+    <mergeCell ref="S17:S18"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="S20:S21"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8875,10 +10296,1740 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="R1:S2 I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="42.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+    </row>
+    <row r="2" s="44" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="44" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R1:S2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="4" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="74" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="P1" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q1" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="e">
+        <f aca="false">IF(B2&gt;0,(1-_xlfn.BINOM.DIST(0,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E2" s="5" t="e">
+        <f aca="false">IF(B2&gt;0,(1-_xlfn.BINOM.DIST(0,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F2" s="5" t="e">
+        <f aca="false">=IF(B2&gt;1,(1-_xlfn.BINOM.DIST(1,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G2" s="5" t="e">
+        <f aca="false">IF(B2&gt;1,(1-_xlfn.BINOM.DIST(1,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <f aca="false">IF(B2&gt;2,(1-_xlfn.BINOM.DIST(2,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <f aca="false">IF(B2&gt;2,(1-_xlfn.BINOM.DIST(2,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <f aca="false">IF(B2&gt;3,(1-_xlfn.BINOM.DIST(3,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <f aca="false">IF(B2&gt;3,(1-_xlfn.BINOM.DIST(3,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <f aca="false">IF(B2&gt;4,(1-_xlfn.BINOM.DIST(4,$B2,($C2-$P$2+1)/$C2,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <f aca="false">IF(B2&gt;4,(1-_xlfn.BINOM.DIST(4,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <f aca="false">3+R2</f>
+        <v>7</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <f aca="false">5+R2</f>
+        <v>9</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <f aca="false">IF(B3&gt;0,(1-_xlfn.BINOM.DIST(0,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="5" t="e">
+        <f aca="false">IF(B3&gt;0,(1-_xlfn.BINOM.DIST(0,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <f aca="false">=IF(B3&gt;1,(1-_xlfn.BINOM.DIST(1,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="e">
+        <f aca="false">IF(B3&gt;1,(1-_xlfn.BINOM.DIST(1,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <f aca="false">IF(B3&gt;2,(1-_xlfn.BINOM.DIST(2,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">IF(B3&gt;2,(1-_xlfn.BINOM.DIST(2,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <f aca="false">IF(B3&gt;3,(1-_xlfn.BINOM.DIST(3,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <f aca="false">IF(B3&gt;3,(1-_xlfn.BINOM.DIST(3,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <f aca="false">IF(B3&gt;4,(1-_xlfn.BINOM.DIST(4,$B3,($C3-$P$2+1)/$C3,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <f aca="false">IF(B3&gt;4,(1-_xlfn.BINOM.DIST(4,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <f aca="false">IF(B4&gt;0,(1-_xlfn.BINOM.DIST(0,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
+        <v>0.578125</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">IF(B4&gt;0,(1-_xlfn.BINOM.DIST(0,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <f aca="false">=IF(B4&gt;1,(1-_xlfn.BINOM.DIST(1,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">IF(B4&gt;1,(1-_xlfn.BINOM.DIST(1,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <f aca="false">IF(B4&gt;2,(1-_xlfn.BINOM.DIST(2,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">IF(B4&gt;2,(1-_xlfn.BINOM.DIST(2,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <f aca="false">IF(B4&gt;3,(1-_xlfn.BINOM.DIST(3,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <f aca="false">IF(B4&gt;3,(1-_xlfn.BINOM.DIST(3,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <f aca="false">IF(B4&gt;4,(1-_xlfn.BINOM.DIST(4,$B4,($C4-$P$2+1)/$C4,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <f aca="false">IF(B4&gt;4,(1-_xlfn.BINOM.DIST(4,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <f aca="false">IF(B5&gt;0,(1-_xlfn.BINOM.DIST(0,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
+        <v>0.578125</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <f aca="false">IF(B5&gt;0,(1-_xlfn.BINOM.DIST(0,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <f aca="false">=IF(B5&gt;1,(1-_xlfn.BINOM.DIST(1,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">IF(B5&gt;1,(1-_xlfn.BINOM.DIST(1,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <f aca="false">IF(B5&gt;2,(1-_xlfn.BINOM.DIST(2,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <f aca="false">IF(B5&gt;2,(1-_xlfn.BINOM.DIST(2,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <f aca="false">IF(B5&gt;3,(1-_xlfn.BINOM.DIST(3,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <f aca="false">IF(B5&gt;3,(1-_xlfn.BINOM.DIST(3,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <f aca="false">IF(B5&gt;4,(1-_xlfn.BINOM.DIST(4,$B5,($C5-$P$2+1)/$C5,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <f aca="false">IF(B5&gt;4,(1-_xlfn.BINOM.DIST(4,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <f aca="false">IF(B6&gt;0,(1-_xlfn.BINOM.DIST(0,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <f aca="false">IF(B6&gt;0,(1-_xlfn.BINOM.DIST(0,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
+        <v>0.555555555555555</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <f aca="false">=IF(B6&gt;1,(1-_xlfn.BINOM.DIST(1,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">IF(B6&gt;1,(1-_xlfn.BINOM.DIST(1,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <f aca="false">IF(B6&gt;2,(1-_xlfn.BINOM.DIST(2,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <f aca="false">IF(B6&gt;2,(1-_xlfn.BINOM.DIST(2,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <f aca="false">IF(B6&gt;3,(1-_xlfn.BINOM.DIST(3,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <f aca="false">IF(B6&gt;3,(1-_xlfn.BINOM.DIST(3,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <f aca="false">IF(B6&gt;4,(1-_xlfn.BINOM.DIST(4,$B6,($C6-$P$2+1)/$C6,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <f aca="false">IF(B6&gt;4,(1-_xlfn.BINOM.DIST(4,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <f aca="false">IF(B7&gt;0,(1-_xlfn.BINOM.DIST(0,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
+        <v>0.784</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <f aca="false">IF(B7&gt;0,(1-_xlfn.BINOM.DIST(0,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
+        <v>0.488</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <f aca="false">=IF(B7&gt;1,(1-_xlfn.BINOM.DIST(1,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
+        <v>0.352</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <f aca="false">IF(B7&gt;1,(1-_xlfn.BINOM.DIST(1,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
+        <v>0.104</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <f aca="false">IF(B7&gt;2,(1-_xlfn.BINOM.DIST(2,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
+        <v>0.0639999999999998</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <f aca="false">IF(B7&gt;2,(1-_xlfn.BINOM.DIST(2,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
+        <v>0.00799999999999956</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <f aca="false">IF(B7&gt;3,(1-_xlfn.BINOM.DIST(3,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <f aca="false">IF(B7&gt;3,(1-_xlfn.BINOM.DIST(3,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <f aca="false">IF(B7&gt;4,(1-_xlfn.BINOM.DIST(4,$B7,($C7-$P$2+1)/$C7,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <f aca="false">IF(B7&gt;4,(1-_xlfn.BINOM.DIST(4,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <f aca="false">IF(B8&gt;0,(1-_xlfn.BINOM.DIST(0,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
+        <v>0.578125</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <f aca="false">IF(B8&gt;0,(1-_xlfn.BINOM.DIST(0,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <f aca="false">=IF(B8&gt;1,(1-_xlfn.BINOM.DIST(1,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <f aca="false">IF(B8&gt;1,(1-_xlfn.BINOM.DIST(1,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <f aca="false">IF(B8&gt;2,(1-_xlfn.BINOM.DIST(2,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <f aca="false">IF(B8&gt;2,(1-_xlfn.BINOM.DIST(2,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <f aca="false">IF(B8&gt;3,(1-_xlfn.BINOM.DIST(3,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <f aca="false">IF(B8&gt;3,(1-_xlfn.BINOM.DIST(3,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <f aca="false">IF(B8&gt;4,(1-_xlfn.BINOM.DIST(4,$B8,($C8-$P$2+1)/$C8,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <f aca="false">IF(B8&gt;4,(1-_xlfn.BINOM.DIST(4,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <f aca="false">IF(B9&gt;0,(1-_xlfn.BINOM.DIST(0,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
+        <v>0.68359375</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <f aca="false">IF(B9&gt;0,(1-_xlfn.BINOM.DIST(0,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <f aca="false">=IF(B9&gt;1,(1-_xlfn.BINOM.DIST(1,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
+        <v>0.26171875</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <f aca="false">IF(B9&gt;1,(1-_xlfn.BINOM.DIST(1,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <f aca="false">IF(B9&gt;2,(1-_xlfn.BINOM.DIST(2,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
+        <v>0.05078125</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <f aca="false">IF(B9&gt;2,(1-_xlfn.BINOM.DIST(2,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <f aca="false">IF(B9&gt;3,(1-_xlfn.BINOM.DIST(3,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
+        <v>0.00390625</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <f aca="false">IF(B9&gt;3,(1-_xlfn.BINOM.DIST(3,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <f aca="false">IF(B9&gt;4,(1-_xlfn.BINOM.DIST(4,$B9,($C9-$P$2+1)/$C9,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <f aca="false">IF(B9&gt;4,(1-_xlfn.BINOM.DIST(4,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <f aca="false">IF(B10&gt;0,(1-_xlfn.BINOM.DIST(0,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <f aca="false">IF(B10&gt;0,(1-_xlfn.BINOM.DIST(0,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
+        <v>0.555555555555555</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <f aca="false">=IF(B10&gt;1,(1-_xlfn.BINOM.DIST(1,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <f aca="false">IF(B10&gt;1,(1-_xlfn.BINOM.DIST(1,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <f aca="false">IF(B10&gt;2,(1-_xlfn.BINOM.DIST(2,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <f aca="false">IF(B10&gt;2,(1-_xlfn.BINOM.DIST(2,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <f aca="false">IF(B10&gt;3,(1-_xlfn.BINOM.DIST(3,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <f aca="false">IF(B10&gt;3,(1-_xlfn.BINOM.DIST(3,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <f aca="false">IF(B10&gt;4,(1-_xlfn.BINOM.DIST(4,$B10,($C10-$P$2+1)/$C10,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <f aca="false">IF(B10&gt;4,(1-_xlfn.BINOM.DIST(4,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <f aca="false">IF(B11&gt;0,(1-_xlfn.BINOM.DIST(0,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <f aca="false">IF(B11&gt;0,(1-_xlfn.BINOM.DIST(0,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
+        <v>0.703703703703704</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <f aca="false">=IF(B11&gt;1,(1-_xlfn.BINOM.DIST(1,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <f aca="false">IF(B11&gt;1,(1-_xlfn.BINOM.DIST(1,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
+        <v>0.259259259259259</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <f aca="false">IF(B11&gt;2,(1-_xlfn.BINOM.DIST(2,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <f aca="false">IF(B11&gt;2,(1-_xlfn.BINOM.DIST(2,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
+        <v>0.0370370370370369</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <f aca="false">IF(B11&gt;3,(1-_xlfn.BINOM.DIST(3,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <f aca="false">IF(B11&gt;3,(1-_xlfn.BINOM.DIST(3,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <f aca="false">IF(B11&gt;4,(1-_xlfn.BINOM.DIST(4,$B11,($C11-$P$2+1)/$C11,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <f aca="false">IF(B11&gt;4,(1-_xlfn.BINOM.DIST(4,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="n">
+        <f aca="false">IF(B12&gt;0,(1-_xlfn.BINOM.DIST(0,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
+        <v>0.784</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <f aca="false">IF(B12&gt;0,(1-_xlfn.BINOM.DIST(0,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
+        <v>0.488</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <f aca="false">=IF(B12&gt;1,(1-_xlfn.BINOM.DIST(1,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
+        <v>0.352</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <f aca="false">IF(B12&gt;1,(1-_xlfn.BINOM.DIST(1,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
+        <v>0.104</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <f aca="false">IF(B12&gt;2,(1-_xlfn.BINOM.DIST(2,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
+        <v>0.0639999999999998</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <f aca="false">IF(B12&gt;2,(1-_xlfn.BINOM.DIST(2,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
+        <v>0.00799999999999956</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <f aca="false">IF(B12&gt;3,(1-_xlfn.BINOM.DIST(3,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <f aca="false">IF(B12&gt;3,(1-_xlfn.BINOM.DIST(3,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <f aca="false">IF(B12&gt;4,(1-_xlfn.BINOM.DIST(4,$B12,($C12-$P$2+1)/$C12,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <f aca="false">IF(B12&gt;4,(1-_xlfn.BINOM.DIST(4,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="n">
+        <f aca="false">IF(B13&gt;0,(1-_xlfn.BINOM.DIST(0,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
+        <v>0.8704</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <f aca="false">IF(B13&gt;0,(1-_xlfn.BINOM.DIST(0,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
+        <v>0.5904</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <f aca="false">=IF(B13&gt;1,(1-_xlfn.BINOM.DIST(1,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
+        <v>0.5248</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <f aca="false">IF(B13&gt;1,(1-_xlfn.BINOM.DIST(1,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
+        <v>0.1808</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <f aca="false">IF(B13&gt;2,(1-_xlfn.BINOM.DIST(2,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
+        <v>0.1792</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <f aca="false">IF(B13&gt;2,(1-_xlfn.BINOM.DIST(2,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
+        <v>0.0271999999999998</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <f aca="false">IF(B13&gt;3,(1-_xlfn.BINOM.DIST(3,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
+        <v>0.0255999999999998</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <f aca="false">IF(B13&gt;3,(1-_xlfn.BINOM.DIST(3,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
+        <v>0.00159999999999982</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <f aca="false">IF(B13&gt;4,(1-_xlfn.BINOM.DIST(4,$B13,($C13-$P$2+1)/$C13,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <f aca="false">IF(B13&gt;4,(1-_xlfn.BINOM.DIST(4,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="n">
+        <f aca="false">IF(B14&gt;0,(1-_xlfn.BINOM.DIST(0,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
+        <v>0.7626953125</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <f aca="false">IF(B14&gt;0,(1-_xlfn.BINOM.DIST(0,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <f aca="false">=IF(B14&gt;1,(1-_xlfn.BINOM.DIST(1,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
+        <v>0.3671875</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <f aca="false">IF(B14&gt;1,(1-_xlfn.BINOM.DIST(1,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <f aca="false">IF(B14&gt;2,(1-_xlfn.BINOM.DIST(2,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
+        <v>0.103515625</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <f aca="false">IF(B14&gt;2,(1-_xlfn.BINOM.DIST(2,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <f aca="false">IF(B14&gt;3,(1-_xlfn.BINOM.DIST(3,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <f aca="false">IF(B14&gt;3,(1-_xlfn.BINOM.DIST(3,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <f aca="false">IF(B14&gt;4,(1-_xlfn.BINOM.DIST(4,$B14,($C14-$P$2+1)/$C14,1)),)</f>
+        <v>0.0009765625</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <f aca="false">IF(B14&gt;4,(1-_xlfn.BINOM.DIST(4,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5" t="n">
+        <f aca="false">IF(B15&gt;0,(1-_xlfn.BINOM.DIST(0,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <f aca="false">IF(B15&gt;0,(1-_xlfn.BINOM.DIST(0,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
+        <v>0.802469135802469</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <f aca="false">=IF(B15&gt;1,(1-_xlfn.BINOM.DIST(1,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <f aca="false">IF(B15&gt;1,(1-_xlfn.BINOM.DIST(1,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
+        <v>0.407407407407407</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <f aca="false">IF(B15&gt;2,(1-_xlfn.BINOM.DIST(2,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <f aca="false">IF(B15&gt;2,(1-_xlfn.BINOM.DIST(2,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <f aca="false">IF(B15&gt;3,(1-_xlfn.BINOM.DIST(3,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
+        <v>0.0625</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <f aca="false">IF(B15&gt;3,(1-_xlfn.BINOM.DIST(3,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
+        <v>0.0123456790123455</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <f aca="false">IF(B15&gt;4,(1-_xlfn.BINOM.DIST(4,$B15,($C15-$P$2+1)/$C15,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <f aca="false">IF(B15&gt;4,(1-_xlfn.BINOM.DIST(4,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5" t="n">
+        <f aca="false">IF(B16&gt;0,(1-_xlfn.BINOM.DIST(0,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
+        <v>0.92224</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <f aca="false">IF(B16&gt;0,(1-_xlfn.BINOM.DIST(0,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
+        <v>0.67232</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <f aca="false">=IF(B16&gt;1,(1-_xlfn.BINOM.DIST(1,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
+        <v>0.66304</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <f aca="false">IF(B16&gt;1,(1-_xlfn.BINOM.DIST(1,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
+        <v>0.26272</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <f aca="false">IF(B16&gt;2,(1-_xlfn.BINOM.DIST(2,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
+        <v>0.31744</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <f aca="false">IF(B16&gt;2,(1-_xlfn.BINOM.DIST(2,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
+        <v>0.0579199999999998</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <f aca="false">IF(B16&gt;3,(1-_xlfn.BINOM.DIST(3,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
+        <v>0.0870400000000002</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <f aca="false">IF(B16&gt;3,(1-_xlfn.BINOM.DIST(3,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
+        <v>0.00671999999999973</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <f aca="false">IF(B16&gt;4,(1-_xlfn.BINOM.DIST(4,$B16,($C16-$P$2+1)/$C16,1)),)</f>
+        <v>0.0102400000000002</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <f aca="false">IF(B16&gt;4,(1-_xlfn.BINOM.DIST(4,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
+        <v>0.000319999999999765</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:M1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="1" sqref="R1:S2 K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="3.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+      <selection pane="topLeft" activeCell="O7" activeCellId="1" sqref="R1:S2 O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9437,7 +12588,7 @@
   <dimension ref="B1:W22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="R1:S2 G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9447,7 +12598,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="17" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="3.98"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11327,7 +14478,7 @@
   <dimension ref="B1:W22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+      <selection pane="topLeft" activeCell="Q20" activeCellId="1" sqref="R1:S2 Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11337,7 +14488,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="3" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="17" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="3.98"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -13217,7 +16368,7 @@
   <dimension ref="B1:W27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
+      <selection pane="topLeft" activeCell="P20" activeCellId="1" sqref="R1:S2 P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15551,7 +18702,7 @@
   <dimension ref="B1:W22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="1" sqref="R1:S2 H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17440,7 +20591,7 @@
   <dimension ref="A1:T44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="1" sqref="R1:S2 H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19864,13 +23015,13 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="1" sqref="R1:S2 D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
@@ -20237,14 +23388,14 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="1" sqref="R1:S2 G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="7" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
@@ -22827,14 +25978,14 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="R1:S2 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.7"/>

</xml_diff>

<commit_message>
Worked on wep v5
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Moves" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,8 +23,8 @@
     <sheet name="Weapons 4.0" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Armor 4.0" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Weapons 5.0" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Armor 5.0" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Weapon 5.0 (Table)" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Weapon 5.0 (Table)" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Armor 5.0" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Sheet2" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Sheet5" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="219">
   <si>
     <t xml:space="preserve">Moves</t>
   </si>
@@ -516,28 +516,10 @@
     <t xml:space="preserve">Full Plate Mail Set</t>
   </si>
   <si>
-    <t xml:space="preserve">Concentration cap</t>
+    <t xml:space="preserve">Guard Bonus</t>
   </si>
   <si>
-    <t xml:space="preserve">Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concealable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hide Overcoat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chain Mail  Hauberk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Certain Backgrounds may allow starting with this.</t>
+    <t xml:space="preserve">To Hit Bonus</t>
   </si>
   <si>
     <t xml:space="preserve">Dice Numb</t>
@@ -576,6 +558,9 @@
     <t xml:space="preserve">5 Lethal</t>
   </si>
   <si>
+    <t xml:space="preserve">Traits and Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pain Threshold</t>
   </si>
   <si>
@@ -585,16 +570,34 @@
     <t xml:space="preserve">Punch</t>
   </si>
   <si>
+    <t xml:space="preserve">Light, Cannot use Guard to against weapons Medium or Larger</t>
+  </si>
+  <si>
     <t xml:space="preserve">Club/Improvised Weapon</t>
   </si>
   <si>
+    <t xml:space="preserve">Weak Versatile (Substitute 1 dice for 1d12 when using in two hands)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concealable , Throw, Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parring Dagger</t>
+  </si>
+  <si>
     <t xml:space="preserve">Short Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Throw, Light</t>
   </si>
   <si>
     <t xml:space="preserve">Hand Axe</t>
   </si>
   <si>
     <t xml:space="preserve">Longsword (One Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versatile (Add 1d12 when using in two hands)</t>
   </si>
   <si>
     <t xml:space="preserve">Longsword (Two Hand)</t>
@@ -615,7 +618,103 @@
     <t xml:space="preserve">Great Sword</t>
   </si>
   <si>
+    <t xml:space="preserve">Two Hand (Substitute 1 dice for 1d12)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Great Hammer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spear (One hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional Reach, Versitile, Throw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spear (Two Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pole Axe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach, Two Hand (Substitute 1 dice for 1d12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff (one Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional Reach, Versitile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff (Two Hand)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1d12 (Two Hand Bonus)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Shields (Buckler, etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can attack for Shove or Damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium Shields (Heater, Etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shove Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large Shield (Kite, Targe, Etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dis. Adv.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentration cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concealable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide Overcoat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain Mail  Hauberk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Certain Backgrounds may allow starting with this.</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1151,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1349,11 +1448,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1493,8 +1604,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="R1:S2 B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1623,8 +1734,8 @@
   </sheetPr>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="1" sqref="R1:S2 I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4213,8 +4324,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="R1:S2 E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4497,8 +4608,8 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="1" sqref="R1:S2 E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6977,8 +7088,8 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="R1:S2 F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8497,8 +8608,8 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="1" sqref="R1:S2 B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8778,8 +8889,8 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="R1:S2 F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10296,10 +10407,2299 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:Y36"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q30" activeCellId="0" sqref="Q30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="7" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="74" width="58.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="75" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="L1" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="76" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="76" t="s">
+        <v>164</v>
+      </c>
+      <c r="P1" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q1" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="R1" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="S1" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="T1" s="75" t="s">
+        <v>125</v>
+      </c>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <f aca="false">IF(E2&gt;0,(1-_xlfn.BINOM.DIST(0,$E2,($F2-$R$2+1)/$F2,1)),0)</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <f aca="false">IF(E2&gt;0,(1-_xlfn.BINOM.DIST(0,$E2,($F2-$S$2+1)/$F2,1)),0)</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <f aca="false">IF(E2&gt;1,(1-_xlfn.BINOM.DIST(1,$E2,($F2-$R$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <f aca="false">IF(E2&gt;1,(1-_xlfn.BINOM.DIST(1,$E2,($F2-$S$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <f aca="false">IF(E2&gt;2,(1-_xlfn.BINOM.DIST(2,$E2,($F2-$R$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <f aca="false">IF(E2&gt;2,(1-_xlfn.BINOM.DIST(2,$E2,($F2-$S$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <f aca="false">IF(E2&gt;3,(1-_xlfn.BINOM.DIST(3,$E2,($F2-$R$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="5" t="n">
+        <f aca="false">IF(E2&gt;3,(1-_xlfn.BINOM.DIST(3,$E2,($F2-$S$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="5" t="n">
+        <f aca="false">IF(E2&gt;4,(1-_xlfn.BINOM.DIST(4,$E2,($F2-$R$2+1)/$F2,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="5" t="n">
+        <f aca="false">IF(E2&gt;4,(1-_xlfn.BINOM.DIST(4,$E2,($F2-$S$2+1)/$F2,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <f aca="false">3+T2</f>
+        <v>3</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <f aca="false">5+T2</f>
+        <v>5</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <f aca="false">IF(E3&gt;0,(1-_xlfn.BINOM.DIST(0,$E3,($F3-$R$2+1)/$F3,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <f aca="false">IF(E3&gt;0,(1-_xlfn.BINOM.DIST(0,$E3,($F3-$S$2+1)/$F3,1)),0)</f>
+        <v>0.555555555555555</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <f aca="false">IF(E3&gt;1,(1-_xlfn.BINOM.DIST(1,$E3,($F3-$R$2+1)/$F3,1)),0)</f>
+        <v>0.444444444444444</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <f aca="false">IF(E3&gt;1,(1-_xlfn.BINOM.DIST(1,$E3,($F3-$S$2+1)/$F3,1)),0)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <f aca="false">IF(E3&gt;2,(1-_xlfn.BINOM.DIST(2,$E3,($F3-$R$2+1)/$F3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <f aca="false">IF(E3&gt;2,(1-_xlfn.BINOM.DIST(2,$E3,($F3-$S$2+1)/$F3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <f aca="false">IF(E3&gt;3,(1-_xlfn.BINOM.DIST(3,$E3,($F3-$R$2+1)/$F3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="5" t="n">
+        <f aca="false">IF(E3&gt;3,(1-_xlfn.BINOM.DIST(3,$E3,($F3-$S$2+1)/$F3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="5" t="n">
+        <f aca="false">IF(E3&gt;4,(1-_xlfn.BINOM.DIST(4,$E3,($F3-$R$2+1)/$F3,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="5" t="n">
+        <f aca="false">IF(E3&gt;4,(1-_xlfn.BINOM.DIST(4,$E3,($F3-$S$2+1)/$F3,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="74" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <f aca="false">IF(E4&gt;0,(1-_xlfn.BINOM.DIST(0,$E4,($F4-$R$2+1)/$F4,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <f aca="false">IF(E4&gt;0,(1-_xlfn.BINOM.DIST(0,$E4,($F4-$S$2+1)/$F4,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <f aca="false">IF(E4&gt;1,(1-_xlfn.BINOM.DIST(1,$E4,($F4-$R$2+1)/$F4,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <f aca="false">IF(E4&gt;1,(1-_xlfn.BINOM.DIST(1,$E4,($F4-$S$2+1)/$F4,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <f aca="false">IF(E4&gt;2,(1-_xlfn.BINOM.DIST(2,$E4,($F4-$R$2+1)/$F4,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <f aca="false">IF(E4&gt;2,(1-_xlfn.BINOM.DIST(2,$E4,($F4-$S$2+1)/$F4,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <f aca="false">IF(E4&gt;3,(1-_xlfn.BINOM.DIST(3,$E4,($F4-$R$2+1)/$F4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <f aca="false">IF(E4&gt;3,(1-_xlfn.BINOM.DIST(3,$E4,($F4-$S$2+1)/$F4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <f aca="false">IF(E4&gt;4,(1-_xlfn.BINOM.DIST(4,$E4,($F4-$R$2+1)/$F4,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <f aca="false">IF(E4&gt;4,(1-_xlfn.BINOM.DIST(4,$E4,($F4-$S$2+1)/$F4,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="74" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <f aca="false">IF(E5&gt;0,(1-_xlfn.BINOM.DIST(0,$E5,($F5-$R$2+1)/$F5,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <f aca="false">IF(E5&gt;0,(1-_xlfn.BINOM.DIST(0,$E5,($F5-$S$2+1)/$F5,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <f aca="false">IF(E5&gt;1,(1-_xlfn.BINOM.DIST(1,$E5,($F5-$R$2+1)/$F5,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <f aca="false">IF(E5&gt;1,(1-_xlfn.BINOM.DIST(1,$E5,($F5-$S$2+1)/$F5,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <f aca="false">IF(E5&gt;2,(1-_xlfn.BINOM.DIST(2,$E5,($F5-$R$2+1)/$F5,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <f aca="false">IF(E5&gt;2,(1-_xlfn.BINOM.DIST(2,$E5,($F5-$S$2+1)/$F5,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <f aca="false">IF(E5&gt;3,(1-_xlfn.BINOM.DIST(3,$E5,($F5-$R$2+1)/$F5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <f aca="false">IF(E5&gt;3,(1-_xlfn.BINOM.DIST(3,$E5,($F5-$S$2+1)/$F5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <f aca="false">IF(E5&gt;4,(1-_xlfn.BINOM.DIST(4,$E5,($F5-$R$2+1)/$F5,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <f aca="false">IF(E5&gt;4,(1-_xlfn.BINOM.DIST(4,$E5,($F5-$S$2+1)/$F5,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="74" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <f aca="false">IF(E6&gt;0,(1-_xlfn.BINOM.DIST(0,$E6,($F6-$R$2+1)/$F6,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <f aca="false">IF(E6&gt;0,(1-_xlfn.BINOM.DIST(0,$E6,($F6-$S$2+1)/$F6,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <f aca="false">IF(E6&gt;1,(1-_xlfn.BINOM.DIST(1,$E6,($F6-$R$2+1)/$F6,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <f aca="false">IF(E6&gt;1,(1-_xlfn.BINOM.DIST(1,$E6,($F6-$S$2+1)/$F6,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <f aca="false">IF(E6&gt;2,(1-_xlfn.BINOM.DIST(2,$E6,($F6-$R$2+1)/$F6,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <f aca="false">IF(E6&gt;2,(1-_xlfn.BINOM.DIST(2,$E6,($F6-$S$2+1)/$F6,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <f aca="false">IF(E6&gt;3,(1-_xlfn.BINOM.DIST(3,$E6,($F6-$R$2+1)/$F6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <f aca="false">IF(E6&gt;3,(1-_xlfn.BINOM.DIST(3,$E6,($F6-$S$2+1)/$F6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <f aca="false">IF(E6&gt;4,(1-_xlfn.BINOM.DIST(4,$E6,($F6-$R$2+1)/$F6,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <f aca="false">IF(E6&gt;4,(1-_xlfn.BINOM.DIST(4,$E6,($F6-$S$2+1)/$F6,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="74" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <f aca="false">IF(E7&gt;0,(1-_xlfn.BINOM.DIST(0,$E7,($F7-$R$2+1)/$F7,1)),0)</f>
+        <v>0.972222222222222</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <f aca="false">IF(E7&gt;0,(1-_xlfn.BINOM.DIST(0,$E7,($F7-$S$2+1)/$F7,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <f aca="false">IF(E7&gt;1,(1-_xlfn.BINOM.DIST(1,$E7,($F7-$R$2+1)/$F7,1)),0)</f>
+        <v>0.694444444444444</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <f aca="false">IF(E7&gt;1,(1-_xlfn.BINOM.DIST(1,$E7,($F7-$S$2+1)/$F7,1)),0)</f>
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <f aca="false">IF(E7&gt;2,(1-_xlfn.BINOM.DIST(2,$E7,($F7-$R$2+1)/$F7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <f aca="false">IF(E7&gt;2,(1-_xlfn.BINOM.DIST(2,$E7,($F7-$S$2+1)/$F7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <f aca="false">IF(E7&gt;3,(1-_xlfn.BINOM.DIST(3,$E7,($F7-$R$2+1)/$F7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="5" t="n">
+        <f aca="false">IF(E7&gt;3,(1-_xlfn.BINOM.DIST(3,$E7,($F7-$S$2+1)/$F7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="5" t="n">
+        <f aca="false">IF(E7&gt;4,(1-_xlfn.BINOM.DIST(4,$E7,($F7-$R$2+1)/$F7,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="5" t="n">
+        <f aca="false">IF(E7&gt;4,(1-_xlfn.BINOM.DIST(4,$E7,($F7-$S$2+1)/$F7,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <f aca="false">IF(E8&gt;0,(1-_xlfn.BINOM.DIST(0,$E8,($F8-$R$2+1)/$F8,1)),0)</f>
+        <v>0.992</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <f aca="false">IF(E8&gt;0,(1-_xlfn.BINOM.DIST(0,$E8,($F8-$S$2+1)/$F8,1)),0)</f>
+        <v>0.936</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <f aca="false">IF(E8&gt;1,(1-_xlfn.BINOM.DIST(1,$E8,($F8-$R$2+1)/$F8,1)),0)</f>
+        <v>0.896</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <f aca="false">IF(E8&gt;1,(1-_xlfn.BINOM.DIST(1,$E8,($F8-$S$2+1)/$F8,1)),0)</f>
+        <v>0.648</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <f aca="false">IF(E8&gt;2,(1-_xlfn.BINOM.DIST(2,$E8,($F8-$R$2+1)/$F8,1)),0)</f>
+        <v>0.512</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <f aca="false">IF(E8&gt;2,(1-_xlfn.BINOM.DIST(2,$E8,($F8-$S$2+1)/$F8,1)),0)</f>
+        <v>0.216</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <f aca="false">IF(E8&gt;3,(1-_xlfn.BINOM.DIST(3,$E8,($F8-$R$2+1)/$F8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="5" t="n">
+        <f aca="false">IF(E8&gt;3,(1-_xlfn.BINOM.DIST(3,$E8,($F8-$S$2+1)/$F8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="5" t="n">
+        <f aca="false">IF(E8&gt;4,(1-_xlfn.BINOM.DIST(4,$E8,($F8-$R$2+1)/$F8,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="5" t="n">
+        <f aca="false">IF(E8&gt;4,(1-_xlfn.BINOM.DIST(4,$E8,($F8-$S$2+1)/$F8,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="74" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <f aca="false">IF(E9&gt;0,(1-_xlfn.BINOM.DIST(0,$E9,($F9-$R$2+1)/$F9,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <f aca="false">IF(E9&gt;0,(1-_xlfn.BINOM.DIST(0,$E9,($F9-$S$2+1)/$F9,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <f aca="false">IF(E9&gt;1,(1-_xlfn.BINOM.DIST(1,$E9,($F9-$R$2+1)/$F9,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <f aca="false">IF(E9&gt;1,(1-_xlfn.BINOM.DIST(1,$E9,($F9-$S$2+1)/$F9,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <f aca="false">IF(E9&gt;2,(1-_xlfn.BINOM.DIST(2,$E9,($F9-$R$2+1)/$F9,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <f aca="false">IF(E9&gt;2,(1-_xlfn.BINOM.DIST(2,$E9,($F9-$S$2+1)/$F9,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <f aca="false">IF(E9&gt;3,(1-_xlfn.BINOM.DIST(3,$E9,($F9-$R$2+1)/$F9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="5" t="n">
+        <f aca="false">IF(E9&gt;3,(1-_xlfn.BINOM.DIST(3,$E9,($F9-$S$2+1)/$F9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="5" t="n">
+        <f aca="false">IF(E9&gt;4,(1-_xlfn.BINOM.DIST(4,$E9,($F9-$R$2+1)/$F9,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="5" t="n">
+        <f aca="false">IF(E9&gt;4,(1-_xlfn.BINOM.DIST(4,$E9,($F9-$S$2+1)/$F9,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5" t="n">
+        <f aca="false">IF(E10&gt;0,(1-_xlfn.BINOM.DIST(0,$E10,($F10-$R$2+1)/$F10,1)),0)</f>
+        <v>0.99609375</v>
+      </c>
+      <c r="H10" s="5" t="n">
+        <f aca="false">IF(E10&gt;0,(1-_xlfn.BINOM.DIST(0,$E10,($F10-$S$2+1)/$F10,1)),0)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="I10" s="5" t="n">
+        <f aca="false">IF(E10&gt;1,(1-_xlfn.BINOM.DIST(1,$E10,($F10-$R$2+1)/$F10,1)),0)</f>
+        <v>0.94921875</v>
+      </c>
+      <c r="J10" s="5" t="n">
+        <f aca="false">IF(E10&gt;1,(1-_xlfn.BINOM.DIST(1,$E10,($F10-$S$2+1)/$F10,1)),0)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="K10" s="5" t="n">
+        <f aca="false">IF(E10&gt;2,(1-_xlfn.BINOM.DIST(2,$E10,($F10-$R$2+1)/$F10,1)),0)</f>
+        <v>0.73828125</v>
+      </c>
+      <c r="L10" s="5" t="n">
+        <f aca="false">IF(E10&gt;2,(1-_xlfn.BINOM.DIST(2,$E10,($F10-$S$2+1)/$F10,1)),0)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <f aca="false">IF(E10&gt;3,(1-_xlfn.BINOM.DIST(3,$E10,($F10-$R$2+1)/$F10,1)),0)</f>
+        <v>0.31640625</v>
+      </c>
+      <c r="N10" s="5" t="n">
+        <f aca="false">IF(E10&gt;3,(1-_xlfn.BINOM.DIST(3,$E10,($F10-$S$2+1)/$F10,1)),0)</f>
+        <v>0.0625</v>
+      </c>
+      <c r="O10" s="5" t="n">
+        <f aca="false">IF(E10&gt;4,(1-_xlfn.BINOM.DIST(4,$E10,($F10-$R$2+1)/$F10,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="n">
+        <f aca="false">IF(E10&gt;4,(1-_xlfn.BINOM.DIST(4,$E10,($F10-$S$2+1)/$F10,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <f aca="false">IF(E11&gt;0,(1-_xlfn.BINOM.DIST(0,$E11,($F11-$R$2+1)/$F11,1)),0)</f>
+        <v>0.972222222222222</v>
+      </c>
+      <c r="H11" s="5" t="n">
+        <f aca="false">IF(E11&gt;0,(1-_xlfn.BINOM.DIST(0,$E11,($F11-$S$2+1)/$F11,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="I11" s="5" t="n">
+        <f aca="false">IF(E11&gt;1,(1-_xlfn.BINOM.DIST(1,$E11,($F11-$R$2+1)/$F11,1)),0)</f>
+        <v>0.694444444444444</v>
+      </c>
+      <c r="J11" s="5" t="n">
+        <f aca="false">IF(E11&gt;1,(1-_xlfn.BINOM.DIST(1,$E11,($F11-$S$2+1)/$F11,1)),0)</f>
+        <v>0.444444444444444</v>
+      </c>
+      <c r="K11" s="5" t="n">
+        <f aca="false">IF(E11&gt;2,(1-_xlfn.BINOM.DIST(2,$E11,($F11-$R$2+1)/$F11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="n">
+        <f aca="false">IF(E11&gt;2,(1-_xlfn.BINOM.DIST(2,$E11,($F11-$S$2+1)/$F11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="5" t="n">
+        <f aca="false">IF(E11&gt;3,(1-_xlfn.BINOM.DIST(3,$E11,($F11-$R$2+1)/$F11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <f aca="false">IF(E11&gt;3,(1-_xlfn.BINOM.DIST(3,$E11,($F11-$S$2+1)/$F11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="5" t="n">
+        <f aca="false">IF(E11&gt;4,(1-_xlfn.BINOM.DIST(4,$E11,($F11-$R$2+1)/$F11,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="n">
+        <f aca="false">IF(E11&gt;4,(1-_xlfn.BINOM.DIST(4,$E11,($F11-$S$2+1)/$F11,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <f aca="false">IF(E12&gt;0,(1-_xlfn.BINOM.DIST(0,$E12,($F12-$R$2+1)/$F12,1)),0)</f>
+        <v>0.99537037037037</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <f aca="false">IF(E12&gt;0,(1-_xlfn.BINOM.DIST(0,$E12,($F12-$S$2+1)/$F12,1)),0)</f>
+        <v>0.962962962962963</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <f aca="false">IF(E12&gt;1,(1-_xlfn.BINOM.DIST(1,$E12,($F12-$R$2+1)/$F12,1)),0)</f>
+        <v>0.925925925925926</v>
+      </c>
+      <c r="J12" s="5" t="n">
+        <f aca="false">IF(E12&gt;1,(1-_xlfn.BINOM.DIST(1,$E12,($F12-$S$2+1)/$F12,1)),0)</f>
+        <v>0.740740740740741</v>
+      </c>
+      <c r="K12" s="5" t="n">
+        <f aca="false">IF(E12&gt;2,(1-_xlfn.BINOM.DIST(2,$E12,($F12-$R$2+1)/$F12,1)),0)</f>
+        <v>0.578703703703704</v>
+      </c>
+      <c r="L12" s="5" t="n">
+        <f aca="false">IF(E12&gt;2,(1-_xlfn.BINOM.DIST(2,$E12,($F12-$S$2+1)/$F12,1)),0)</f>
+        <v>0.296296296296296</v>
+      </c>
+      <c r="M12" s="5" t="n">
+        <f aca="false">IF(E12&gt;3,(1-_xlfn.BINOM.DIST(3,$E12,($F12-$R$2+1)/$F12,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="5" t="n">
+        <f aca="false">IF(E12&gt;3,(1-_xlfn.BINOM.DIST(3,$E12,($F12-$S$2+1)/$F12,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="5" t="n">
+        <f aca="false">IF(E12&gt;4,(1-_xlfn.BINOM.DIST(4,$E12,($F12-$R$2+1)/$F12,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="5" t="n">
+        <f aca="false">IF(E12&gt;4,(1-_xlfn.BINOM.DIST(4,$E12,($F12-$S$2+1)/$F12,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G13" s="5" t="n">
+        <f aca="false">IF(E13&gt;0,(1-_xlfn.BINOM.DIST(0,$E13,($F13-$R$2+1)/$F13,1)),0)</f>
+        <v>0.992</v>
+      </c>
+      <c r="H13" s="5" t="n">
+        <f aca="false">IF(E13&gt;0,(1-_xlfn.BINOM.DIST(0,$E13,($F13-$S$2+1)/$F13,1)),0)</f>
+        <v>0.936</v>
+      </c>
+      <c r="I13" s="5" t="n">
+        <f aca="false">IF(E13&gt;1,(1-_xlfn.BINOM.DIST(1,$E13,($F13-$R$2+1)/$F13,1)),0)</f>
+        <v>0.896</v>
+      </c>
+      <c r="J13" s="5" t="n">
+        <f aca="false">IF(E13&gt;1,(1-_xlfn.BINOM.DIST(1,$E13,($F13-$S$2+1)/$F13,1)),0)</f>
+        <v>0.648</v>
+      </c>
+      <c r="K13" s="5" t="n">
+        <f aca="false">IF(E13&gt;2,(1-_xlfn.BINOM.DIST(2,$E13,($F13-$R$2+1)/$F13,1)),0)</f>
+        <v>0.512</v>
+      </c>
+      <c r="L13" s="5" t="n">
+        <f aca="false">IF(E13&gt;2,(1-_xlfn.BINOM.DIST(2,$E13,($F13-$S$2+1)/$F13,1)),0)</f>
+        <v>0.216</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <f aca="false">IF(E13&gt;3,(1-_xlfn.BINOM.DIST(3,$E13,($F13-$R$2+1)/$F13,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="5" t="n">
+        <f aca="false">IF(E13&gt;3,(1-_xlfn.BINOM.DIST(3,$E13,($F13-$S$2+1)/$F13,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="5" t="n">
+        <f aca="false">IF(E13&gt;4,(1-_xlfn.BINOM.DIST(4,$E13,($F13-$R$2+1)/$F13,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="5" t="n">
+        <f aca="false">IF(E13&gt;4,(1-_xlfn.BINOM.DIST(4,$E13,($F13-$S$2+1)/$F13,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5" t="n">
+        <f aca="false">IF(E14&gt;0,(1-_xlfn.BINOM.DIST(0,$E14,($F14-$R$2+1)/$F14,1)),0)</f>
+        <v>0.9984</v>
+      </c>
+      <c r="H14" s="5" t="n">
+        <f aca="false">IF(E14&gt;0,(1-_xlfn.BINOM.DIST(0,$E14,($F14-$S$2+1)/$F14,1)),0)</f>
+        <v>0.9744</v>
+      </c>
+      <c r="I14" s="5" t="n">
+        <f aca="false">IF(E14&gt;1,(1-_xlfn.BINOM.DIST(1,$E14,($F14-$R$2+1)/$F14,1)),0)</f>
+        <v>0.9728</v>
+      </c>
+      <c r="J14" s="5" t="n">
+        <f aca="false">IF(E14&gt;1,(1-_xlfn.BINOM.DIST(1,$E14,($F14-$S$2+1)/$F14,1)),0)</f>
+        <v>0.8208</v>
+      </c>
+      <c r="K14" s="5" t="n">
+        <f aca="false">IF(E14&gt;2,(1-_xlfn.BINOM.DIST(2,$E14,($F14-$R$2+1)/$F14,1)),0)</f>
+        <v>0.8192</v>
+      </c>
+      <c r="L14" s="5" t="n">
+        <f aca="false">IF(E14&gt;2,(1-_xlfn.BINOM.DIST(2,$E14,($F14-$S$2+1)/$F14,1)),0)</f>
+        <v>0.4752</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <f aca="false">IF(E14&gt;3,(1-_xlfn.BINOM.DIST(3,$E14,($F14-$R$2+1)/$F14,1)),0)</f>
+        <v>0.4096</v>
+      </c>
+      <c r="N14" s="5" t="n">
+        <f aca="false">IF(E14&gt;3,(1-_xlfn.BINOM.DIST(3,$E14,($F14-$S$2+1)/$F14,1)),0)</f>
+        <v>0.1296</v>
+      </c>
+      <c r="O14" s="5" t="n">
+        <f aca="false">IF(E14&gt;4,(1-_xlfn.BINOM.DIST(4,$E14,($F14-$R$2+1)/$F14,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="5" t="n">
+        <f aca="false">IF(E14&gt;4,(1-_xlfn.BINOM.DIST(4,$E14,($F14-$S$2+1)/$F14,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5" t="n">
+        <f aca="false">IF(E15&gt;0,(1-_xlfn.BINOM.DIST(0,$E15,($F15-$R$2+1)/$F15,1)),0)</f>
+        <v>0.9990234375</v>
+      </c>
+      <c r="H15" s="5" t="n">
+        <f aca="false">IF(E15&gt;0,(1-_xlfn.BINOM.DIST(0,$E15,($F15-$S$2+1)/$F15,1)),0)</f>
+        <v>0.96875</v>
+      </c>
+      <c r="I15" s="5" t="n">
+        <f aca="false">IF(E15&gt;1,(1-_xlfn.BINOM.DIST(1,$E15,($F15-$R$2+1)/$F15,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="J15" s="5" t="n">
+        <f aca="false">IF(E15&gt;1,(1-_xlfn.BINOM.DIST(1,$E15,($F15-$S$2+1)/$F15,1)),0)</f>
+        <v>0.8125</v>
+      </c>
+      <c r="K15" s="5" t="n">
+        <f aca="false">IF(E15&gt;2,(1-_xlfn.BINOM.DIST(2,$E15,($F15-$R$2+1)/$F15,1)),0)</f>
+        <v>0.896484375</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <f aca="false">IF(E15&gt;2,(1-_xlfn.BINOM.DIST(2,$E15,($F15-$S$2+1)/$F15,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M15" s="5" t="n">
+        <f aca="false">IF(E15&gt;3,(1-_xlfn.BINOM.DIST(3,$E15,($F15-$R$2+1)/$F15,1)),0)</f>
+        <v>0.6328125</v>
+      </c>
+      <c r="N15" s="5" t="n">
+        <f aca="false">IF(E15&gt;3,(1-_xlfn.BINOM.DIST(3,$E15,($F15-$S$2+1)/$F15,1)),0)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="O15" s="5" t="n">
+        <f aca="false">IF(E15&gt;4,(1-_xlfn.BINOM.DIST(4,$E15,($F15-$R$2+1)/$F15,1)),)</f>
+        <v>0.2373046875</v>
+      </c>
+      <c r="P15" s="5" t="n">
+        <f aca="false">IF(E15&gt;4,(1-_xlfn.BINOM.DIST(4,$E15,($F15-$S$2+1)/$F15,1)),0)</f>
+        <v>0.03125</v>
+      </c>
+      <c r="Q15" s="74" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <f aca="false">IF(E16&gt;0,(1-_xlfn.BINOM.DIST(0,$E16,($F16-$R$2+1)/$F16,1)),0)</f>
+        <v>0.999228395061728</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <f aca="false">IF(E16&gt;0,(1-_xlfn.BINOM.DIST(0,$E16,($F16-$S$2+1)/$F16,1)),0)</f>
+        <v>0.987654320987654</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <f aca="false">IF(E16&gt;1,(1-_xlfn.BINOM.DIST(1,$E16,($F16-$R$2+1)/$F16,1)),0)</f>
+        <v>0.983796296296296</v>
+      </c>
+      <c r="J16" s="5" t="n">
+        <f aca="false">IF(E16&gt;1,(1-_xlfn.BINOM.DIST(1,$E16,($F16-$S$2+1)/$F16,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="K16" s="5" t="n">
+        <f aca="false">IF(E16&gt;2,(1-_xlfn.BINOM.DIST(2,$E16,($F16-$R$2+1)/$F16,1)),0)</f>
+        <v>0.868055555555556</v>
+      </c>
+      <c r="L16" s="5" t="n">
+        <f aca="false">IF(E16&gt;2,(1-_xlfn.BINOM.DIST(2,$E16,($F16-$S$2+1)/$F16,1)),0)</f>
+        <v>0.592592592592593</v>
+      </c>
+      <c r="M16" s="5" t="n">
+        <f aca="false">IF(E16&gt;3,(1-_xlfn.BINOM.DIST(3,$E16,($F16-$R$2+1)/$F16,1)),0)</f>
+        <v>0.482253086419753</v>
+      </c>
+      <c r="N16" s="5" t="n">
+        <f aca="false">IF(E16&gt;3,(1-_xlfn.BINOM.DIST(3,$E16,($F16-$S$2+1)/$F16,1)),0)</f>
+        <v>0.197530864197531</v>
+      </c>
+      <c r="O16" s="5" t="n">
+        <f aca="false">IF(E16&gt;4,(1-_xlfn.BINOM.DIST(4,$E16,($F16-$R$2+1)/$F16,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="5" t="n">
+        <f aca="false">IF(E16&gt;4,(1-_xlfn.BINOM.DIST(4,$E16,($F16-$S$2+1)/$F16,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5" t="n">
+        <f aca="false">IF(E17&gt;0,(1-_xlfn.BINOM.DIST(0,$E17,($F17-$R$2+1)/$F17,1)),0)</f>
+        <v>0.99968</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <f aca="false">IF(E17&gt;0,(1-_xlfn.BINOM.DIST(0,$E17,($F17-$S$2+1)/$F17,1)),0)</f>
+        <v>0.98976</v>
+      </c>
+      <c r="I17" s="5" t="n">
+        <f aca="false">IF(E17&gt;1,(1-_xlfn.BINOM.DIST(1,$E17,($F17-$R$2+1)/$F17,1)),0)</f>
+        <v>0.99328</v>
+      </c>
+      <c r="J17" s="5" t="n">
+        <f aca="false">IF(E17&gt;1,(1-_xlfn.BINOM.DIST(1,$E17,($F17-$S$2+1)/$F17,1)),0)</f>
+        <v>0.91296</v>
+      </c>
+      <c r="K17" s="5" t="n">
+        <f aca="false">IF(E17&gt;2,(1-_xlfn.BINOM.DIST(2,$E17,($F17-$R$2+1)/$F17,1)),0)</f>
+        <v>0.94208</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <f aca="false">IF(E17&gt;2,(1-_xlfn.BINOM.DIST(2,$E17,($F17-$S$2+1)/$F17,1)),0)</f>
+        <v>0.68256</v>
+      </c>
+      <c r="M17" s="5" t="n">
+        <f aca="false">IF(E17&gt;3,(1-_xlfn.BINOM.DIST(3,$E17,($F17-$R$2+1)/$F17,1)),0)</f>
+        <v>0.73728</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <f aca="false">IF(E17&gt;3,(1-_xlfn.BINOM.DIST(3,$E17,($F17-$S$2+1)/$F17,1)),0)</f>
+        <v>0.33696</v>
+      </c>
+      <c r="O17" s="5" t="n">
+        <f aca="false">IF(E17&gt;4,(1-_xlfn.BINOM.DIST(4,$E17,($F17-$R$2+1)/$F17,1)),)</f>
+        <v>0.32768</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <f aca="false">IF(E17&gt;4,(1-_xlfn.BINOM.DIST(4,$E17,($F17-$S$2+1)/$F17,1)),0)</f>
+        <v>0.0777600000000001</v>
+      </c>
+      <c r="Q17" s="78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5" t="n">
+        <f aca="false">IF(E18&gt;0,(1-_xlfn.BINOM.DIST(0,$E18,($F18-$R$2+1)/$F18,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <f aca="false">IF(E18&gt;0,(1-_xlfn.BINOM.DIST(0,$E18,($F18-$S$2+1)/$F18,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I18" s="5" t="n">
+        <f aca="false">IF(E18&gt;1,(1-_xlfn.BINOM.DIST(1,$E18,($F18-$R$2+1)/$F18,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J18" s="5" t="n">
+        <f aca="false">IF(E18&gt;1,(1-_xlfn.BINOM.DIST(1,$E18,($F18-$S$2+1)/$F18,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="5" t="n">
+        <f aca="false">IF(E18&gt;2,(1-_xlfn.BINOM.DIST(2,$E18,($F18-$R$2+1)/$F18,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L18" s="5" t="n">
+        <f aca="false">IF(E18&gt;2,(1-_xlfn.BINOM.DIST(2,$E18,($F18-$S$2+1)/$F18,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M18" s="5" t="n">
+        <f aca="false">IF(E18&gt;3,(1-_xlfn.BINOM.DIST(3,$E18,($F18-$R$2+1)/$F18,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="5" t="n">
+        <f aca="false">IF(E18&gt;3,(1-_xlfn.BINOM.DIST(3,$E18,($F18-$S$2+1)/$F18,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="5" t="n">
+        <f aca="false">IF(E18&gt;4,(1-_xlfn.BINOM.DIST(4,$E18,($F18-$R$2+1)/$F18,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="5" t="n">
+        <f aca="false">IF(E18&gt;4,(1-_xlfn.BINOM.DIST(4,$E18,($F18-$S$2+1)/$F18,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="74" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G19" s="5" t="n">
+        <f aca="false">IF(E19&gt;0,(1-_xlfn.BINOM.DIST(0,$E19,($F19-$R$2+1)/$F19,1)),0)</f>
+        <v>0.99609375</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <f aca="false">IF(E19&gt;0,(1-_xlfn.BINOM.DIST(0,$E19,($F19-$S$2+1)/$F19,1)),0)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="I19" s="5" t="n">
+        <f aca="false">IF(E19&gt;1,(1-_xlfn.BINOM.DIST(1,$E19,($F19-$R$2+1)/$F19,1)),0)</f>
+        <v>0.94921875</v>
+      </c>
+      <c r="J19" s="5" t="n">
+        <f aca="false">IF(E19&gt;1,(1-_xlfn.BINOM.DIST(1,$E19,($F19-$S$2+1)/$F19,1)),0)</f>
+        <v>0.6875</v>
+      </c>
+      <c r="K19" s="5" t="n">
+        <f aca="false">IF(E19&gt;2,(1-_xlfn.BINOM.DIST(2,$E19,($F19-$R$2+1)/$F19,1)),0)</f>
+        <v>0.73828125</v>
+      </c>
+      <c r="L19" s="5" t="n">
+        <f aca="false">IF(E19&gt;2,(1-_xlfn.BINOM.DIST(2,$E19,($F19-$S$2+1)/$F19,1)),0)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="M19" s="5" t="n">
+        <f aca="false">IF(E19&gt;3,(1-_xlfn.BINOM.DIST(3,$E19,($F19-$R$2+1)/$F19,1)),0)</f>
+        <v>0.31640625</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <f aca="false">IF(E19&gt;3,(1-_xlfn.BINOM.DIST(3,$E19,($F19-$S$2+1)/$F19,1)),0)</f>
+        <v>0.0625</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <f aca="false">IF(E19&gt;4,(1-_xlfn.BINOM.DIST(4,$E19,($F19-$R$2+1)/$F19,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="5" t="n">
+        <f aca="false">IF(E19&gt;4,(1-_xlfn.BINOM.DIST(4,$E19,($F19-$S$2+1)/$F19,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5" t="n">
+        <f aca="false">IF(E20&gt;0,(1-_xlfn.BINOM.DIST(0,$E20,($F20-$R$2+1)/$F20,1)),0)</f>
+        <v>0.999228395061728</v>
+      </c>
+      <c r="H20" s="5" t="n">
+        <f aca="false">IF(E20&gt;0,(1-_xlfn.BINOM.DIST(0,$E20,($F20-$S$2+1)/$F20,1)),0)</f>
+        <v>0.987654320987654</v>
+      </c>
+      <c r="I20" s="5" t="n">
+        <f aca="false">IF(E20&gt;1,(1-_xlfn.BINOM.DIST(1,$E20,($F20-$R$2+1)/$F20,1)),0)</f>
+        <v>0.983796296296296</v>
+      </c>
+      <c r="J20" s="5" t="n">
+        <f aca="false">IF(E20&gt;1,(1-_xlfn.BINOM.DIST(1,$E20,($F20-$S$2+1)/$F20,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="K20" s="5" t="n">
+        <f aca="false">IF(E20&gt;2,(1-_xlfn.BINOM.DIST(2,$E20,($F20-$R$2+1)/$F20,1)),0)</f>
+        <v>0.868055555555556</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <f aca="false">IF(E20&gt;2,(1-_xlfn.BINOM.DIST(2,$E20,($F20-$S$2+1)/$F20,1)),0)</f>
+        <v>0.592592592592593</v>
+      </c>
+      <c r="M20" s="5" t="n">
+        <f aca="false">IF(E20&gt;3,(1-_xlfn.BINOM.DIST(3,$E20,($F20-$R$2+1)/$F20,1)),0)</f>
+        <v>0.482253086419753</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <f aca="false">IF(E20&gt;3,(1-_xlfn.BINOM.DIST(3,$E20,($F20-$S$2+1)/$F20,1)),0)</f>
+        <v>0.197530864197531</v>
+      </c>
+      <c r="O20" s="5" t="n">
+        <f aca="false">IF(E20&gt;4,(1-_xlfn.BINOM.DIST(4,$E20,($F20-$R$2+1)/$F20,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <f aca="false">IF(E20&gt;4,(1-_xlfn.BINOM.DIST(4,$E20,($F20-$S$2+1)/$F20,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="78" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5" t="n">
+        <f aca="false">IF(E21&gt;0,(1-_xlfn.BINOM.DIST(0,$E21,($F21-$R$2+1)/$F21,1)),0)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="H21" s="5" t="n">
+        <f aca="false">IF(E21&gt;0,(1-_xlfn.BINOM.DIST(0,$E21,($F21-$S$2+1)/$F21,1)),0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="I21" s="5" t="n">
+        <f aca="false">IF(E21&gt;1,(1-_xlfn.BINOM.DIST(1,$E21,($F21-$R$2+1)/$F21,1)),0)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="J21" s="5" t="n">
+        <f aca="false">IF(E21&gt;1,(1-_xlfn.BINOM.DIST(1,$E21,($F21-$S$2+1)/$F21,1)),0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="K21" s="5" t="n">
+        <f aca="false">IF(E21&gt;2,(1-_xlfn.BINOM.DIST(2,$E21,($F21-$R$2+1)/$F21,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <f aca="false">IF(E21&gt;2,(1-_xlfn.BINOM.DIST(2,$E21,($F21-$S$2+1)/$F21,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="5" t="n">
+        <f aca="false">IF(E21&gt;3,(1-_xlfn.BINOM.DIST(3,$E21,($F21-$R$2+1)/$F21,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <f aca="false">IF(E21&gt;3,(1-_xlfn.BINOM.DIST(3,$E21,($F21-$S$2+1)/$F21,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="5" t="n">
+        <f aca="false">IF(E21&gt;4,(1-_xlfn.BINOM.DIST(4,$E21,($F21-$R$2+1)/$F21,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="5" t="n">
+        <f aca="false">IF(E21&gt;4,(1-_xlfn.BINOM.DIST(4,$E21,($F21-$S$2+1)/$F21,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="78" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G22" s="5" t="n">
+        <f aca="false">IF(E22&gt;0,(1-_xlfn.BINOM.DIST(0,$E22,($F22-$R$2+1)/$F22,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H22" s="5" t="n">
+        <f aca="false">IF(E22&gt;0,(1-_xlfn.BINOM.DIST(0,$E22,($F22-$S$2+1)/$F22,1)),0)</f>
+        <v>0.875</v>
+      </c>
+      <c r="I22" s="5" t="n">
+        <f aca="false">IF(E22&gt;1,(1-_xlfn.BINOM.DIST(1,$E22,($F22-$R$2+1)/$F22,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J22" s="5" t="n">
+        <f aca="false">IF(E22&gt;1,(1-_xlfn.BINOM.DIST(1,$E22,($F22-$S$2+1)/$F22,1)),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="5" t="n">
+        <f aca="false">IF(E22&gt;2,(1-_xlfn.BINOM.DIST(2,$E22,($F22-$R$2+1)/$F22,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L22" s="5" t="n">
+        <f aca="false">IF(E22&gt;2,(1-_xlfn.BINOM.DIST(2,$E22,($F22-$S$2+1)/$F22,1)),0)</f>
+        <v>0.125</v>
+      </c>
+      <c r="M22" s="5" t="n">
+        <f aca="false">IF(E22&gt;3,(1-_xlfn.BINOM.DIST(3,$E22,($F22-$R$2+1)/$F22,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="5" t="n">
+        <f aca="false">IF(E22&gt;3,(1-_xlfn.BINOM.DIST(3,$E22,($F22-$S$2+1)/$F22,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="5" t="n">
+        <f aca="false">IF(E22&gt;4,(1-_xlfn.BINOM.DIST(4,$E22,($F22-$R$2+1)/$F22,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="5" t="n">
+        <f aca="false">IF(E22&gt;4,(1-_xlfn.BINOM.DIST(4,$E22,($F22-$S$2+1)/$F22,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="78" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G23" s="5" t="n">
+        <f aca="false">IF(E23&gt;0,(1-_xlfn.BINOM.DIST(0,$E23,($F23-$R$2+1)/$F23,1)),0)</f>
+        <v>0.833333333333333</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <f aca="false">IF(E23&gt;0,(1-_xlfn.BINOM.DIST(0,$E23,($F23-$S$2+1)/$F23,1)),0)</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="I23" s="5" t="n">
+        <f aca="false">IF(E23&gt;1,(1-_xlfn.BINOM.DIST(1,$E23,($F23-$R$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="n">
+        <f aca="false">IF(E23&gt;1,(1-_xlfn.BINOM.DIST(1,$E23,($F23-$S$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="5" t="n">
+        <f aca="false">IF(E23&gt;2,(1-_xlfn.BINOM.DIST(2,$E23,($F23-$R$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="5" t="n">
+        <f aca="false">IF(E23&gt;2,(1-_xlfn.BINOM.DIST(2,$E23,($F23-$S$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="5" t="n">
+        <f aca="false">IF(E23&gt;3,(1-_xlfn.BINOM.DIST(3,$E23,($F23-$R$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="5" t="n">
+        <f aca="false">IF(E23&gt;3,(1-_xlfn.BINOM.DIST(3,$E23,($F23-$S$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="5" t="n">
+        <f aca="false">IF(E23&gt;4,(1-_xlfn.BINOM.DIST(4,$E23,($F23-$R$2+1)/$F23,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="5" t="n">
+        <f aca="false">IF(E23&gt;4,(1-_xlfn.BINOM.DIST(4,$E23,($F23-$S$2+1)/$F23,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="74" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G25" s="5" t="n">
+        <f aca="false">IF(E25&gt;0,(1-_xlfn.BINOM.DIST(0,$E25,($F25-$R$2+1)/$F25,1)),0)</f>
+        <v>0.888888888888889</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <f aca="false">IF(E25&gt;0,(1-_xlfn.BINOM.DIST(0,$E25,($F25-$S$2+1)/$F25,1)),0)</f>
+        <v>0.555555555555555</v>
+      </c>
+      <c r="I25" s="5" t="n">
+        <f aca="false">IF(E25&gt;1,(1-_xlfn.BINOM.DIST(1,$E25,($F25-$R$2+1)/$F25,1)),0)</f>
+        <v>0.444444444444444</v>
+      </c>
+      <c r="J25" s="5" t="n">
+        <f aca="false">IF(E25&gt;1,(1-_xlfn.BINOM.DIST(1,$E25,($F25-$S$2+1)/$F25,1)),0)</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="K25" s="5" t="n">
+        <f aca="false">IF(E25&gt;2,(1-_xlfn.BINOM.DIST(2,$E25,($F25-$R$2+1)/$F25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="5" t="n">
+        <f aca="false">IF(E25&gt;2,(1-_xlfn.BINOM.DIST(2,$E25,($F25-$S$2+1)/$F25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="5" t="n">
+        <f aca="false">IF(E25&gt;3,(1-_xlfn.BINOM.DIST(3,$E25,($F25-$R$2+1)/$F25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="5" t="n">
+        <f aca="false">IF(E25&gt;3,(1-_xlfn.BINOM.DIST(3,$E25,($F25-$S$2+1)/$F25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="5" t="n">
+        <f aca="false">IF(E25&gt;4,(1-_xlfn.BINOM.DIST(4,$E25,($F25-$R$2+1)/$F25,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="5" t="n">
+        <f aca="false">IF(E25&gt;4,(1-_xlfn.BINOM.DIST(4,$E25,($F25-$S$2+1)/$F25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="78" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5" t="n">
+        <f aca="false">IF(E26&gt;0,(1-_xlfn.BINOM.DIST(0,$E26,($F26-$R$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="5" t="n">
+        <f aca="false">IF(E26&gt;0,(1-_xlfn.BINOM.DIST(0,$E26,($F26-$S$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="5" t="n">
+        <f aca="false">IF(E26&gt;1,(1-_xlfn.BINOM.DIST(1,$E26,($F26-$R$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="5" t="n">
+        <f aca="false">IF(E26&gt;1,(1-_xlfn.BINOM.DIST(1,$E26,($F26-$S$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="5" t="n">
+        <f aca="false">IF(E26&gt;2,(1-_xlfn.BINOM.DIST(2,$E26,($F26-$R$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <f aca="false">IF(E26&gt;2,(1-_xlfn.BINOM.DIST(2,$E26,($F26-$S$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="5" t="n">
+        <f aca="false">IF(E26&gt;3,(1-_xlfn.BINOM.DIST(3,$E26,($F26-$R$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="5" t="n">
+        <f aca="false">IF(E26&gt;3,(1-_xlfn.BINOM.DIST(3,$E26,($F26-$S$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="5" t="n">
+        <f aca="false">IF(E26&gt;4,(1-_xlfn.BINOM.DIST(4,$E26,($F26-$R$2+1)/$F26,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="5" t="n">
+        <f aca="false">IF(E26&gt;4,(1-_xlfn.BINOM.DIST(4,$E26,($F26-$S$2+1)/$F26,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5" t="n">
+        <f aca="false">IF(E27&gt;0,(1-_xlfn.BINOM.DIST(0,$E27,($F27-$R$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="5" t="n">
+        <f aca="false">IF(E27&gt;0,(1-_xlfn.BINOM.DIST(0,$E27,($F27-$S$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="5" t="n">
+        <f aca="false">IF(E27&gt;1,(1-_xlfn.BINOM.DIST(1,$E27,($F27-$R$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5" t="n">
+        <f aca="false">IF(E27&gt;1,(1-_xlfn.BINOM.DIST(1,$E27,($F27-$S$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="5" t="n">
+        <f aca="false">IF(E27&gt;2,(1-_xlfn.BINOM.DIST(2,$E27,($F27-$R$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="5" t="n">
+        <f aca="false">IF(E27&gt;2,(1-_xlfn.BINOM.DIST(2,$E27,($F27-$S$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="5" t="n">
+        <f aca="false">IF(E27&gt;3,(1-_xlfn.BINOM.DIST(3,$E27,($F27-$R$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="5" t="n">
+        <f aca="false">IF(E27&gt;3,(1-_xlfn.BINOM.DIST(3,$E27,($F27-$S$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5" t="n">
+        <f aca="false">IF(E27&gt;4,(1-_xlfn.BINOM.DIST(4,$E27,($F27-$R$2+1)/$F27,1)),)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="5" t="n">
+        <f aca="false">IF(E27&gt;4,(1-_xlfn.BINOM.DIST(4,$E27,($F27-$S$2+1)/$F27,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <f aca="false">IF(E29&gt;0,(1-_xlfn.BINOM.DIST(0,$E29,0.75,1)),0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <f aca="false">IF(E29&gt;0,(1-_xlfn.BINOM.DIST(0,$E29,0.25,1)),0)</f>
+        <v>0.25</v>
+      </c>
+      <c r="I29" s="5" t="n">
+        <f aca="false">IF(E29&gt;1,(1-_xlfn.BINOM.DIST(1,$E29,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="5" t="n">
+        <f aca="false">IF(E29&gt;1,(1-_xlfn.BINOM.DIST(1,$E29,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="5" t="n">
+        <f aca="false">IF(E29&gt;2,(1-_xlfn.BINOM.DIST(2,$E29,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="5" t="n">
+        <f aca="false">IF(E29&gt;2,(1-_xlfn.BINOM.DIST(2,$E29,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="5" t="n">
+        <f aca="false">IF(E29&gt;3,(1-_xlfn.BINOM.DIST(3,$E29,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="5" t="n">
+        <f aca="false">IF(E29&gt;3,(1-_xlfn.BINOM.DIST(3,$E29,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="5" t="n">
+        <f aca="false">IF(E29&gt;4,(1-_xlfn.BINOM.DIST(4,$E29,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="5" t="n">
+        <f aca="false">IF(E29&gt;4,(1-_xlfn.BINOM.DIST(4,$E29,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <f aca="false">IF(E30&gt;0,(1-_xlfn.BINOM.DIST(0,$E30,0.75,1)),0)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="H30" s="5" t="n">
+        <f aca="false">IF(E30&gt;0,(1-_xlfn.BINOM.DIST(0,$E30,0.25,1)),0)</f>
+        <v>0.4375</v>
+      </c>
+      <c r="I30" s="5" t="n">
+        <f aca="false">IF(E30&gt;1,(1-_xlfn.BINOM.DIST(1,$E30,0.75,1)),0)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="J30" s="5" t="n">
+        <f aca="false">IF(E30&gt;1,(1-_xlfn.BINOM.DIST(1,$E30,0.25,1)),0)</f>
+        <v>0.0625</v>
+      </c>
+      <c r="K30" s="5" t="n">
+        <f aca="false">IF(E30&gt;2,(1-_xlfn.BINOM.DIST(2,$E30,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <f aca="false">IF(E30&gt;2,(1-_xlfn.BINOM.DIST(2,$E30,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="5" t="n">
+        <f aca="false">IF(E30&gt;3,(1-_xlfn.BINOM.DIST(3,$E30,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="5" t="n">
+        <f aca="false">IF(E30&gt;3,(1-_xlfn.BINOM.DIST(3,$E30,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="5" t="n">
+        <f aca="false">IF(E30&gt;4,(1-_xlfn.BINOM.DIST(4,$E30,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="5" t="n">
+        <f aca="false">IF(E30&gt;4,(1-_xlfn.BINOM.DIST(4,$E30,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <f aca="false">IF(E31&gt;0,(1-_xlfn.BINOM.DIST(0,$E31,0.75,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <f aca="false">IF(E31&gt;0,(1-_xlfn.BINOM.DIST(0,$E31,0.25,1)),0)</f>
+        <v>0.578125</v>
+      </c>
+      <c r="I31" s="5" t="n">
+        <f aca="false">IF(E31&gt;1,(1-_xlfn.BINOM.DIST(1,$E31,0.75,1)),0)</f>
+        <v>0.84375</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <f aca="false">IF(E31&gt;1,(1-_xlfn.BINOM.DIST(1,$E31,0.25,1)),0)</f>
+        <v>0.15625</v>
+      </c>
+      <c r="K31" s="5" t="n">
+        <f aca="false">IF(E31&gt;2,(1-_xlfn.BINOM.DIST(2,$E31,0.75,1)),0)</f>
+        <v>0.421875</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <f aca="false">IF(E31&gt;2,(1-_xlfn.BINOM.DIST(2,$E31,0.25,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="M31" s="5" t="n">
+        <f aca="false">IF(E31&gt;3,(1-_xlfn.BINOM.DIST(3,$E31,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <f aca="false">IF(E31&gt;3,(1-_xlfn.BINOM.DIST(3,$E31,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="5" t="n">
+        <f aca="false">IF(E31&gt;4,(1-_xlfn.BINOM.DIST(4,$E31,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <f aca="false">IF(E31&gt;4,(1-_xlfn.BINOM.DIST(4,$E31,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G32" s="5" t="n">
+        <f aca="false">IF(E32&gt;0,(1-_xlfn.BINOM.DIST(0,$E32,0.75,1)),0)</f>
+        <v>0.99609375</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <f aca="false">IF(E32&gt;0,(1-_xlfn.BINOM.DIST(0,$E32,0.25,1)),0)</f>
+        <v>0.68359375</v>
+      </c>
+      <c r="I32" s="5" t="n">
+        <f aca="false">IF(E32&gt;1,(1-_xlfn.BINOM.DIST(1,$E32,0.75,1)),0)</f>
+        <v>0.94921875</v>
+      </c>
+      <c r="J32" s="5" t="n">
+        <f aca="false">IF(E32&gt;1,(1-_xlfn.BINOM.DIST(1,$E32,0.25,1)),0)</f>
+        <v>0.26171875</v>
+      </c>
+      <c r="K32" s="5" t="n">
+        <f aca="false">IF(E32&gt;2,(1-_xlfn.BINOM.DIST(2,$E32,0.75,1)),0)</f>
+        <v>0.73828125</v>
+      </c>
+      <c r="L32" s="5" t="n">
+        <f aca="false">IF(E32&gt;2,(1-_xlfn.BINOM.DIST(2,$E32,0.25,1)),0)</f>
+        <v>0.05078125</v>
+      </c>
+      <c r="M32" s="5" t="n">
+        <f aca="false">IF(E32&gt;3,(1-_xlfn.BINOM.DIST(3,$E32,0.75,1)),0)</f>
+        <v>0.31640625</v>
+      </c>
+      <c r="N32" s="5" t="n">
+        <f aca="false">IF(E32&gt;3,(1-_xlfn.BINOM.DIST(3,$E32,0.25,1)),0)</f>
+        <v>0.00390625</v>
+      </c>
+      <c r="O32" s="5" t="n">
+        <f aca="false">IF(E32&gt;4,(1-_xlfn.BINOM.DIST(4,$E32,0.75,1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="5" t="n">
+        <f aca="false">IF(E32&gt;4,(1-_xlfn.BINOM.DIST(4,$E32,0.25,1)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5" t="n">
+        <f aca="false">IF(E33&gt;0,(1-_xlfn.BINOM.DIST(0,$E33,0.75,1)),0)</f>
+        <v>0.9990234375</v>
+      </c>
+      <c r="H33" s="5" t="n">
+        <f aca="false">IF(E33&gt;0,(1-_xlfn.BINOM.DIST(0,$E33,0.25,1)),0)</f>
+        <v>0.7626953125</v>
+      </c>
+      <c r="I33" s="5" t="n">
+        <f aca="false">IF(E33&gt;1,(1-_xlfn.BINOM.DIST(1,$E33,0.75,1)),0)</f>
+        <v>0.984375</v>
+      </c>
+      <c r="J33" s="5" t="n">
+        <f aca="false">IF(E33&gt;1,(1-_xlfn.BINOM.DIST(1,$E33,0.25,1)),0)</f>
+        <v>0.3671875</v>
+      </c>
+      <c r="K33" s="5" t="n">
+        <f aca="false">IF(E33&gt;2,(1-_xlfn.BINOM.DIST(2,$E33,0.75,1)),0)</f>
+        <v>0.896484375</v>
+      </c>
+      <c r="L33" s="5" t="n">
+        <f aca="false">IF(E33&gt;2,(1-_xlfn.BINOM.DIST(2,$E33,0.25,1)),0)</f>
+        <v>0.103515625</v>
+      </c>
+      <c r="M33" s="5" t="n">
+        <f aca="false">IF(E33&gt;3,(1-_xlfn.BINOM.DIST(3,$E33,0.75,1)),0)</f>
+        <v>0.6328125</v>
+      </c>
+      <c r="N33" s="5" t="n">
+        <f aca="false">IF(E33&gt;3,(1-_xlfn.BINOM.DIST(3,$E33,0.25,1)),0)</f>
+        <v>0.015625</v>
+      </c>
+      <c r="O33" s="5" t="n">
+        <f aca="false">IF(E33&gt;4,(1-_xlfn.BINOM.DIST(4,$E33,0.75,1)),0)</f>
+        <v>0.2373046875</v>
+      </c>
+      <c r="P33" s="5" t="n">
+        <f aca="false">IF(E33&gt;4,(1-_xlfn.BINOM.DIST(4,$E33,0.25,1)),0)</f>
+        <v>0.0009765625</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G34" s="5" t="n">
+        <f aca="false">IF(E34&gt;0,(1-_xlfn.BINOM.DIST(0,$E34,0.75,1)),0)</f>
+        <v>0.999755859375</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <f aca="false">IF(E34&gt;0,(1-_xlfn.BINOM.DIST(0,$E34,0.25,1)),0)</f>
+        <v>0.822021484375</v>
+      </c>
+      <c r="I34" s="5" t="n">
+        <f aca="false">IF(E34&gt;1,(1-_xlfn.BINOM.DIST(1,$E34,0.75,1)),0)</f>
+        <v>0.995361328125</v>
+      </c>
+      <c r="J34" s="5" t="n">
+        <f aca="false">IF(E34&gt;1,(1-_xlfn.BINOM.DIST(1,$E34,0.25,1)),0)</f>
+        <v>0.466064453125</v>
+      </c>
+      <c r="K34" s="5" t="n">
+        <f aca="false">IF(E34&gt;2,(1-_xlfn.BINOM.DIST(2,$E34,0.75,1)),0)</f>
+        <v>0.96240234375</v>
+      </c>
+      <c r="L34" s="5" t="n">
+        <f aca="false">IF(E34&gt;2,(1-_xlfn.BINOM.DIST(2,$E34,0.25,1)),0)</f>
+        <v>0.16943359375</v>
+      </c>
+      <c r="M34" s="5" t="n">
+        <f aca="false">IF(E34&gt;3,(1-_xlfn.BINOM.DIST(3,$E34,0.75,1)),0)</f>
+        <v>0.83056640625</v>
+      </c>
+      <c r="N34" s="5" t="n">
+        <f aca="false">IF(E34&gt;3,(1-_xlfn.BINOM.DIST(3,$E34,0.25,1)),0)</f>
+        <v>0.03759765625</v>
+      </c>
+      <c r="O34" s="5" t="n">
+        <f aca="false">IF(E34&gt;4,(1-_xlfn.BINOM.DIST(4,$E34,0.75,1)),0)</f>
+        <v>0.533935546875</v>
+      </c>
+      <c r="P34" s="5" t="n">
+        <f aca="false">IF(E34&gt;4,(1-_xlfn.BINOM.DIST(4,$E34,0.25,1)),0)</f>
+        <v>0.004638671875</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G35" s="5" t="n">
+        <f aca="false">IF(E35&gt;0,(1-_xlfn.BINOM.DIST(0,$E35,0.75,1)),0)</f>
+        <v>0.99993896484375</v>
+      </c>
+      <c r="H35" s="5" t="n">
+        <f aca="false">IF(E35&gt;0,(1-_xlfn.BINOM.DIST(0,$E35,0.25,1)),0)</f>
+        <v>0.86651611328125</v>
+      </c>
+      <c r="I35" s="5" t="n">
+        <f aca="false">IF(E35&gt;1,(1-_xlfn.BINOM.DIST(1,$E35,0.75,1)),0)</f>
+        <v>0.9986572265625</v>
+      </c>
+      <c r="J35" s="5" t="n">
+        <f aca="false">IF(E35&gt;1,(1-_xlfn.BINOM.DIST(1,$E35,0.25,1)),0)</f>
+        <v>0.5550537109375</v>
+      </c>
+      <c r="K35" s="5" t="n">
+        <f aca="false">IF(E35&gt;2,(1-_xlfn.BINOM.DIST(2,$E35,0.75,1)),0)</f>
+        <v>0.98712158203125</v>
+      </c>
+      <c r="L35" s="5" t="n">
+        <f aca="false">IF(E35&gt;2,(1-_xlfn.BINOM.DIST(2,$E35,0.25,1)),0)</f>
+        <v>0.24359130859375</v>
+      </c>
+      <c r="M35" s="5" t="n">
+        <f aca="false">IF(E35&gt;3,(1-_xlfn.BINOM.DIST(3,$E35,0.75,1)),0)</f>
+        <v>0.929443359375</v>
+      </c>
+      <c r="N35" s="5" t="n">
+        <f aca="false">IF(E35&gt;3,(1-_xlfn.BINOM.DIST(3,$E35,0.25,1)),0)</f>
+        <v>0.070556640625</v>
+      </c>
+      <c r="O35" s="5" t="n">
+        <f aca="false">IF(E35&gt;4,(1-_xlfn.BINOM.DIST(4,$E35,0.75,1)),0)</f>
+        <v>0.75640869140625</v>
+      </c>
+      <c r="P35" s="5" t="n">
+        <f aca="false">IF(E35&gt;4,(1-_xlfn.BINOM.DIST(4,$E35,0.25,1)),0)</f>
+        <v>0.01287841796875</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G36" s="5" t="n">
+        <f aca="false">IF(E36&gt;0,(1-_xlfn.BINOM.DIST(0,$E36,0.75,1)),0)</f>
+        <v>0.999984741210938</v>
+      </c>
+      <c r="H36" s="5" t="n">
+        <f aca="false">IF(E36&gt;0,(1-_xlfn.BINOM.DIST(0,$E36,0.25,1)),0)</f>
+        <v>0.899887084960938</v>
+      </c>
+      <c r="I36" s="5" t="n">
+        <f aca="false">IF(E36&gt;1,(1-_xlfn.BINOM.DIST(1,$E36,0.75,1)),0)</f>
+        <v>0.999618530273438</v>
+      </c>
+      <c r="J36" s="5" t="n">
+        <f aca="false">IF(E36&gt;1,(1-_xlfn.BINOM.DIST(1,$E36,0.25,1)),0)</f>
+        <v>0.632919311523438</v>
+      </c>
+      <c r="K36" s="5" t="n">
+        <f aca="false">IF(E36&gt;2,(1-_xlfn.BINOM.DIST(2,$E36,0.75,1)),0)</f>
+        <v>0.995773315429688</v>
+      </c>
+      <c r="L36" s="5" t="n">
+        <f aca="false">IF(E36&gt;2,(1-_xlfn.BINOM.DIST(2,$E36,0.25,1)),0)</f>
+        <v>0.321456909179687</v>
+      </c>
+      <c r="M36" s="5" t="n">
+        <f aca="false">IF(E36&gt;3,(1-_xlfn.BINOM.DIST(3,$E36,0.75,1)),0)</f>
+        <v>0.972702026367188</v>
+      </c>
+      <c r="N36" s="5" t="n">
+        <f aca="false">IF(E36&gt;3,(1-_xlfn.BINOM.DIST(3,$E36,0.25,1)),0)</f>
+        <v>0.113815307617188</v>
+      </c>
+      <c r="O36" s="5" t="n">
+        <f aca="false">IF(E36&gt;4,(1-_xlfn.BINOM.DIST(4,$E36,0.75,1)),0)</f>
+        <v>0.886184692382813</v>
+      </c>
+      <c r="P36" s="5" t="n">
+        <f aca="false">IF(E36&gt;4,(1-_xlfn.BINOM.DIST(4,$E36,0.25,1)),0)</f>
+        <v>0.0272979736328125</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G37:Q1048576 G28:Q28 G31:Q33 Q23:Q24 G1:P4 G6:P24 Q1:Q8 Q15 Q18">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G29:Q36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:Q27">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:P5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q10">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q12">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q13">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q19">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q21">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q22">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="1" sqref="R1:S2 I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10340,13 +12740,13 @@
         <v>124</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="I1" s="44" t="s">
         <v>94</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
@@ -10365,24 +12765,24 @@
         <v>97</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="G2" s="44" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="I2" s="44" t="s">
         <v>98</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>156</v>
+        <v>215</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -10397,13 +12797,13 @@
         <v>97</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>98</v>
@@ -10423,13 +12823,13 @@
         <v>97</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>98</v>
@@ -10452,19 +12852,19 @@
         <v>97</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>101</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10481,13 +12881,13 @@
         <v>97</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>101</v>
@@ -10590,7 +12990,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>157</v>
+        <v>216</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
@@ -10611,10 +13011,10 @@
         <v>10</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>158</v>
+        <v>217</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10732,885 +13132,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AMJ16"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R2" activeCellId="0" sqref="R1:S2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="4" style="5" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="74" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="74" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="74" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>165</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="I1" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="J1" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="K1" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="L1" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="M1" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="P1" s="74" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q1" s="74" t="s">
-        <v>173</v>
-      </c>
-      <c r="R1" s="74" t="s">
-        <v>125</v>
-      </c>
-      <c r="U1" s="0"/>
-      <c r="V1" s="0"/>
-      <c r="W1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="e">
-        <f aca="false">IF(B2&gt;0,(1-_xlfn.BINOM.DIST(0,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E2" s="5" t="e">
-        <f aca="false">IF(B2&gt;0,(1-_xlfn.BINOM.DIST(0,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F2" s="5" t="e">
-        <f aca="false">=IF(B2&gt;1,(1-_xlfn.BINOM.DIST(1,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G2" s="5" t="e">
-        <f aca="false">IF(B2&gt;1,(1-_xlfn.BINOM.DIST(1,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <f aca="false">IF(B2&gt;2,(1-_xlfn.BINOM.DIST(2,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <f aca="false">IF(B2&gt;2,(1-_xlfn.BINOM.DIST(2,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <f aca="false">IF(B2&gt;3,(1-_xlfn.BINOM.DIST(3,$B2,($C2-$P$2+1)/$C2,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <f aca="false">IF(B2&gt;3,(1-_xlfn.BINOM.DIST(3,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <f aca="false">IF(B2&gt;4,(1-_xlfn.BINOM.DIST(4,$B2,($C2-$P$2+1)/$C2,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <f aca="false">IF(B2&gt;4,(1-_xlfn.BINOM.DIST(4,$B2,($C2-$Q$2+1)/$C2,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <f aca="false">3+R2</f>
-        <v>7</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <f aca="false">5+R2</f>
-        <v>9</v>
-      </c>
-      <c r="R2" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <f aca="false">IF(B3&gt;0,(1-_xlfn.BINOM.DIST(0,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="e">
-        <f aca="false">IF(B3&gt;0,(1-_xlfn.BINOM.DIST(0,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <f aca="false">=IF(B3&gt;1,(1-_xlfn.BINOM.DIST(1,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="5" t="e">
-        <f aca="false">IF(B3&gt;1,(1-_xlfn.BINOM.DIST(1,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <f aca="false">IF(B3&gt;2,(1-_xlfn.BINOM.DIST(2,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <f aca="false">IF(B3&gt;2,(1-_xlfn.BINOM.DIST(2,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <f aca="false">IF(B3&gt;3,(1-_xlfn.BINOM.DIST(3,$B3,($C3-$P$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <f aca="false">IF(B3&gt;3,(1-_xlfn.BINOM.DIST(3,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <f aca="false">IF(B3&gt;4,(1-_xlfn.BINOM.DIST(4,$B3,($C3-$P$2+1)/$C3,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <f aca="false">IF(B3&gt;4,(1-_xlfn.BINOM.DIST(4,$B3,($C3-$Q$2+1)/$C3,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <f aca="false">IF(B4&gt;0,(1-_xlfn.BINOM.DIST(0,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
-        <v>0.578125</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <f aca="false">IF(B4&gt;0,(1-_xlfn.BINOM.DIST(0,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">=IF(B4&gt;1,(1-_xlfn.BINOM.DIST(1,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <f aca="false">IF(B4&gt;1,(1-_xlfn.BINOM.DIST(1,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <f aca="false">IF(B4&gt;2,(1-_xlfn.BINOM.DIST(2,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
-        <v>0.015625</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <f aca="false">IF(B4&gt;2,(1-_xlfn.BINOM.DIST(2,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <f aca="false">IF(B4&gt;3,(1-_xlfn.BINOM.DIST(3,$B4,($C4-$P$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <f aca="false">IF(B4&gt;3,(1-_xlfn.BINOM.DIST(3,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <f aca="false">IF(B4&gt;4,(1-_xlfn.BINOM.DIST(4,$B4,($C4-$P$2+1)/$C4,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <f aca="false">IF(B4&gt;4,(1-_xlfn.BINOM.DIST(4,$B4,($C4-$Q$2+1)/$C4,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">IF(B5&gt;0,(1-_xlfn.BINOM.DIST(0,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
-        <v>0.578125</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <f aca="false">IF(B5&gt;0,(1-_xlfn.BINOM.DIST(0,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">=IF(B5&gt;1,(1-_xlfn.BINOM.DIST(1,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <f aca="false">IF(B5&gt;1,(1-_xlfn.BINOM.DIST(1,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <f aca="false">IF(B5&gt;2,(1-_xlfn.BINOM.DIST(2,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
-        <v>0.015625</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <f aca="false">IF(B5&gt;2,(1-_xlfn.BINOM.DIST(2,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <f aca="false">IF(B5&gt;3,(1-_xlfn.BINOM.DIST(3,$B5,($C5-$P$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <f aca="false">IF(B5&gt;3,(1-_xlfn.BINOM.DIST(3,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <f aca="false">IF(B5&gt;4,(1-_xlfn.BINOM.DIST(4,$B5,($C5-$P$2+1)/$C5,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <f aca="false">IF(B5&gt;4,(1-_xlfn.BINOM.DIST(4,$B5,($C5-$Q$2+1)/$C5,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <f aca="false">IF(B6&gt;0,(1-_xlfn.BINOM.DIST(0,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
-        <v>0.75</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <f aca="false">IF(B6&gt;0,(1-_xlfn.BINOM.DIST(0,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
-        <v>0.555555555555555</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <f aca="false">=IF(B6&gt;1,(1-_xlfn.BINOM.DIST(1,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
-        <v>0.25</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <f aca="false">IF(B6&gt;1,(1-_xlfn.BINOM.DIST(1,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
-        <v>0.111111111111111</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <f aca="false">IF(B6&gt;2,(1-_xlfn.BINOM.DIST(2,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <f aca="false">IF(B6&gt;2,(1-_xlfn.BINOM.DIST(2,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <f aca="false">IF(B6&gt;3,(1-_xlfn.BINOM.DIST(3,$B6,($C6-$P$2+1)/$C6,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <f aca="false">IF(B6&gt;3,(1-_xlfn.BINOM.DIST(3,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <f aca="false">IF(B6&gt;4,(1-_xlfn.BINOM.DIST(4,$B6,($C6-$P$2+1)/$C6,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <f aca="false">IF(B6&gt;4,(1-_xlfn.BINOM.DIST(4,$B6,($C6-$Q$2+1)/$C6,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <f aca="false">IF(B7&gt;0,(1-_xlfn.BINOM.DIST(0,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
-        <v>0.784</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <f aca="false">IF(B7&gt;0,(1-_xlfn.BINOM.DIST(0,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
-        <v>0.488</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <f aca="false">=IF(B7&gt;1,(1-_xlfn.BINOM.DIST(1,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
-        <v>0.352</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <f aca="false">IF(B7&gt;1,(1-_xlfn.BINOM.DIST(1,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
-        <v>0.104</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <f aca="false">IF(B7&gt;2,(1-_xlfn.BINOM.DIST(2,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
-        <v>0.0639999999999998</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <f aca="false">IF(B7&gt;2,(1-_xlfn.BINOM.DIST(2,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
-        <v>0.00799999999999956</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <f aca="false">IF(B7&gt;3,(1-_xlfn.BINOM.DIST(3,$B7,($C7-$P$2+1)/$C7,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <f aca="false">IF(B7&gt;3,(1-_xlfn.BINOM.DIST(3,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <f aca="false">IF(B7&gt;4,(1-_xlfn.BINOM.DIST(4,$B7,($C7-$P$2+1)/$C7,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <f aca="false">IF(B7&gt;4,(1-_xlfn.BINOM.DIST(4,$B7,($C7-$Q$2+1)/$C7,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <f aca="false">IF(B8&gt;0,(1-_xlfn.BINOM.DIST(0,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
-        <v>0.578125</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <f aca="false">IF(B8&gt;0,(1-_xlfn.BINOM.DIST(0,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <f aca="false">=IF(B8&gt;1,(1-_xlfn.BINOM.DIST(1,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <f aca="false">IF(B8&gt;1,(1-_xlfn.BINOM.DIST(1,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <f aca="false">IF(B8&gt;2,(1-_xlfn.BINOM.DIST(2,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
-        <v>0.015625</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <f aca="false">IF(B8&gt;2,(1-_xlfn.BINOM.DIST(2,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <f aca="false">IF(B8&gt;3,(1-_xlfn.BINOM.DIST(3,$B8,($C8-$P$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <f aca="false">IF(B8&gt;3,(1-_xlfn.BINOM.DIST(3,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <f aca="false">IF(B8&gt;4,(1-_xlfn.BINOM.DIST(4,$B8,($C8-$P$2+1)/$C8,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <f aca="false">IF(B8&gt;4,(1-_xlfn.BINOM.DIST(4,$B8,($C8-$Q$2+1)/$C8,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <f aca="false">IF(B9&gt;0,(1-_xlfn.BINOM.DIST(0,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
-        <v>0.68359375</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <f aca="false">IF(B9&gt;0,(1-_xlfn.BINOM.DIST(0,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <f aca="false">=IF(B9&gt;1,(1-_xlfn.BINOM.DIST(1,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
-        <v>0.26171875</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <f aca="false">IF(B9&gt;1,(1-_xlfn.BINOM.DIST(1,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <f aca="false">IF(B9&gt;2,(1-_xlfn.BINOM.DIST(2,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
-        <v>0.05078125</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <f aca="false">IF(B9&gt;2,(1-_xlfn.BINOM.DIST(2,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <f aca="false">IF(B9&gt;3,(1-_xlfn.BINOM.DIST(3,$B9,($C9-$P$2+1)/$C9,1)),0)</f>
-        <v>0.00390625</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <f aca="false">IF(B9&gt;3,(1-_xlfn.BINOM.DIST(3,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <f aca="false">IF(B9&gt;4,(1-_xlfn.BINOM.DIST(4,$B9,($C9-$P$2+1)/$C9,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <f aca="false">IF(B9&gt;4,(1-_xlfn.BINOM.DIST(4,$B9,($C9-$Q$2+1)/$C9,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <f aca="false">IF(B10&gt;0,(1-_xlfn.BINOM.DIST(0,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
-        <v>0.75</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <f aca="false">IF(B10&gt;0,(1-_xlfn.BINOM.DIST(0,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
-        <v>0.555555555555555</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <f aca="false">=IF(B10&gt;1,(1-_xlfn.BINOM.DIST(1,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <f aca="false">IF(B10&gt;1,(1-_xlfn.BINOM.DIST(1,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
-        <v>0.111111111111111</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <f aca="false">IF(B10&gt;2,(1-_xlfn.BINOM.DIST(2,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="n">
-        <f aca="false">IF(B10&gt;2,(1-_xlfn.BINOM.DIST(2,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="5" t="n">
-        <f aca="false">IF(B10&gt;3,(1-_xlfn.BINOM.DIST(3,$B10,($C10-$P$2+1)/$C10,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="5" t="n">
-        <f aca="false">IF(B10&gt;3,(1-_xlfn.BINOM.DIST(3,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="5" t="n">
-        <f aca="false">IF(B10&gt;4,(1-_xlfn.BINOM.DIST(4,$B10,($C10-$P$2+1)/$C10,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="5" t="n">
-        <f aca="false">IF(B10&gt;4,(1-_xlfn.BINOM.DIST(4,$B10,($C10-$Q$2+1)/$C10,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <f aca="false">IF(B11&gt;0,(1-_xlfn.BINOM.DIST(0,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
-        <v>0.875</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <f aca="false">IF(B11&gt;0,(1-_xlfn.BINOM.DIST(0,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
-        <v>0.703703703703704</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <f aca="false">=IF(B11&gt;1,(1-_xlfn.BINOM.DIST(1,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <f aca="false">IF(B11&gt;1,(1-_xlfn.BINOM.DIST(1,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
-        <v>0.259259259259259</v>
-      </c>
-      <c r="H11" s="5" t="n">
-        <f aca="false">IF(B11&gt;2,(1-_xlfn.BINOM.DIST(2,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
-        <v>0.125</v>
-      </c>
-      <c r="I11" s="5" t="n">
-        <f aca="false">IF(B11&gt;2,(1-_xlfn.BINOM.DIST(2,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
-        <v>0.0370370370370369</v>
-      </c>
-      <c r="J11" s="5" t="n">
-        <f aca="false">IF(B11&gt;3,(1-_xlfn.BINOM.DIST(3,$B11,($C11-$P$2+1)/$C11,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="5" t="n">
-        <f aca="false">IF(B11&gt;3,(1-_xlfn.BINOM.DIST(3,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="5" t="n">
-        <f aca="false">IF(B11&gt;4,(1-_xlfn.BINOM.DIST(4,$B11,($C11-$P$2+1)/$C11,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="5" t="n">
-        <f aca="false">IF(B11&gt;4,(1-_xlfn.BINOM.DIST(4,$B11,($C11-$Q$2+1)/$C11,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <f aca="false">IF(B12&gt;0,(1-_xlfn.BINOM.DIST(0,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
-        <v>0.784</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <f aca="false">IF(B12&gt;0,(1-_xlfn.BINOM.DIST(0,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
-        <v>0.488</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <f aca="false">=IF(B12&gt;1,(1-_xlfn.BINOM.DIST(1,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
-        <v>0.352</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <f aca="false">IF(B12&gt;1,(1-_xlfn.BINOM.DIST(1,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
-        <v>0.104</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <f aca="false">IF(B12&gt;2,(1-_xlfn.BINOM.DIST(2,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
-        <v>0.0639999999999998</v>
-      </c>
-      <c r="I12" s="5" t="n">
-        <f aca="false">IF(B12&gt;2,(1-_xlfn.BINOM.DIST(2,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
-        <v>0.00799999999999956</v>
-      </c>
-      <c r="J12" s="5" t="n">
-        <f aca="false">IF(B12&gt;3,(1-_xlfn.BINOM.DIST(3,$B12,($C12-$P$2+1)/$C12,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="5" t="n">
-        <f aca="false">IF(B12&gt;3,(1-_xlfn.BINOM.DIST(3,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="5" t="n">
-        <f aca="false">IF(B12&gt;4,(1-_xlfn.BINOM.DIST(4,$B12,($C12-$P$2+1)/$C12,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="5" t="n">
-        <f aca="false">IF(B12&gt;4,(1-_xlfn.BINOM.DIST(4,$B12,($C12-$Q$2+1)/$C12,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <f aca="false">IF(B13&gt;0,(1-_xlfn.BINOM.DIST(0,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
-        <v>0.8704</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <f aca="false">IF(B13&gt;0,(1-_xlfn.BINOM.DIST(0,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
-        <v>0.5904</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <f aca="false">=IF(B13&gt;1,(1-_xlfn.BINOM.DIST(1,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
-        <v>0.5248</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <f aca="false">IF(B13&gt;1,(1-_xlfn.BINOM.DIST(1,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
-        <v>0.1808</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <f aca="false">IF(B13&gt;2,(1-_xlfn.BINOM.DIST(2,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
-        <v>0.1792</v>
-      </c>
-      <c r="I13" s="5" t="n">
-        <f aca="false">IF(B13&gt;2,(1-_xlfn.BINOM.DIST(2,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
-        <v>0.0271999999999998</v>
-      </c>
-      <c r="J13" s="5" t="n">
-        <f aca="false">IF(B13&gt;3,(1-_xlfn.BINOM.DIST(3,$B13,($C13-$P$2+1)/$C13,1)),0)</f>
-        <v>0.0255999999999998</v>
-      </c>
-      <c r="K13" s="5" t="n">
-        <f aca="false">IF(B13&gt;3,(1-_xlfn.BINOM.DIST(3,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
-        <v>0.00159999999999982</v>
-      </c>
-      <c r="L13" s="5" t="n">
-        <f aca="false">IF(B13&gt;4,(1-_xlfn.BINOM.DIST(4,$B13,($C13-$P$2+1)/$C13,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="5" t="n">
-        <f aca="false">IF(B13&gt;4,(1-_xlfn.BINOM.DIST(4,$B13,($C13-$Q$2+1)/$C13,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <f aca="false">IF(B14&gt;0,(1-_xlfn.BINOM.DIST(0,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
-        <v>0.7626953125</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <f aca="false">IF(B14&gt;0,(1-_xlfn.BINOM.DIST(0,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <f aca="false">=IF(B14&gt;1,(1-_xlfn.BINOM.DIST(1,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
-        <v>0.3671875</v>
-      </c>
-      <c r="G14" s="5" t="n">
-        <f aca="false">IF(B14&gt;1,(1-_xlfn.BINOM.DIST(1,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <f aca="false">IF(B14&gt;2,(1-_xlfn.BINOM.DIST(2,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
-        <v>0.103515625</v>
-      </c>
-      <c r="I14" s="5" t="n">
-        <f aca="false">IF(B14&gt;2,(1-_xlfn.BINOM.DIST(2,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="5" t="n">
-        <f aca="false">IF(B14&gt;3,(1-_xlfn.BINOM.DIST(3,$B14,($C14-$P$2+1)/$C14,1)),0)</f>
-        <v>0.015625</v>
-      </c>
-      <c r="K14" s="5" t="n">
-        <f aca="false">IF(B14&gt;3,(1-_xlfn.BINOM.DIST(3,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="5" t="n">
-        <f aca="false">IF(B14&gt;4,(1-_xlfn.BINOM.DIST(4,$B14,($C14-$P$2+1)/$C14,1)),)</f>
-        <v>0.0009765625</v>
-      </c>
-      <c r="M14" s="5" t="n">
-        <f aca="false">IF(B14&gt;4,(1-_xlfn.BINOM.DIST(4,$B14,($C14-$Q$2+1)/$C14,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <f aca="false">IF(B15&gt;0,(1-_xlfn.BINOM.DIST(0,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
-        <v>0.9375</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <f aca="false">IF(B15&gt;0,(1-_xlfn.BINOM.DIST(0,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
-        <v>0.802469135802469</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <f aca="false">=IF(B15&gt;1,(1-_xlfn.BINOM.DIST(1,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
-        <v>0.6875</v>
-      </c>
-      <c r="G15" s="5" t="n">
-        <f aca="false">IF(B15&gt;1,(1-_xlfn.BINOM.DIST(1,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
-        <v>0.407407407407407</v>
-      </c>
-      <c r="H15" s="5" t="n">
-        <f aca="false">IF(B15&gt;2,(1-_xlfn.BINOM.DIST(2,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
-        <v>0.3125</v>
-      </c>
-      <c r="I15" s="5" t="n">
-        <f aca="false">IF(B15&gt;2,(1-_xlfn.BINOM.DIST(2,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
-        <v>0.111111111111111</v>
-      </c>
-      <c r="J15" s="5" t="n">
-        <f aca="false">IF(B15&gt;3,(1-_xlfn.BINOM.DIST(3,$B15,($C15-$P$2+1)/$C15,1)),0)</f>
-        <v>0.0625</v>
-      </c>
-      <c r="K15" s="5" t="n">
-        <f aca="false">IF(B15&gt;3,(1-_xlfn.BINOM.DIST(3,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
-        <v>0.0123456790123455</v>
-      </c>
-      <c r="L15" s="5" t="n">
-        <f aca="false">IF(B15&gt;4,(1-_xlfn.BINOM.DIST(4,$B15,($C15-$P$2+1)/$C15,1)),)</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="5" t="n">
-        <f aca="false">IF(B15&gt;4,(1-_xlfn.BINOM.DIST(4,$B15,($C15-$Q$2+1)/$C15,1)),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D16" s="5" t="n">
-        <f aca="false">IF(B16&gt;0,(1-_xlfn.BINOM.DIST(0,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
-        <v>0.92224</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <f aca="false">IF(B16&gt;0,(1-_xlfn.BINOM.DIST(0,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
-        <v>0.67232</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <f aca="false">=IF(B16&gt;1,(1-_xlfn.BINOM.DIST(1,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
-        <v>0.66304</v>
-      </c>
-      <c r="G16" s="5" t="n">
-        <f aca="false">IF(B16&gt;1,(1-_xlfn.BINOM.DIST(1,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
-        <v>0.26272</v>
-      </c>
-      <c r="H16" s="5" t="n">
-        <f aca="false">IF(B16&gt;2,(1-_xlfn.BINOM.DIST(2,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
-        <v>0.31744</v>
-      </c>
-      <c r="I16" s="5" t="n">
-        <f aca="false">IF(B16&gt;2,(1-_xlfn.BINOM.DIST(2,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
-        <v>0.0579199999999998</v>
-      </c>
-      <c r="J16" s="5" t="n">
-        <f aca="false">IF(B16&gt;3,(1-_xlfn.BINOM.DIST(3,$B16,($C16-$P$2+1)/$C16,1)),0)</f>
-        <v>0.0870400000000002</v>
-      </c>
-      <c r="K16" s="5" t="n">
-        <f aca="false">IF(B16&gt;3,(1-_xlfn.BINOM.DIST(3,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
-        <v>0.00671999999999973</v>
-      </c>
-      <c r="L16" s="5" t="n">
-        <f aca="false">IF(B16&gt;4,(1-_xlfn.BINOM.DIST(4,$B16,($C16-$P$2+1)/$C16,1)),)</f>
-        <v>0.0102400000000002</v>
-      </c>
-      <c r="M16" s="5" t="n">
-        <f aca="false">IF(B16&gt;4,(1-_xlfn.BINOM.DIST(4,$B16,($C16-$Q$2+1)/$C16,1)),0)</f>
-        <v>0.000319999999999765</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="D1:M1048576">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="num" val="0.6"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFBA131A"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF89C765"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -11618,8 +13139,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="1" sqref="R1:S2 K11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12028,8 +13549,8 @@
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="1" sqref="R1:S2 O7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12587,8 +14108,8 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="R1:S2 G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14477,8 +15998,8 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q20" activeCellId="1" sqref="R1:S2 Q20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q20" activeCellId="0" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16367,8 +17888,8 @@
   </sheetPr>
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P20" activeCellId="1" sqref="R1:S2 P20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18701,8 +20222,8 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="1" sqref="R1:S2 H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20590,8 +22111,8 @@
   </sheetPr>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="1" sqref="R1:S2 H29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23015,8 +24536,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D48" activeCellId="1" sqref="R1:S2 D48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23387,8 +24908,8 @@
   </sheetPr>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="1" sqref="R1:S2 G29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25977,8 +27498,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="R1:S2 E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Increased base weapon damage
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="238">
   <si>
     <t xml:space="preserve">Moves</t>
   </si>
@@ -726,29 +726,13 @@
     <t xml:space="preserve">Concealable, Light</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Throw, Light, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Forceful (-2 On opponents DR instead of -1, works with Minimum damage.)</t>
-    </r>
+    <t xml:space="preserve">Throw, Light, Forceful (-2 On opponents DR instead of -1)</t>
   </si>
   <si>
     <t xml:space="preserve">Longsword </t>
   </si>
   <si>
-    <t xml:space="preserve">Versatile (Double DB and +1 Guard when using in two hands)</t>
+    <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
   </si>
   <si>
     <t xml:space="preserve">WarHammer </t>
@@ -759,17 +743,8 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Versatile (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Double DB and +1 Guard </t>
+      <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
     </r>
     <r>
       <rPr>
@@ -778,103 +753,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> when using in two hands), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Forceful (-2 On opponents DR instead of -1, works with Minimum damage.)</t>
+      <t xml:space="preserve">, Forceful (-2 On opponents DR instead of -1)</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">Battle Axe </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Versatile (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Double DB and +1 Guard </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> when using in two hands)</t>
-    </r>
+    <t xml:space="preserve">Two Hand (Double DB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Two Hand (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Double DB and +1 Guard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Two Hand (Double DB), Forceful (-2 On opponents DR instead of -1)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Two Hand (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Double DB and +1 Guard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">), Forceful (-2 On opponents DR instead of -1)</t>
-    </r>
+    <t xml:space="preserve">Two Hand (Double DB and +1 Guard)</t>
   </si>
   <si>
     <t xml:space="preserve">Spear </t>
@@ -883,82 +775,19 @@
     <t xml:space="preserve">Optional Reach (Can Hit at 10ft), Versitile, Throw</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Reach (Can hit at 10ft, disadvantage at 5ft), Two Hand (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Double DB and +1 Guard</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Reach (Can hit at 10ft, disadvantage at 5ft), Two Hand (Double DB and +1 Guard)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Optional Reach </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Can Hit at 10ft)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, Versitile</t>
-    </r>
+    <t xml:space="preserve">Staff </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional Reach (Can Hit at 10ft), Versitile</t>
   </si>
   <si>
     <t xml:space="preserve">Shove Attack (push 5ft back instead of doing damage)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Shove Attack </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (push 5ft back instead of doing damage)</t>
-    </r>
+    <t xml:space="preserve">Shove Attack  (push 5ft back instead of doing damage)</t>
   </si>
 </sst>
 </file>
@@ -1744,13 +1573,13 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,11 +1702,11 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.7"/>
@@ -2241,10 +2070,10 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
@@ -4828,11 +4657,11 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
@@ -5111,13 +4940,13 @@
       <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.7"/>
@@ -7590,10 +7419,10 @@
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
@@ -9087,11 +8916,11 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="11.99"/>
@@ -9367,11 +9196,11 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
@@ -9804,18 +9633,18 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="58.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
@@ -9916,7 +9745,7 @@
         <v>49</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
@@ -9939,7 +9768,7 @@
         <v>46</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0</v>
@@ -9962,12 +9791,12 @@
         <v>46</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="79" t="s">
+      <c r="G5" s="2" t="s">
         <v>221</v>
       </c>
     </row>
@@ -9985,7 +9814,7 @@
         <v>49</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0</v>
@@ -10008,7 +9837,7 @@
         <v>49</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>2</v>
@@ -10031,16 +9860,16 @@
         <v>49</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>223</v>
       </c>
@@ -10054,7 +9883,7 @@
         <v>60</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>0</v>
@@ -10077,16 +9906,16 @@
         <v>60</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="79" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>227</v>
       </c>
@@ -10100,13 +9929,13 @@
         <v>60</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>228</v>
+      <c r="G11" s="79" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10123,13 +9952,13 @@
         <v>68</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10146,13 +9975,13 @@
         <v>68</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>4</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10169,13 +9998,13 @@
         <v>68</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10192,7 +10021,7 @@
         <v>60</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1</v>
@@ -10215,7 +10044,7 @@
         <v>68</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>4</v>
@@ -10226,7 +10055,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>77</v>
+        <v>234</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -10238,73 +10067,73 @@
         <v>60</v>
       </c>
       <c r="E17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="0" t="n">
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C18" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>234</v>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>83</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>0</v>
@@ -10313,103 +10142,17 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>8</v>
-      </c>
-    </row>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="G32:G1048576 G23 G26:G28 G19 G1:G8 G12 G15">
+  <conditionalFormatting sqref="G31:G1048576 G22 G25:G27 G18 G1:G8 G12 G15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10421,7 +10164,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:G31">
+  <conditionalFormatting sqref="G23:G30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10433,7 +10176,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G22">
+  <conditionalFormatting sqref="G19:G21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10529,18 +10272,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="num" val="0.6"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFBA131A"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF89C765"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -10562,7 +10293,7 @@
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
   </cols>
@@ -10971,7 +10702,7 @@
       <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="2.99"/>
   </cols>
@@ -11529,7 +11260,7 @@
       <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -13418,7 +13149,7 @@
       <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -15307,7 +15038,7 @@
       <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -17640,16 +17371,16 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="7" style="5" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7"/>
@@ -19969,7 +19700,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="3.57"/>
@@ -21857,7 +21588,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.57"/>
@@ -24279,9 +24010,9 @@
       <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
@@ -24650,10 +24381,10 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>

</xml_diff>

<commit_message>
working on armor pen
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -720,7 +720,7 @@
     <t xml:space="preserve">Base Damage</t>
   </si>
   <si>
-    <t xml:space="preserve">Min Damage</t>
+    <t xml:space="preserve">Armor Pen</t>
   </si>
   <si>
     <t xml:space="preserve">Concealable, Light</t>
@@ -738,23 +738,7 @@
     <t xml:space="preserve">WarHammer </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, Forceful (-2 On opponents DR instead of -1)</t>
-    </r>
+    <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands), Forceful (-2 On opponents DR instead of -1)</t>
   </si>
   <si>
     <t xml:space="preserve">Battle Axe </t>
@@ -775,7 +759,7 @@
     <t xml:space="preserve">Optional Reach (Can Hit at 10ft), Versitile, Throw</t>
   </si>
   <si>
-    <t xml:space="preserve">Reach (Can hit at 10ft, disadvantage at 5ft), Two Hand (Double DB and +1 Guard)</t>
+    <t xml:space="preserve">Reach (Can hit at 10ft, Two Hand (Double DB and +1 Guard)</t>
   </si>
   <si>
     <t xml:space="preserve">Staff </t>
@@ -800,7 +784,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -836,11 +820,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1059,7 +1038,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1376,10 +1355,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1573,7 +1548,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.3"/>
@@ -1702,7 +1677,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -2070,7 +2045,7 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
@@ -4657,7 +4632,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -4940,7 +4915,7 @@
       <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -7419,7 +7394,7 @@
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
@@ -8916,7 +8891,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -9196,7 +9171,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -9633,10 +9608,10 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
@@ -9759,7 +9734,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -9782,7 +9757,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -9911,7 +9886,7 @@
       <c r="F10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="79" t="s">
+      <c r="G10" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -9934,7 +9909,7 @@
       <c r="F11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="2" t="s">
         <v>224</v>
       </c>
     </row>
@@ -9955,7 +9930,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>228</v>
@@ -9978,7 +9953,7 @@
         <v>7</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>229</v>
@@ -10001,7 +9976,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>230</v>
@@ -10293,7 +10268,7 @@
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
   </cols>
@@ -10702,7 +10677,7 @@
       <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="2.99"/>
   </cols>
@@ -11260,7 +11235,7 @@
       <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -13149,7 +13124,7 @@
       <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.01171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -15038,7 +15013,7 @@
       <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -17371,7 +17346,7 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
@@ -19700,7 +19675,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="3.57"/>
@@ -21588,7 +21563,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.57"/>
@@ -24010,7 +23985,7 @@
       <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -24381,7 +24356,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>

</xml_diff>

<commit_message>
Weapons and armor 6.1
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Moves" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,8 +25,10 @@
     <sheet name="Armor 4.0" sheetId="15" state="hidden" r:id="rId16"/>
     <sheet name="Armor 5.0" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="Weapon 6.0" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Sheet2" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Sheet5" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Weapon 6.1" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Armor 6.1" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Sheet2" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Sheet5" sheetId="21" state="visible" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="259">
   <si>
     <t xml:space="preserve">Moves</t>
   </si>
@@ -723,10 +725,31 @@
     <t xml:space="preserve">Armor Pen</t>
   </si>
   <si>
+    <t xml:space="preserve">Skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brawling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concealable, Throw, Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blades/Brawling</t>
+  </si>
+  <si>
     <t xml:space="preserve">Concealable, Light</t>
   </si>
   <si>
-    <t xml:space="preserve">Throw, Light, Forceful (-2 On opponents DR instead of -1)</t>
+    <t xml:space="preserve">Short Sword / Rapier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blunt Weapons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axes</t>
   </si>
   <si>
     <t xml:space="preserve">Longsword </t>
@@ -735,10 +758,7 @@
     <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
   </si>
   <si>
-    <t xml:space="preserve">WarHammer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands), Forceful (-2 On opponents DR instead of -1)</t>
+    <t xml:space="preserve">WarHammer / Mace</t>
   </si>
   <si>
     <t xml:space="preserve">Battle Axe </t>
@@ -747,31 +767,140 @@
     <t xml:space="preserve">Two Hand (Double DB)</t>
   </si>
   <si>
-    <t xml:space="preserve">Two Hand (Double DB), Forceful (-2 On opponents DR instead of -1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two Hand (Double DB and +1 Guard)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spear </t>
   </si>
   <si>
-    <t xml:space="preserve">Optional Reach (Can Hit at 10ft), Versitile, Throw</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Reach (Can Hit at 10ft), Throw, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Reach (Can hit at 10ft, Two Hand (Double DB and +1 Guard)</t>
+    <t xml:space="preserve">Pole Arms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach (Can hit at 10ft, Two Hand (Double DB), Leverage (+3 damage and +3 AP when the opponent is farther then 5ft) </t>
   </si>
   <si>
     <t xml:space="preserve">Staff </t>
   </si>
   <si>
-    <t xml:space="preserve">Optional Reach (Can Hit at 10ft), Versitile</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Reach (Can Hit at 10ft), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Versatile (Double DB, +1 Guard, and +1 Min Damage when using in two hands)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Shield</t>
   </si>
   <si>
     <t xml:space="preserve">Shove Attack (push 5ft back instead of doing damage)</t>
   </si>
   <si>
     <t xml:space="preserve">Shove Attack  (push 5ft back instead of doing damage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damage Per Die (DPD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armor Penetration (AP) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versatile (+1 AP and Guard when using in two hands)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two Hand </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Reach (Can Hit at 10ft), Throw, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Versatile (+1 AP and Guard when using in two hands)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach (Can hit at 10ft, Two Hand (Double DB), Leverage (+1 DPD and SB when the opponent is farther then 5ft) </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Reach (Can Hit at 10ft), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Versatile (+1 AP and Guard when using in two hands)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Shove Attack (push 5ft back)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aim Bonus Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mana Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide/Leather Overcoat</t>
   </si>
 </sst>
 </file>
@@ -784,7 +913,7 @@
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -821,8 +950,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +991,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBCE4E5"/>
         <bgColor rgb="FFDCE6F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
   </fills>
@@ -1038,7 +1178,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1355,6 +1495,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1548,7 +1700,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.3"/>
@@ -1677,7 +1829,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -2045,7 +2197,7 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
@@ -4632,7 +4784,7 @@
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -4915,7 +5067,7 @@
       <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
@@ -7394,7 +7546,7 @@
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>
@@ -8891,7 +9043,7 @@
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -9168,10 +9320,10 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -9607,11 +9759,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
@@ -9620,7 +9772,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="58.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.29"/>
@@ -9650,13 +9802,7 @@
         <v>41</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>44</v>
+        <v>221</v>
       </c>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
@@ -9674,7 +9820,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>45</v>
+        <v>222</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -9691,19 +9837,8 @@
       <c r="F2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <f aca="false">3+J2</f>
-        <v>3</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <f aca="false">5+J2</f>
-        <v>5</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>0</v>
+      <c r="H2" s="0" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9725,8 +9860,8 @@
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>50</v>
+      <c r="H3" s="79" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9749,7 +9884,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>52</v>
+        <v>223</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9766,18 +9904,21 @@
         <v>46</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>55</v>
+        <v>226</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>2</v>
@@ -9796,6 +9937,9 @@
       </c>
       <c r="G6" s="11" t="s">
         <v>54</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9818,7 +9962,10 @@
         <v>2</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>222</v>
+        <v>57</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9843,10 +9990,13 @@
       <c r="G8" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>2</v>
@@ -9864,12 +10014,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -9887,12 +10040,15 @@
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>226</v>
+        <v>231</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -9910,7 +10066,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>224</v>
+        <v>231</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9933,10 +10092,13 @@
         <v>2</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>70</v>
       </c>
@@ -9956,7 +10118,10 @@
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>229</v>
+        <v>234</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9979,12 +10144,15 @@
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1</v>
@@ -10002,7 +10170,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>232</v>
+        <v>236</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10019,18 +10190,21 @@
         <v>68</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>238</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1</v>
@@ -10048,8 +10222,14 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>235</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" s="80" customFormat="true" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="81"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -10073,6 +10253,9 @@
       <c r="G19" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="H19" s="0" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -10094,7 +10277,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>236</v>
+        <v>242</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10117,7 +10303,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10163,7 +10352,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
+  <conditionalFormatting sqref="G10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10175,7 +10364,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+  <conditionalFormatting sqref="G11">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10187,7 +10376,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
+  <conditionalFormatting sqref="G13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10199,7 +10388,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
+  <conditionalFormatting sqref="G14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10211,7 +10400,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
+  <conditionalFormatting sqref="G16">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10223,7 +10412,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
+  <conditionalFormatting sqref="G17">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10235,7 +10424,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
+  <conditionalFormatting sqref="G9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -10262,400 +10451,709 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="n">
+    <row r="1" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="79" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="n">
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="n">
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="F14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" s="80" customFormat="true" ht="7.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="81"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
+      <c r="C21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <conditionalFormatting sqref="G31:G1048576 G22 G25:G27 G18 G1:G8 G12 G15">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23:G30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G21">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFBA131A"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF89C765"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -10671,555 +11169,501 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="2.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="42.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="n">
+    <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I3" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="n">
+      <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="n">
+      <c r="D4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="J4" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="C5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>213</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>213</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="J5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K5" s="0" t="n">
+      <c r="J5" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="L5" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
+      <c r="G11" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="C12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="C14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="L8" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="M8" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="L9" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="M9" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="G10" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="L11" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="M11" s="0" t="n">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="F12" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="L12" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="M12" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
+      <c r="G14" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -11232,10 +11676,10 @@
   <dimension ref="B1:W22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.03125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -13113,6 +13557,973 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="2.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -13124,7 +14535,7 @@
       <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.03125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -15013,7 +16424,7 @@
       <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -17342,11 +18753,11 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
@@ -19675,7 +21086,7 @@
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="3.57"/>
@@ -21563,7 +22974,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.57"/>
@@ -23985,7 +25396,7 @@
       <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
@@ -24356,7 +25767,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="9.13"/>

</xml_diff>

<commit_message>
added the start of actions
</commit_message>
<xml_diff>
--- a/rules/d10Chart_other.xlsx
+++ b/rules/d10Chart_other.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Moves" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,8 +27,9 @@
     <sheet name="Weapon 6.0" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Weapon 6.1" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Armor 6.1" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="Sheet2" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Sheet5" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Actions 6.1" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Sheet2" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Sheet5" sheetId="22" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="304">
   <si>
     <t xml:space="preserve">Moves</t>
   </si>
@@ -836,23 +837,7 @@
     <t xml:space="preserve">Short Reach (Disadvantage when attacking an opponent with a weapon size medium or larger who is guarding against you,while not grappled, advantage against opponents while grappling).</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Concealable, Throw, Light, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Short Reach (Disadvantage when attacking an opponent with a weapon size medium or larger who is guarding against you,while not grappled, advantage against opponents while grappling).</t>
-    </r>
+    <t xml:space="preserve">Concealable, Throw, Light, Short Reach (Disadvantage when attacking an opponent with a weapon size medium or larger who is guarding against you,while not grappled, advantage against opponents while grappling).</t>
   </si>
   <si>
     <t xml:space="preserve">Versatile (+1 DPD, AP and Guard when using in two hands)</t>
@@ -873,13 +858,13 @@
     <t xml:space="preserve">Two Hand </t>
   </si>
   <si>
-    <t xml:space="preserve">Reach (Can Hit at 10ft), Throw, Versatile (+1 DPD, AP and Guard when using in two hands)</t>
+    <t xml:space="preserve">Reach (When using two hands, can hit at 10ft, and while guarding melee attacks against you have disadvantage when the attacker start their turn outside of 5ft and they do not have reach.), Throw, Versatile (+1 DPD, AP and Guard when using in two hands)</t>
   </si>
   <si>
     <t xml:space="preserve">Spear (Two Hands)</t>
   </si>
   <si>
-    <t xml:space="preserve">Reach (Can hit at 10ft, Two Hand (Double DB), Leverage (+2 DPD and +1 SB when the opponent is farther then 5ft) </t>
+    <t xml:space="preserve">Reach, Two Hand, Leverage (+2 DPD and +1 SB when the opponent is farther then 5ft) </t>
   </si>
   <si>
     <t xml:space="preserve">Pole Axe (Leverage)</t>
@@ -888,7 +873,7 @@
     <t xml:space="preserve">Staff</t>
   </si>
   <si>
-    <t xml:space="preserve">Reach (Can Hit at 10ft), Versatile (+1 DPD, AP and Guard when using in two hands)</t>
+    <t xml:space="preserve">Reach, Versatile (+1 DPD, AP and Guard when using in two hands)</t>
   </si>
   <si>
     <t xml:space="preserve">Staff (Two Hands)</t>
@@ -917,25 +902,99 @@
   <si>
     <t xml:space="preserve">Hide/Leather Overcoat</t>
   </si>
+  <si>
+    <t xml:space="preserve">Brigantine Chest-piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Head</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental Skill 
+Reduction
+Applies to Focus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leather/Padded Cowl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain Mail Cowl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Face Helmet (Sallet, Viking Helm, Etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partially Closed Face Helm (Roman Legionnaire, Barbute,etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Enclosed Helm (Frog mouth, Armet Etc…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defensive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counter Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Stamina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choose one attack against you this turn, roll your main weapon attack and add your off hand weapons defense bonus to the roll (if applicable). The attack with the lower roll fails. The attack with the higher roll is successful and adds 1 to their weapons DPD. If the rolls are equal both attacks are successful and both add 1 their weapons DPD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cannot Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guard Stance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actively Guard yours against up to two attacks per turn, allowing you do use your reflex + your weapon defense bonuses as your Defense Rating against those attacks while you maintain this stance.
+The following breaks Guard Stance: Taking any other action other then Attack, Dodge or Sprint, moving more then your Base Move Speed (willingly or not), getting knocked prone, or taking a wound.
+On your first turn of any combat, you may do this as a Free Action.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base move in any direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attempt dodge all melee attacks targeting you. Roll the Dodge skill and subtract 1 for each additional attack against you after the first. If you roll above the attackers reflex, the dodge is success and their attack fails regardless of what they roll for it. You only roll once  and it is possible to only dodge some of the oncoming attacks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must move atleast 5ft in an empty 5ft area. If not available then this action automatically fails. Can move up to Base move, but all moved through spaces must be empty.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="@"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="General"/>
-    <numFmt numFmtId="168" formatCode="0.00%"/>
-    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -957,7 +1016,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -965,23 +1023,10 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1458,7 +1503,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1466,7 +1511,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="149">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1791,23 +1836,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="1" fillId="7" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1819,11 +1856,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="7" borderId="22" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1831,7 +1864,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="7" borderId="23" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="7" borderId="23" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1847,7 +1880,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1859,23 +1892,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="27" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="27" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1899,19 +1928,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="8" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="8" borderId="26" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="8" borderId="27" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="8" borderId="27" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1923,11 +1948,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1943,7 +1964,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1955,7 +1976,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1967,19 +1988,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="8" borderId="30" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="30" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="8" borderId="30" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="8" borderId="31" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="8" borderId="31" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1999,15 +2016,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="7" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="7" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="7" borderId="0" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2027,15 +2040,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="36" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="36" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="36" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="37" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="37" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2043,7 +2052,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2059,7 +2068,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2067,7 +2076,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="7" borderId="8" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="40" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="7" borderId="8" xfId="19" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2085,6 +2098,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2129,7 +2150,6 @@
     <dxf>
       <font>
         <name val="Arial"/>
-        <charset val="1"/>
         <family val="0"/>
       </font>
       <numFmt numFmtId="164" formatCode="@"/>
@@ -2142,7 +2162,6 @@
     <dxf>
       <font>
         <name val="Arial"/>
-        <charset val="1"/>
         <family val="0"/>
       </font>
       <numFmt numFmtId="164" formatCode="@"/>
@@ -2155,7 +2174,6 @@
     <dxf>
       <font>
         <name val="Arial"/>
-        <charset val="1"/>
         <family val="0"/>
       </font>
       <numFmt numFmtId="164" formatCode="@"/>
@@ -2276,17 +2294,17 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -2320,7 +2338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
@@ -2331,7 +2349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -2348,7 +2366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>16</v>
       </c>
@@ -2362,7 +2380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>19</v>
       </c>
@@ -2405,14 +2423,14 @@
   </sheetPr>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
@@ -2420,7 +2438,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="2" width="40.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4992,15 +5010,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
@@ -5275,17 +5293,17 @@
   </sheetPr>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.7"/>
@@ -7754,14 +7772,14 @@
   </sheetPr>
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
@@ -7769,7 +7787,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="2" width="40.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
         <v>25</v>
       </c>
@@ -9251,15 +9269,15 @@
   </sheetPr>
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="11.99"/>
@@ -9531,20 +9549,20 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="7" style="5" width="8.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="58.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="7"/>
@@ -9552,7 +9570,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="76" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="76" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="76" t="s">
         <v>87</v>
       </c>
@@ -11860,15 +11878,15 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
@@ -12300,27 +12318,27 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="78" width="58.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="78" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="76" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="76" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="76" t="s">
         <v>87</v>
       </c>
@@ -12525,7 +12543,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>230</v>
       </c>
@@ -12551,7 +12569,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>232</v>
       </c>
@@ -12577,7 +12595,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>233</v>
       </c>
@@ -12681,7 +12699,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>235</v>
       </c>
@@ -12707,7 +12725,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>191</v>
       </c>
@@ -12733,7 +12751,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>239</v>
       </c>
@@ -12978,1477 +12996,1477 @@
   </sheetPr>
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="78" width="58.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="81" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="82" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="82" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="83" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="84" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="85" width="2.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="78" width="58.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="5" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="81" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="81" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="81" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="82" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="83" width="2.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="94" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86" t="s">
+    <row r="1" s="91" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="85" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="85" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="85" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="I1" s="86" t="s">
         <v>246</v>
       </c>
-      <c r="J1" s="87" t="s">
+      <c r="J1" s="85" t="s">
         <v>247</v>
       </c>
-      <c r="K1" s="89" t="s">
+      <c r="K1" s="87" t="s">
         <v>248</v>
       </c>
-      <c r="L1" s="89" t="s">
+      <c r="L1" s="87" t="s">
         <v>249</v>
       </c>
-      <c r="M1" s="90" t="s">
+      <c r="M1" s="87" t="s">
         <v>250</v>
       </c>
-      <c r="N1" s="91" t="s">
+      <c r="N1" s="88" t="s">
         <v>251</v>
       </c>
-      <c r="O1" s="92"/>
-      <c r="P1" s="87" t="s">
+      <c r="O1" s="89"/>
+      <c r="P1" s="85" t="s">
         <v>252</v>
       </c>
-      <c r="Q1" s="87" t="s">
+      <c r="Q1" s="85" t="s">
         <v>253</v>
       </c>
-      <c r="R1" s="87" t="s">
+      <c r="R1" s="85" t="s">
         <v>254</v>
       </c>
-      <c r="S1" s="87" t="s">
+      <c r="S1" s="85" t="s">
         <v>255</v>
       </c>
-      <c r="T1" s="93" t="s">
+      <c r="T1" s="90" t="s">
         <v>256</v>
       </c>
-      <c r="AME1" s="95"/>
-      <c r="AMF1" s="95"/>
-      <c r="AMG1" s="95"/>
-      <c r="AMH1" s="95"/>
-      <c r="AMI1" s="95"/>
-      <c r="AMJ1" s="95"/>
+      <c r="AME1" s="92"/>
+      <c r="AMF1" s="92"/>
+      <c r="AMG1" s="92"/>
+      <c r="AMH1" s="92"/>
+      <c r="AMI1" s="92"/>
+      <c r="AMJ1" s="92"/>
     </row>
     <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="93" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="97" t="s">
+      <c r="B2" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="98" t="s">
+      <c r="E2" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="99" t="n">
+      <c r="I2" s="96" t="n">
         <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C2-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J2" s="97" t="n">
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J2" s="94" t="n">
         <f aca="false">(-$T$2-4+$R$2+F2)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K2" s="97" t="n">
+        <f aca="false">I2*(1-(_xlfn.BINOM.DIST(0,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L2" s="97" t="n">
+        <f aca="false">I2*(_xlfn.BINOM.DIST(2,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M2" s="97" t="n">
+        <f aca="false">I2*(_xlfn.BINOM.DIST(2,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="98" t="n">
+        <f aca="false">(K2-L2)*E2+(L2-M2)*E2*2+M2*E2*3</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="P2" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="R2" s="94" t="n">
         <v>2</v>
       </c>
-      <c r="K2" s="100" t="n">
-        <f aca="false">I2*(1-(_xlfn.BINOM.DIST(0,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L2" s="100" t="n">
-        <f aca="false">I2*(_xlfn.BINOM.DIST(2,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M2" s="101" t="n">
-        <f aca="false">I2*(_xlfn.BINOM.DIST(2,2,IF(J2&lt;1, 11, IF(J2&gt;11, 1, 12-J2))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J2&lt;1, $Q$2-1, IF(J2&gt;($Q$2-1), 0, IF(J2&gt;11, 1, $Q$2-J2)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N2" s="102" t="n">
-        <f aca="false">(K2-L2)*E2+(L2-M2)*E2*2+M2*E2*3</f>
-        <v>1.83767361111111</v>
-      </c>
-      <c r="P2" s="97" t="n">
+      <c r="S2" s="94" t="n">
+        <v>22</v>
+      </c>
+      <c r="T2" s="99" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="100" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="102"/>
+      <c r="H3" s="103" t="s">
+        <v>222</v>
+      </c>
+      <c r="I3" s="104" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J3" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F3)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K3" s="105" t="n">
+        <f aca="false">I3*(1-(_xlfn.BINOM.DIST(0,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L3" s="105" t="n">
+        <f aca="false">I3*(_xlfn.BINOM.DIST(2,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M3" s="105" t="n">
+        <f aca="false">I3*(_xlfn.BINOM.DIST(2,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="106" t="n">
+        <f aca="false">(K3-L3)*E3+(L3-M3)*E3*2+M3*E3*3</f>
+        <v>0.712962962962963</v>
+      </c>
+      <c r="O3" s="83"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="101"/>
+      <c r="S3" s="101"/>
+      <c r="T3" s="107"/>
+    </row>
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="95" t="s">
+        <v>258</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>224</v>
+      </c>
+      <c r="I4" s="109" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J4" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F4)*-1</f>
         <v>5</v>
       </c>
-      <c r="Q2" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="R2" s="97" t="n">
+      <c r="K4" s="97" t="n">
+        <f aca="false">I4*(1-(_xlfn.BINOM.DIST(0,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L4" s="97" t="n">
+        <f aca="false">I4*(_xlfn.BINOM.DIST(2,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M4" s="97" t="n">
+        <f aca="false">I4*(_xlfn.BINOM.DIST(2,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N4" s="98" t="n">
+        <f aca="false">(K4-L4)*E4+(L4-M4)*E4*2+M4*E4*3</f>
+        <v>0.950617283950617</v>
+      </c>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="99"/>
+    </row>
+    <row r="5" s="108" customFormat="true" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="101" t="n">
         <v>2</v>
       </c>
-      <c r="S2" s="97" t="n">
-        <v>18</v>
-      </c>
-      <c r="T2" s="103" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="104" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="105" t="s">
+      <c r="F5" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="110" t="s">
+        <v>225</v>
+      </c>
+      <c r="H5" s="101" t="s">
+        <v>224</v>
+      </c>
+      <c r="I5" s="104" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J5" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F5)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K5" s="105" t="n">
+        <f aca="false">I5*(1-(_xlfn.BINOM.DIST(0,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L5" s="105" t="n">
+        <f aca="false">I5*(_xlfn.BINOM.DIST(2,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M5" s="105" t="n">
+        <f aca="false">I5*(_xlfn.BINOM.DIST(2,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N5" s="106" t="n">
+        <f aca="false">(K5-L5)*E5+(L5-M5)*E5*2+M5*E5*3</f>
+        <v>0.950617283950617</v>
+      </c>
+      <c r="O5" s="83"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="101"/>
+      <c r="S5" s="101"/>
+      <c r="T5" s="107"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="93" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="105" t="n">
+      <c r="E6" s="94" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="94" t="s">
+        <v>227</v>
+      </c>
+      <c r="I6" s="109" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-12))/144,0)/$Q$2)</f>
+        <v>0.427083333333333</v>
+      </c>
+      <c r="J6" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F6)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K6" s="97" t="n">
+        <f aca="false">I6*(1-(_xlfn.BINOM.DIST(0,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,1))))</f>
+        <v>0.3203125</v>
+      </c>
+      <c r="L6" s="97" t="n">
+        <f aca="false">I6*(_xlfn.BINOM.DIST(2,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,0))))</f>
+        <v>0.106770833333333</v>
+      </c>
+      <c r="M6" s="97" t="n">
+        <f aca="false">I6*(_xlfn.BINOM.DIST(2,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="98" t="n">
+        <f aca="false">(K6-L6)*E6+(L6-M6)*E6*2+M6*E6*3</f>
+        <v>1.28125</v>
+      </c>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="94"/>
+      <c r="R6" s="94"/>
+      <c r="S6" s="94"/>
+      <c r="T6" s="99"/>
+    </row>
+    <row r="7" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="102" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="101" t="s">
+        <v>228</v>
+      </c>
+      <c r="I7" s="104" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J7" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F7)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K7" s="105" t="n">
+        <f aca="false">I7*(1-(_xlfn.BINOM.DIST(0,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L7" s="105" t="n">
+        <f aca="false">I7*(_xlfn.BINOM.DIST(2,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M7" s="105" t="n">
+        <f aca="false">I7*(_xlfn.BINOM.DIST(2,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N7" s="106" t="n">
+        <f aca="false">(K7-L7)*E7+(L7-M7)*E7*2+M7*E7*3</f>
+        <v>1.42592592592593</v>
+      </c>
+      <c r="O7" s="83"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="101"/>
+      <c r="R7" s="101"/>
+      <c r="S7" s="101"/>
+      <c r="T7" s="107"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="95" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="I8" s="109" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J8" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F8)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K8" s="97" t="n">
+        <f aca="false">I8*(1-(_xlfn.BINOM.DIST(0,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L8" s="97" t="n">
+        <f aca="false">I8*(_xlfn.BINOM.DIST(2,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M8" s="97" t="n">
+        <f aca="false">I8*(_xlfn.BINOM.DIST(2,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="98" t="n">
+        <f aca="false">(K8-L8)*E8+(L8-M8)*E8*2+M8*E8*3</f>
+        <v>1.42592592592593</v>
+      </c>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="94"/>
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="99"/>
+    </row>
+    <row r="9" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="100" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="111" t="s">
+        <v>259</v>
+      </c>
+      <c r="H9" s="112" t="s">
+        <v>227</v>
+      </c>
+      <c r="I9" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-12))/144,0)/$Q$2)</f>
+        <v>0.427083333333333</v>
+      </c>
+      <c r="J9" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F9)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K9" s="105" t="n">
+        <f aca="false">I9*(1-(_xlfn.BINOM.DIST(0,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,1))))</f>
+        <v>0.3203125</v>
+      </c>
+      <c r="L9" s="105" t="n">
+        <f aca="false">I9*(_xlfn.BINOM.DIST(2,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,0))))</f>
+        <v>0.106770833333333</v>
+      </c>
+      <c r="M9" s="105" t="n">
+        <f aca="false">I9*(_xlfn.BINOM.DIST(2,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="106" t="n">
+        <f aca="false">(K9-L9)*E9+(L9-M9)*E9*2+M9*E9*3</f>
+        <v>1.28125</v>
+      </c>
+      <c r="O9" s="83"/>
+      <c r="P9" s="101"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="101"/>
+      <c r="T9" s="107"/>
+    </row>
+    <row r="10" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="100" t="s">
+        <v>260</v>
+      </c>
+      <c r="B10" s="101" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="106"/>
-      <c r="H3" s="107" t="s">
-        <v>222</v>
-      </c>
-      <c r="I3" s="108" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C3-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J3" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F3)*-1</f>
+      <c r="C10" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="111"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-12))/144,0)/$Q$2)</f>
+        <v>0.427083333333333</v>
+      </c>
+      <c r="J10" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F10)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K10" s="105" t="n">
+        <f aca="false">I10*(1-(_xlfn.BINOM.DIST(0,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,1))))</f>
+        <v>0.365294656635802</v>
+      </c>
+      <c r="L10" s="105" t="n">
+        <f aca="false">I10*(_xlfn.BINOM.DIST(2,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,0))))</f>
+        <v>0.17992862654321</v>
+      </c>
+      <c r="M10" s="105" t="n">
+        <f aca="false">I10*(_xlfn.BINOM.DIST(2,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,0)))</f>
+        <v>0.0242211612654321</v>
+      </c>
+      <c r="N10" s="106" t="n">
+        <f aca="false">(K10-L10)*E10+(L10-M10)*E10*2+M10*E10*3</f>
+        <v>2.27777777777778</v>
+      </c>
+      <c r="O10" s="83"/>
+      <c r="P10" s="101"/>
+      <c r="Q10" s="101"/>
+      <c r="R10" s="101"/>
+      <c r="S10" s="101"/>
+      <c r="T10" s="107"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="94" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="114" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="115" t="s">
+        <v>228</v>
+      </c>
+      <c r="I11" s="116" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J11" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F11)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K11" s="97" t="n">
+        <f aca="false">I11*(1-(_xlfn.BINOM.DIST(0,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L11" s="97" t="n">
+        <f aca="false">I11*(_xlfn.BINOM.DIST(2,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M11" s="97" t="n">
+        <f aca="false">I11*(_xlfn.BINOM.DIST(2,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N11" s="98" t="n">
+        <f aca="false">(K11-L11)*E11+(L11-M11)*E11*2+M11*E11*3</f>
+        <v>1.42592592592593</v>
+      </c>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="94"/>
+      <c r="S11" s="94"/>
+      <c r="T11" s="99"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="93" t="s">
+        <v>261</v>
+      </c>
+      <c r="B12" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="94" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="109" t="n">
-        <f aca="false">I3*(1-(_xlfn.BINOM.DIST(0,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L3" s="109" t="n">
-        <f aca="false">I3*(_xlfn.BINOM.DIST(2,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M3" s="110" t="n">
-        <f aca="false">I3*(_xlfn.BINOM.DIST(2,2,IF(J3&lt;1, 11, IF(J3&gt;11, 1, 12-J3))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J3&lt;1, $Q$2-1, IF(J3&gt;($Q$2-1), 0, IF(J3&gt;11, 1, $Q$2-J3)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N3" s="111" t="n">
-        <f aca="false">(K3-L3)*E3+(L3-M3)*E3*2+M3*E3*3</f>
-        <v>3.67534722222222</v>
-      </c>
-      <c r="O3" s="85"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="112"/>
-    </row>
-    <row r="4" customFormat="false" ht="46.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="97" t="s">
+      <c r="G12" s="114"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="116" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J12" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F12)*-1</f>
+        <v>4</v>
+      </c>
+      <c r="K12" s="97" t="n">
+        <f aca="false">I12*(1-(_xlfn.BINOM.DIST(0,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,1))))</f>
+        <v>0.330075445816187</v>
+      </c>
+      <c r="L12" s="97" t="n">
+        <f aca="false">I12*(_xlfn.BINOM.DIST(2,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,0))))</f>
+        <v>0.211248285322359</v>
+      </c>
+      <c r="M12" s="97" t="n">
+        <f aca="false">I12*(_xlfn.BINOM.DIST(2,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,0)))</f>
+        <v>0.0528120713305898</v>
+      </c>
+      <c r="N12" s="98" t="n">
+        <f aca="false">(K12-L12)*E12+(L12-M12)*E12*2+M12*E12*3</f>
+        <v>2.37654320987654</v>
+      </c>
+      <c r="P12" s="94"/>
+      <c r="Q12" s="94"/>
+      <c r="R12" s="94"/>
+      <c r="S12" s="94"/>
+      <c r="T12" s="99"/>
+    </row>
+    <row r="13" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="111" t="s">
+        <v>259</v>
+      </c>
+      <c r="H13" s="112" t="s">
+        <v>229</v>
+      </c>
+      <c r="I13" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J13" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F13)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K13" s="105" t="n">
+        <f aca="false">I13*(1-(_xlfn.BINOM.DIST(0,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L13" s="105" t="n">
+        <f aca="false">I13*(_xlfn.BINOM.DIST(2,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M13" s="105" t="n">
+        <f aca="false">I13*(_xlfn.BINOM.DIST(2,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="106" t="n">
+        <f aca="false">(K13-L13)*E13+(L13-M13)*E13*2+M13*E13*3</f>
+        <v>1.42592592592593</v>
+      </c>
+      <c r="O13" s="83"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="107"/>
+    </row>
+    <row r="14" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="100" t="s">
+        <v>262</v>
+      </c>
+      <c r="B14" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="101" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="111"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J14" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F14)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K14" s="105" t="n">
+        <f aca="false">I14*(1-(_xlfn.BINOM.DIST(0,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L14" s="105" t="n">
+        <f aca="false">I14*(_xlfn.BINOM.DIST(2,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M14" s="105" t="n">
+        <f aca="false">I14*(_xlfn.BINOM.DIST(2,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N14" s="106" t="n">
+        <f aca="false">(K14-L14)*E14+(L14-M14)*E14*2+M14*E14*3</f>
+        <v>2.37654320987654</v>
+      </c>
+      <c r="O14" s="83"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
+      <c r="R14" s="101"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="107"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="93" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="94" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="95" t="s">
+        <v>263</v>
+      </c>
+      <c r="H15" s="94" t="s">
+        <v>227</v>
+      </c>
+      <c r="I15" s="109" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-12))/144,0)/$Q$2)</f>
+        <v>0.427083333333333</v>
+      </c>
+      <c r="J15" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F15)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K15" s="97" t="n">
+        <f aca="false">I15*(1-(_xlfn.BINOM.DIST(0,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,1))))</f>
+        <v>0.365294656635802</v>
+      </c>
+      <c r="L15" s="97" t="n">
+        <f aca="false">I15*(_xlfn.BINOM.DIST(2,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,0))))</f>
+        <v>0.17992862654321</v>
+      </c>
+      <c r="M15" s="97" t="n">
+        <f aca="false">I15*(_xlfn.BINOM.DIST(2,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,0)))</f>
+        <v>0.0242211612654321</v>
+      </c>
+      <c r="N15" s="98" t="n">
+        <f aca="false">(K15-L15)*E15+(L15-M15)*E15*2+M15*E15*3</f>
+        <v>2.84722222222222</v>
+      </c>
+      <c r="P15" s="94"/>
+      <c r="Q15" s="94"/>
+      <c r="R15" s="94"/>
+      <c r="S15" s="94"/>
+      <c r="T15" s="99"/>
+    </row>
+    <row r="16" s="108" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="101" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" s="110" t="s">
+        <v>263</v>
+      </c>
+      <c r="H16" s="101" t="s">
+        <v>228</v>
+      </c>
+      <c r="I16" s="104" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J16" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F16)*-1</f>
+        <v>4</v>
+      </c>
+      <c r="K16" s="105" t="n">
+        <f aca="false">I16*(1-(_xlfn.BINOM.DIST(0,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,1))))</f>
+        <v>0.330075445816187</v>
+      </c>
+      <c r="L16" s="105" t="n">
+        <f aca="false">I16*(_xlfn.BINOM.DIST(2,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,0))))</f>
+        <v>0.211248285322359</v>
+      </c>
+      <c r="M16" s="105" t="n">
+        <f aca="false">I16*(_xlfn.BINOM.DIST(2,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,0)))</f>
+        <v>0.0528120713305898</v>
+      </c>
+      <c r="N16" s="106" t="n">
+        <f aca="false">(K16-L16)*E16+(L16-M16)*E16*2+M16*E16*3</f>
+        <v>2.97067901234568</v>
+      </c>
+      <c r="O16" s="83"/>
+      <c r="P16" s="101"/>
+      <c r="Q16" s="101"/>
+      <c r="R16" s="101"/>
+      <c r="S16" s="101"/>
+      <c r="T16" s="107"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="95" t="s">
+        <v>264</v>
+      </c>
+      <c r="H17" s="94" t="s">
+        <v>229</v>
+      </c>
+      <c r="I17" s="109" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J17" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F17)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K17" s="97" t="n">
+        <f aca="false">I17*(1-(_xlfn.BINOM.DIST(0,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L17" s="97" t="n">
+        <f aca="false">I17*(_xlfn.BINOM.DIST(2,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M17" s="97" t="n">
+        <f aca="false">I17*(_xlfn.BINOM.DIST(2,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N17" s="98" t="n">
+        <f aca="false">(K17-L17)*E17+(L17-M17)*E17*2+M17*E17*3</f>
+        <v>2.85185185185185</v>
+      </c>
+      <c r="P17" s="94"/>
+      <c r="Q17" s="94"/>
+      <c r="R17" s="94"/>
+      <c r="S17" s="94"/>
+      <c r="T17" s="99"/>
+    </row>
+    <row r="18" s="108" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="100" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="101" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="H18" s="112" t="s">
+        <v>237</v>
+      </c>
+      <c r="I18" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J18" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F18)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K18" s="105" t="n">
+        <f aca="false">I18*(1-(_xlfn.BINOM.DIST(0,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L18" s="105" t="n">
+        <f aca="false">I18*(_xlfn.BINOM.DIST(2,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M18" s="105" t="n">
+        <f aca="false">I18*(_xlfn.BINOM.DIST(2,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="106" t="n">
+        <f aca="false">(K18-L18)*E18+(L18-M18)*E18*2+M18*E18*3</f>
+        <v>1.06944444444444</v>
+      </c>
+      <c r="O18" s="83"/>
+      <c r="P18" s="101"/>
+      <c r="Q18" s="101"/>
+      <c r="R18" s="101"/>
+      <c r="S18" s="101"/>
+      <c r="T18" s="107"/>
+    </row>
+    <row r="19" s="108" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="100" t="s">
+        <v>266</v>
+      </c>
+      <c r="B19" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="101" t="n">
+        <v>4</v>
+      </c>
+      <c r="F19" s="101" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="111"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J19" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F19)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K19" s="105" t="n">
+        <f aca="false">I19*(1-(_xlfn.BINOM.DIST(0,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L19" s="105" t="n">
+        <f aca="false">I19*(_xlfn.BINOM.DIST(2,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M19" s="105" t="n">
+        <f aca="false">I19*(_xlfn.BINOM.DIST(2,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N19" s="106" t="n">
+        <f aca="false">(K19-L19)*E19+(L19-M19)*E19*2+M19*E19*3</f>
+        <v>1.90123456790123</v>
+      </c>
+      <c r="O19" s="83"/>
+      <c r="P19" s="101"/>
+      <c r="Q19" s="101"/>
+      <c r="R19" s="101"/>
+      <c r="S19" s="101"/>
+      <c r="T19" s="107"/>
+    </row>
+    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="93" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="F20" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="114" t="s">
+        <v>267</v>
+      </c>
+      <c r="H20" s="115" t="s">
+        <v>237</v>
+      </c>
+      <c r="I20" s="116" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J20" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F20)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K20" s="97" t="n">
+        <f aca="false">I20*(1-(_xlfn.BINOM.DIST(0,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L20" s="97" t="n">
+        <f aca="false">I20*(_xlfn.BINOM.DIST(2,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M20" s="97" t="n">
+        <f aca="false">I20*(_xlfn.BINOM.DIST(2,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N20" s="98" t="n">
+        <f aca="false">(K20-L20)*E20+(L20-M20)*E20*2+M20*E20*3</f>
+        <v>1.90123456790123</v>
+      </c>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="94"/>
+      <c r="S20" s="94"/>
+      <c r="T20" s="99"/>
+    </row>
+    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="93" t="s">
+        <v>268</v>
+      </c>
+      <c r="B21" s="94" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="94" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="94" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" s="94" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" s="114"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="116" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J21" s="94" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F21)*-1</f>
+        <v>4</v>
+      </c>
+      <c r="K21" s="97" t="n">
+        <f aca="false">I21*(1-(_xlfn.BINOM.DIST(0,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,1))))</f>
+        <v>0.330075445816187</v>
+      </c>
+      <c r="L21" s="97" t="n">
+        <f aca="false">I21*(_xlfn.BINOM.DIST(2,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,0))))</f>
+        <v>0.211248285322359</v>
+      </c>
+      <c r="M21" s="97" t="n">
+        <f aca="false">I21*(_xlfn.BINOM.DIST(2,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,0)))</f>
+        <v>0.0528120713305898</v>
+      </c>
+      <c r="N21" s="98" t="n">
+        <f aca="false">(K21-L21)*E21+(L21-M21)*E21*2+M21*E21*3</f>
+        <v>3.56481481481481</v>
+      </c>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="94"/>
+      <c r="R21" s="94"/>
+      <c r="S21" s="94"/>
+      <c r="T21" s="99"/>
+    </row>
+    <row r="22" s="108" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="101" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="111" t="s">
+        <v>270</v>
+      </c>
+      <c r="H22" s="112" t="s">
+        <v>237</v>
+      </c>
+      <c r="I22" s="113" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J22" s="101" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F22)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K22" s="105" t="n">
+        <f aca="false">I22*(1-(_xlfn.BINOM.DIST(0,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L22" s="105" t="n">
+        <f aca="false">I22*(_xlfn.BINOM.DIST(2,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M22" s="105" t="n">
+        <f aca="false">I22*(_xlfn.BINOM.DIST(2,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="106" t="n">
+        <f aca="false">(K22-L22)*E22+(L22-M22)*E22*2+M22*E22*3</f>
+        <v>0.712962962962963</v>
+      </c>
+      <c r="O22" s="83"/>
+      <c r="P22" s="101"/>
+      <c r="Q22" s="101"/>
+      <c r="R22" s="101"/>
+      <c r="S22" s="101"/>
+      <c r="T22" s="107"/>
+    </row>
+    <row r="23" s="108" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="117" t="s">
+        <v>271</v>
+      </c>
+      <c r="B23" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="118" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="118" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" s="118" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="111"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="119" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J23" s="118" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F23)*-1</f>
+        <v>5</v>
+      </c>
+      <c r="K23" s="120" t="n">
+        <f aca="false">I23*(1-(_xlfn.BINOM.DIST(0,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,1))))</f>
+        <v>0.304907193072702</v>
+      </c>
+      <c r="L23" s="120" t="n">
+        <f aca="false">I23*(_xlfn.BINOM.DIST(2,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,0))))</f>
+        <v>0.150184327846365</v>
+      </c>
+      <c r="M23" s="120" t="n">
+        <f aca="false">I23*(_xlfn.BINOM.DIST(2,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,0)))</f>
+        <v>0.0202171210562414</v>
+      </c>
+      <c r="N23" s="121" t="n">
+        <f aca="false">(K23-L23)*E23+(L23-M23)*E23*2+M23*E23*3</f>
+        <v>1.42592592592593</v>
+      </c>
+      <c r="O23" s="83"/>
+      <c r="P23" s="118"/>
+      <c r="Q23" s="118"/>
+      <c r="R23" s="118"/>
+      <c r="S23" s="118"/>
+      <c r="T23" s="122"/>
+    </row>
+    <row r="24" s="124" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="123"/>
+      <c r="G24" s="125"/>
+      <c r="I24" s="126"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="127"/>
+      <c r="O24" s="83"/>
+      <c r="T24" s="128"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="129" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="130" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="130" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="97" t="n">
+      <c r="E25" s="130" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" s="130" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="131" t="s">
+        <v>272</v>
+      </c>
+      <c r="H25" s="130" t="s">
+        <v>241</v>
+      </c>
+      <c r="I25" s="96" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J25" s="130" t="n">
+        <f aca="false">(-$T$2-4+$R$2+F25)*-1</f>
+        <v>6</v>
+      </c>
+      <c r="K25" s="132" t="n">
+        <f aca="false">I25*(1-(_xlfn.BINOM.DIST(0,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,1))))</f>
+        <v>0.267361111111111</v>
+      </c>
+      <c r="L25" s="132" t="n">
+        <f aca="false">I25*(_xlfn.BINOM.DIST(2,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,0))))</f>
+        <v>0.0891203703703704</v>
+      </c>
+      <c r="M25" s="132" t="n">
+        <f aca="false">I25*(_xlfn.BINOM.DIST(2,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,0)))</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="133" t="n">
+        <f aca="false">(K25-L25)*E25+(L25-M25)*E25*2+M25*E25*3</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="P25" s="130"/>
+      <c r="Q25" s="130"/>
+      <c r="R25" s="130"/>
+      <c r="S25" s="130"/>
+      <c r="T25" s="134"/>
+    </row>
+    <row r="26" s="108" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="100" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="101" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="114" t="s">
-        <v>258</v>
-      </c>
-      <c r="H4" s="97" t="s">
-        <v>224</v>
-      </c>
-      <c r="I4" s="115" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C4-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J4" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F4)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K4" s="100" t="n">
-        <f aca="false">I4*(1-(_xlfn.BINOM.DIST(0,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L4" s="100" t="n">
-        <f aca="false">I4*(_xlfn.BINOM.DIST(2,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M4" s="101" t="n">
-        <f aca="false">I4*(_xlfn.BINOM.DIST(2,2,IF(J4&lt;1, 11, IF(J4&gt;11, 1, 12-J4))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J4&lt;1, $Q$2-1, IF(J4&gt;($Q$2-1), 0, IF(J4&gt;11, 1, $Q$2-J4)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N4" s="102" t="n">
-        <f aca="false">(K4-L4)*E4+(L4-M4)*E4*2+M4*E4*3</f>
-        <v>4.11892361111111</v>
-      </c>
-      <c r="P4" s="97"/>
-      <c r="Q4" s="97"/>
-      <c r="R4" s="97"/>
-      <c r="S4" s="97"/>
-      <c r="T4" s="103"/>
-    </row>
-    <row r="5" s="113" customFormat="true" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="104" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="105" t="s">
+      <c r="C26" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="116" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="105" t="s">
-        <v>224</v>
-      </c>
-      <c r="I5" s="108" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C5-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J5" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F5)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K5" s="109" t="n">
-        <f aca="false">I5*(1-(_xlfn.BINOM.DIST(0,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L5" s="109" t="n">
-        <f aca="false">I5*(_xlfn.BINOM.DIST(2,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M5" s="110" t="n">
-        <f aca="false">I5*(_xlfn.BINOM.DIST(2,2,IF(J5&lt;1, 11, IF(J5&gt;11, 1, 12-J5))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J5&lt;1, $Q$2-1, IF(J5&gt;($Q$2-1), 0, IF(J5&gt;11, 1, $Q$2-J5)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N5" s="111" t="n">
-        <f aca="false">(K5-L5)*E5+(L5-M5)*E5*2+M5*E5*3</f>
-        <v>4.11892361111111</v>
-      </c>
-      <c r="O5" s="85"/>
-      <c r="P5" s="105"/>
-      <c r="Q5" s="105"/>
-      <c r="R5" s="105"/>
-      <c r="S5" s="105"/>
-      <c r="T5" s="112"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="96" t="s">
-        <v>226</v>
-      </c>
-      <c r="B6" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="97" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="97" t="n">
+      <c r="E26" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="110" t="s">
+        <v>272</v>
+      </c>
+      <c r="H26" s="101" t="s">
+        <v>241</v>
+      </c>
+      <c r="I26" s="135" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J26" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="K26" s="135" t="s">
+        <v>213</v>
+      </c>
+      <c r="L26" s="135" t="s">
+        <v>213</v>
+      </c>
+      <c r="M26" s="135" t="s">
+        <v>213</v>
+      </c>
+      <c r="N26" s="101" t="s">
+        <v>213</v>
+      </c>
+      <c r="O26" s="83"/>
+      <c r="P26" s="101"/>
+      <c r="Q26" s="101"/>
+      <c r="R26" s="101"/>
+      <c r="S26" s="101"/>
+      <c r="T26" s="107"/>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="136" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="137" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="114" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="I6" s="115" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C6-12))/144,0)/$Q$2)</f>
-        <v>0.8125</v>
-      </c>
-      <c r="J6" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F6)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K6" s="100" t="n">
-        <f aca="false">I6*(1-(_xlfn.BINOM.DIST(0,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,1))))</f>
-        <v>0.806857638888889</v>
-      </c>
-      <c r="L6" s="100" t="n">
-        <f aca="false">I6*(_xlfn.BINOM.DIST(2,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,0))))</f>
-        <v>0.733506944444444</v>
-      </c>
-      <c r="M6" s="101" t="n">
-        <f aca="false">I6*(_xlfn.BINOM.DIST(2,2,IF(J6&lt;1, 11, IF(J6&gt;11, 1, 12-J6))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J6&lt;1, $Q$2-1, IF(J6&gt;($Q$2-1), 0, IF(J6&gt;11, 1, $Q$2-J6)))/$Q$2,0)))</f>
-        <v>0.423177083333333</v>
-      </c>
-      <c r="N6" s="102" t="n">
-        <f aca="false">(K6-L6)*E6+(L6-M6)*E6*2+M6*E6*3</f>
-        <v>5.890625</v>
-      </c>
-      <c r="P6" s="97"/>
-      <c r="Q6" s="97"/>
-      <c r="R6" s="97"/>
-      <c r="S6" s="97"/>
-      <c r="T6" s="103"/>
-    </row>
-    <row r="7" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="104" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="105" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="105" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="106" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="105" t="s">
-        <v>228</v>
-      </c>
-      <c r="I7" s="108" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C7-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J7" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F7)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K7" s="109" t="n">
-        <f aca="false">I7*(1-(_xlfn.BINOM.DIST(0,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L7" s="109" t="n">
-        <f aca="false">I7*(_xlfn.BINOM.DIST(2,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M7" s="110" t="n">
-        <f aca="false">I7*(_xlfn.BINOM.DIST(2,2,IF(J7&lt;1, 11, IF(J7&gt;11, 1, 12-J7))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J7&lt;1, $Q$2-1, IF(J7&gt;($Q$2-1), 0, IF(J7&gt;11, 1, $Q$2-J7)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N7" s="111" t="n">
-        <f aca="false">(K7-L7)*E7+(L7-M7)*E7*2+M7*E7*3</f>
-        <v>6.17838541666667</v>
-      </c>
-      <c r="O7" s="85"/>
-      <c r="P7" s="105"/>
-      <c r="Q7" s="105"/>
-      <c r="R7" s="105"/>
-      <c r="S7" s="105"/>
-      <c r="T7" s="112"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="96" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="97" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="F8" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="114" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="97" t="s">
-        <v>229</v>
-      </c>
-      <c r="I8" s="115" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C8-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J8" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F8)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K8" s="100" t="n">
-        <f aca="false">I8*(1-(_xlfn.BINOM.DIST(0,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L8" s="100" t="n">
-        <f aca="false">I8*(_xlfn.BINOM.DIST(2,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M8" s="101" t="n">
-        <f aca="false">I8*(_xlfn.BINOM.DIST(2,2,IF(J8&lt;1, 11, IF(J8&gt;11, 1, 12-J8))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J8&lt;1, $Q$2-1, IF(J8&gt;($Q$2-1), 0, IF(J8&gt;11, 1, $Q$2-J8)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N8" s="102" t="n">
-        <f aca="false">(K8-L8)*E8+(L8-M8)*E8*2+M8*E8*3</f>
-        <v>7.35069444444444</v>
-      </c>
-      <c r="P8" s="97"/>
-      <c r="Q8" s="97"/>
-      <c r="R8" s="97"/>
-      <c r="S8" s="97"/>
-      <c r="T8" s="103"/>
-    </row>
-    <row r="9" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="104" t="s">
-        <v>230</v>
-      </c>
-      <c r="B9" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="105" t="s">
+      <c r="C27" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="105" t="n">
-        <v>3</v>
-      </c>
-      <c r="F9" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="117" t="s">
-        <v>259</v>
-      </c>
-      <c r="H9" s="118" t="s">
-        <v>227</v>
-      </c>
-      <c r="I9" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C9-12))/144,0)/$Q$2)</f>
-        <v>0.8125</v>
-      </c>
-      <c r="J9" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F9)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K9" s="109" t="n">
-        <f aca="false">I9*(1-(_xlfn.BINOM.DIST(0,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,1))))</f>
-        <v>0.806857638888889</v>
-      </c>
-      <c r="L9" s="109" t="n">
-        <f aca="false">I9*(_xlfn.BINOM.DIST(2,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,0))))</f>
-        <v>0.733506944444444</v>
-      </c>
-      <c r="M9" s="110" t="n">
-        <f aca="false">I9*(_xlfn.BINOM.DIST(2,2,IF(J9&lt;1, 11, IF(J9&gt;11, 1, 12-J9))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J9&lt;1, $Q$2-1, IF(J9&gt;($Q$2-1), 0, IF(J9&gt;11, 1, $Q$2-J9)))/$Q$2,0)))</f>
-        <v>0.423177083333333</v>
-      </c>
-      <c r="N9" s="111" t="n">
-        <f aca="false">(K9-L9)*E9+(L9-M9)*E9*2+M9*E9*3</f>
-        <v>5.890625</v>
-      </c>
-      <c r="O9" s="85"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
-      <c r="T9" s="112"/>
-    </row>
-    <row r="10" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="104" t="s">
-        <v>260</v>
-      </c>
-      <c r="B10" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="105" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="117"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C10-12))/144,0)/$Q$2)</f>
-        <v>0.8125</v>
-      </c>
-      <c r="J10" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F10)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K10" s="109" t="n">
-        <f aca="false">I10*(1-(_xlfn.BINOM.DIST(0,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,1))))</f>
-        <v>0.811794704861111</v>
-      </c>
-      <c r="L10" s="109" t="n">
-        <f aca="false">I10*(_xlfn.BINOM.DIST(2,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,0))))</f>
-        <v>0.791341145833333</v>
-      </c>
-      <c r="M10" s="110" t="n">
-        <f aca="false">I10*(_xlfn.BINOM.DIST(2,2,IF(J10&lt;1, 11, IF(J10&gt;11, 1, 12-J10))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J10&lt;1, $Q$2-1, IF(J10&gt;($Q$2-1), 0, IF(J10&gt;11, 1, $Q$2-J10)))/$Q$2,0)))</f>
-        <v>0.597384982638889</v>
-      </c>
-      <c r="N10" s="111" t="n">
-        <f aca="false">(K10-L10)*E10+(L10-M10)*E10*2+M10*E10*3</f>
-        <v>8.80208333333333</v>
-      </c>
-      <c r="O10" s="85"/>
-      <c r="P10" s="105"/>
-      <c r="Q10" s="105"/>
-      <c r="R10" s="105"/>
-      <c r="S10" s="105"/>
-      <c r="T10" s="112"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="B11" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="97" t="n">
-        <v>3</v>
-      </c>
-      <c r="F11" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="120" t="s">
-        <v>259</v>
-      </c>
-      <c r="H11" s="121" t="s">
-        <v>228</v>
-      </c>
-      <c r="I11" s="122" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C11-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J11" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F11)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K11" s="100" t="n">
-        <f aca="false">I11*(1-(_xlfn.BINOM.DIST(0,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L11" s="100" t="n">
-        <f aca="false">I11*(_xlfn.BINOM.DIST(2,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M11" s="101" t="n">
-        <f aca="false">I11*(_xlfn.BINOM.DIST(2,2,IF(J11&lt;1, 11, IF(J11&gt;11, 1, 12-J11))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J11&lt;1, $Q$2-1, IF(J11&gt;($Q$2-1), 0, IF(J11&gt;11, 1, $Q$2-J11)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N11" s="102" t="n">
-        <f aca="false">(K11-L11)*E11+(L11-M11)*E11*2+M11*E11*3</f>
-        <v>6.17838541666667</v>
-      </c>
-      <c r="P11" s="97"/>
-      <c r="Q11" s="97"/>
-      <c r="R11" s="97"/>
-      <c r="S11" s="97"/>
-      <c r="T11" s="103"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="96" t="s">
-        <v>261</v>
-      </c>
-      <c r="B12" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="97" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="F12" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="120"/>
-      <c r="H12" s="121"/>
-      <c r="I12" s="122" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C12-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J12" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F12)*-1</f>
-        <v>-0</v>
-      </c>
-      <c r="K12" s="100" t="n">
-        <f aca="false">I12*(1-(_xlfn.BINOM.DIST(0,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L12" s="100" t="n">
-        <f aca="false">I12*(_xlfn.BINOM.DIST(2,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M12" s="101" t="n">
-        <f aca="false">I12*(_xlfn.BINOM.DIST(2,2,IF(J12&lt;1, 11, IF(J12&gt;11, 1, 12-J12))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J12&lt;1, $Q$2-1, IF(J12&gt;($Q$2-1), 0, IF(J12&gt;11, 1, $Q$2-J12)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N12" s="102" t="n">
-        <f aca="false">(K12-L12)*E12+(L12-M12)*E12*2+M12*E12*3</f>
-        <v>8.23784722222222</v>
-      </c>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="97"/>
-      <c r="T12" s="103"/>
-    </row>
-    <row r="13" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="104" t="s">
-        <v>233</v>
-      </c>
-      <c r="B13" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="105" t="n">
-        <v>4</v>
-      </c>
-      <c r="F13" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="117" t="s">
-        <v>259</v>
-      </c>
-      <c r="H13" s="118" t="s">
-        <v>229</v>
-      </c>
-      <c r="I13" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C13-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J13" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F13)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K13" s="109" t="n">
-        <f aca="false">I13*(1-(_xlfn.BINOM.DIST(0,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L13" s="109" t="n">
-        <f aca="false">I13*(_xlfn.BINOM.DIST(2,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M13" s="110" t="n">
-        <f aca="false">I13*(_xlfn.BINOM.DIST(2,2,IF(J13&lt;1, 11, IF(J13&gt;11, 1, 12-J13))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J13&lt;1, $Q$2-1, IF(J13&gt;($Q$2-1), 0, IF(J13&gt;11, 1, $Q$2-J13)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N13" s="111" t="n">
-        <f aca="false">(K13-L13)*E13+(L13-M13)*E13*2+M13*E13*3</f>
-        <v>7.35069444444444</v>
-      </c>
-      <c r="O13" s="85"/>
-      <c r="P13" s="105"/>
-      <c r="Q13" s="105"/>
-      <c r="R13" s="105"/>
-      <c r="S13" s="105"/>
-      <c r="T13" s="112"/>
-    </row>
-    <row r="14" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="104" t="s">
-        <v>262</v>
-      </c>
-      <c r="B14" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="105" t="n">
-        <v>5</v>
-      </c>
-      <c r="F14" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="117"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C14-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J14" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F14)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="109" t="n">
-        <f aca="false">I14*(1-(_xlfn.BINOM.DIST(0,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L14" s="109" t="n">
-        <f aca="false">I14*(_xlfn.BINOM.DIST(2,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M14" s="110" t="n">
-        <f aca="false">I14*(_xlfn.BINOM.DIST(2,2,IF(J14&lt;1, 11, IF(J14&gt;11, 1, 12-J14))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J14&lt;1, $Q$2-1, IF(J14&gt;($Q$2-1), 0, IF(J14&gt;11, 1, $Q$2-J14)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N14" s="111" t="n">
-        <f aca="false">(K14-L14)*E14+(L14-M14)*E14*2+M14*E14*3</f>
-        <v>10.2973090277778</v>
-      </c>
-      <c r="O14" s="85"/>
-      <c r="P14" s="105"/>
-      <c r="Q14" s="105"/>
-      <c r="R14" s="105"/>
-      <c r="S14" s="105"/>
-      <c r="T14" s="112"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="96" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="97" t="n">
-        <v>5</v>
-      </c>
-      <c r="F15" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="114" t="s">
-        <v>263</v>
-      </c>
-      <c r="H15" s="97" t="s">
-        <v>227</v>
-      </c>
-      <c r="I15" s="115" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C15-12))/144,0)/$Q$2)</f>
-        <v>0.8125</v>
-      </c>
-      <c r="J15" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F15)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="100" t="n">
-        <f aca="false">I15*(1-(_xlfn.BINOM.DIST(0,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,1))))</f>
-        <v>0.811794704861111</v>
-      </c>
-      <c r="L15" s="100" t="n">
-        <f aca="false">I15*(_xlfn.BINOM.DIST(2,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,0))))</f>
-        <v>0.791341145833333</v>
-      </c>
-      <c r="M15" s="101" t="n">
-        <f aca="false">I15*(_xlfn.BINOM.DIST(2,2,IF(J15&lt;1, 11, IF(J15&gt;11, 1, 12-J15))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J15&lt;1, $Q$2-1, IF(J15&gt;($Q$2-1), 0, IF(J15&gt;11, 1, $Q$2-J15)))/$Q$2,0)))</f>
-        <v>0.597384982638889</v>
-      </c>
-      <c r="N15" s="102" t="n">
-        <f aca="false">(K15-L15)*E15+(L15-M15)*E15*2+M15*E15*3</f>
-        <v>11.0026041666667</v>
-      </c>
-      <c r="P15" s="97"/>
-      <c r="Q15" s="97"/>
-      <c r="R15" s="97"/>
-      <c r="S15" s="97"/>
-      <c r="T15" s="103"/>
-    </row>
-    <row r="16" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="104" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="105" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="105" t="n">
-        <v>5</v>
-      </c>
-      <c r="F16" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" s="116" t="s">
-        <v>263</v>
-      </c>
-      <c r="H16" s="105" t="s">
-        <v>228</v>
-      </c>
-      <c r="I16" s="108" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C16-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J16" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F16)*-1</f>
-        <v>-0</v>
-      </c>
-      <c r="K16" s="109" t="n">
-        <f aca="false">I16*(1-(_xlfn.BINOM.DIST(0,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L16" s="109" t="n">
-        <f aca="false">I16*(_xlfn.BINOM.DIST(2,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M16" s="110" t="n">
-        <f aca="false">I16*(_xlfn.BINOM.DIST(2,2,IF(J16&lt;1, 11, IF(J16&gt;11, 1, 12-J16))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J16&lt;1, $Q$2-1, IF(J16&gt;($Q$2-1), 0, IF(J16&gt;11, 1, $Q$2-J16)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N16" s="111" t="n">
-        <f aca="false">(K16-L16)*E16+(L16-M16)*E16*2+M16*E16*3</f>
-        <v>10.2973090277778</v>
-      </c>
-      <c r="O16" s="85"/>
-      <c r="P16" s="105"/>
-      <c r="Q16" s="105"/>
-      <c r="R16" s="105"/>
-      <c r="S16" s="105"/>
-      <c r="T16" s="112"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="F17" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="114" t="s">
-        <v>264</v>
-      </c>
-      <c r="H17" s="97" t="s">
-        <v>229</v>
-      </c>
-      <c r="I17" s="115" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C17-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J17" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F17)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K17" s="100" t="n">
-        <f aca="false">I17*(1-(_xlfn.BINOM.DIST(0,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L17" s="100" t="n">
-        <f aca="false">I17*(_xlfn.BINOM.DIST(2,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M17" s="101" t="n">
-        <f aca="false">I17*(_xlfn.BINOM.DIST(2,2,IF(J17&lt;1, 11, IF(J17&gt;11, 1, 12-J17))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J17&lt;1, $Q$2-1, IF(J17&gt;($Q$2-1), 0, IF(J17&gt;11, 1, $Q$2-J17)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N17" s="102" t="n">
-        <f aca="false">(K17-L17)*E17+(L17-M17)*E17*2+M17*E17*3</f>
-        <v>12.3567708333333</v>
-      </c>
-      <c r="P17" s="97"/>
-      <c r="Q17" s="97"/>
-      <c r="R17" s="97"/>
-      <c r="S17" s="97"/>
-      <c r="T17" s="103"/>
-    </row>
-    <row r="18" s="113" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="104" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="105" t="n">
-        <v>3</v>
-      </c>
-      <c r="F18" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="117" t="s">
-        <v>265</v>
-      </c>
-      <c r="H18" s="118" t="s">
-        <v>237</v>
-      </c>
-      <c r="I18" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C18-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J18" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F18)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K18" s="109" t="n">
-        <f aca="false">I18*(1-(_xlfn.BINOM.DIST(0,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L18" s="109" t="n">
-        <f aca="false">I18*(_xlfn.BINOM.DIST(2,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M18" s="110" t="n">
-        <f aca="false">I18*(_xlfn.BINOM.DIST(2,2,IF(J18&lt;1, 11, IF(J18&gt;11, 1, 12-J18))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J18&lt;1, $Q$2-1, IF(J18&gt;($Q$2-1), 0, IF(J18&gt;11, 1, $Q$2-J18)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N18" s="111" t="n">
-        <f aca="false">(K18-L18)*E18+(L18-M18)*E18*2+M18*E18*3</f>
-        <v>5.51302083333333</v>
-      </c>
-      <c r="O18" s="85"/>
-      <c r="P18" s="105"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="105"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="112"/>
-    </row>
-    <row r="19" s="113" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="104" t="s">
-        <v>266</v>
-      </c>
-      <c r="B19" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="105" t="n">
-        <v>4</v>
-      </c>
-      <c r="F19" s="105" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="117"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C19-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J19" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F19)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K19" s="109" t="n">
-        <f aca="false">I19*(1-(_xlfn.BINOM.DIST(0,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L19" s="109" t="n">
-        <f aca="false">I19*(_xlfn.BINOM.DIST(2,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M19" s="110" t="n">
-        <f aca="false">I19*(_xlfn.BINOM.DIST(2,2,IF(J19&lt;1, 11, IF(J19&gt;11, 1, 12-J19))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J19&lt;1, $Q$2-1, IF(J19&gt;($Q$2-1), 0, IF(J19&gt;11, 1, $Q$2-J19)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N19" s="111" t="n">
-        <f aca="false">(K19-L19)*E19+(L19-M19)*E19*2+M19*E19*3</f>
-        <v>8.23784722222222</v>
-      </c>
-      <c r="O19" s="85"/>
-      <c r="P19" s="105"/>
-      <c r="Q19" s="105"/>
-      <c r="R19" s="105"/>
-      <c r="S19" s="105"/>
-      <c r="T19" s="112"/>
-    </row>
-    <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="96" t="s">
-        <v>191</v>
-      </c>
-      <c r="B20" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="F20" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="120" t="s">
-        <v>267</v>
-      </c>
-      <c r="H20" s="121" t="s">
-        <v>237</v>
-      </c>
-      <c r="I20" s="122" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C20-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J20" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F20)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K20" s="100" t="n">
-        <f aca="false">I20*(1-(_xlfn.BINOM.DIST(0,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L20" s="100" t="n">
-        <f aca="false">I20*(_xlfn.BINOM.DIST(2,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M20" s="101" t="n">
-        <f aca="false">I20*(_xlfn.BINOM.DIST(2,2,IF(J20&lt;1, 11, IF(J20&gt;11, 1, 12-J20))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J20&lt;1, $Q$2-1, IF(J20&gt;($Q$2-1), 0, IF(J20&gt;11, 1, $Q$2-J20)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N20" s="102" t="n">
-        <f aca="false">(K20-L20)*E20+(L20-M20)*E20*2+M20*E20*3</f>
-        <v>8.23784722222222</v>
-      </c>
-      <c r="P20" s="97"/>
-      <c r="Q20" s="97"/>
-      <c r="R20" s="97"/>
-      <c r="S20" s="97"/>
-      <c r="T20" s="103"/>
-    </row>
-    <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="96" t="s">
-        <v>268</v>
-      </c>
-      <c r="B21" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="F21" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="120"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="122" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C21-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J21" s="97" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F21)*-1</f>
-        <v>-0</v>
-      </c>
-      <c r="K21" s="100" t="n">
-        <f aca="false">I21*(1-(_xlfn.BINOM.DIST(0,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L21" s="100" t="n">
-        <f aca="false">I21*(_xlfn.BINOM.DIST(2,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M21" s="101" t="n">
-        <f aca="false">I21*(_xlfn.BINOM.DIST(2,2,IF(J21&lt;1, 11, IF(J21&gt;11, 1, 12-J21))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J21&lt;1, $Q$2-1, IF(J21&gt;($Q$2-1), 0, IF(J21&gt;11, 1, $Q$2-J21)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N21" s="102" t="n">
-        <f aca="false">(K21-L21)*E21+(L21-M21)*E21*2+M21*E21*3</f>
-        <v>12.3567708333333</v>
-      </c>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="97"/>
-      <c r="R21" s="97"/>
-      <c r="S21" s="97"/>
-      <c r="T21" s="103"/>
-    </row>
-    <row r="22" s="113" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="104" t="s">
-        <v>269</v>
-      </c>
-      <c r="B22" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="105" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="117" t="s">
-        <v>270</v>
-      </c>
-      <c r="H22" s="118" t="s">
-        <v>237</v>
-      </c>
-      <c r="I22" s="119" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C22-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J22" s="105" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F22)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K22" s="109" t="n">
-        <f aca="false">I22*(1-(_xlfn.BINOM.DIST(0,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L22" s="109" t="n">
-        <f aca="false">I22*(_xlfn.BINOM.DIST(2,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M22" s="110" t="n">
-        <f aca="false">I22*(_xlfn.BINOM.DIST(2,2,IF(J22&lt;1, 11, IF(J22&gt;11, 1, 12-J22))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J22&lt;1, $Q$2-1, IF(J22&gt;($Q$2-1), 0, IF(J22&gt;11, 1, $Q$2-J22)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N22" s="111" t="n">
-        <f aca="false">(K22-L22)*E22+(L22-M22)*E22*2+M22*E22*3</f>
-        <v>3.67534722222222</v>
-      </c>
-      <c r="O22" s="85"/>
-      <c r="P22" s="105"/>
-      <c r="Q22" s="105"/>
-      <c r="R22" s="105"/>
-      <c r="S22" s="105"/>
-      <c r="T22" s="112"/>
-    </row>
-    <row r="23" s="113" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="123" t="s">
-        <v>271</v>
-      </c>
-      <c r="B23" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="124" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="124" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="124" t="n">
-        <v>3</v>
-      </c>
-      <c r="F23" s="124" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="117"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="125" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C23-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J23" s="124" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F23)*-1</f>
-        <v>1</v>
-      </c>
-      <c r="K23" s="126" t="n">
-        <f aca="false">I23*(1-(_xlfn.BINOM.DIST(0,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,1))))</f>
-        <v>0.75975658275463</v>
-      </c>
-      <c r="L23" s="126" t="n">
-        <f aca="false">I23*(_xlfn.BINOM.DIST(2,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,0))))</f>
-        <v>0.740614149305556</v>
-      </c>
-      <c r="M23" s="127" t="n">
-        <f aca="false">I23*(_xlfn.BINOM.DIST(2,2,IF(J23&lt;1, 11, IF(J23&gt;11, 1, 12-J23))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J23&lt;1, $Q$2-1, IF(J23&gt;($Q$2-1), 0, IF(J23&gt;11, 1, $Q$2-J23)))/$Q$2,0)))</f>
-        <v>0.55909107349537</v>
-      </c>
-      <c r="N23" s="128" t="n">
-        <f aca="false">(K23-L23)*E23+(L23-M23)*E23*2+M23*E23*3</f>
-        <v>6.17838541666667</v>
-      </c>
-      <c r="O23" s="85"/>
-      <c r="P23" s="124"/>
-      <c r="Q23" s="124"/>
-      <c r="R23" s="124"/>
-      <c r="S23" s="124"/>
-      <c r="T23" s="129"/>
-    </row>
-    <row r="24" s="131" customFormat="true" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="130"/>
-      <c r="G24" s="132"/>
-      <c r="I24" s="133"/>
-      <c r="K24" s="134"/>
-      <c r="L24" s="134"/>
-      <c r="M24" s="85"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="85"/>
-      <c r="T24" s="136"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="137" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="138" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="138" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="138" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="138" t="n">
-        <v>1</v>
-      </c>
-      <c r="F25" s="138" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="139" t="s">
-        <v>272</v>
-      </c>
-      <c r="H25" s="138" t="s">
+      <c r="E27" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="138" t="s">
+        <v>273</v>
+      </c>
+      <c r="H27" s="137" t="s">
         <v>241</v>
       </c>
-      <c r="I25" s="99" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C25-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J25" s="138" t="n">
-        <f aca="false">(-$T$2-4+$R$2+F25)*-1</f>
-        <v>2</v>
-      </c>
-      <c r="K25" s="140" t="n">
-        <f aca="false">I25*(1-(_xlfn.BINOM.DIST(0,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,1)*IF($Q$2&lt;1, 1, _xlfn.BINOM.DIST(0,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,1))))</f>
-        <v>0.75513599537037</v>
-      </c>
-      <c r="L25" s="140" t="n">
-        <f aca="false">I25*(_xlfn.BINOM.DIST(2,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)+(_xlfn.BINOM.DIST(1,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,0))))</f>
-        <v>0.686487268518519</v>
-      </c>
-      <c r="M25" s="141" t="n">
-        <f aca="false">I25*(_xlfn.BINOM.DIST(2,2,IF(J25&lt;1, 11, IF(J25&gt;11, 1, 12-J25))/12,0)*IF($Q$2&lt;1, 0, _xlfn.BINOM.DIST(1,1,IF(J25&lt;1, $Q$2-1, IF(J25&gt;($Q$2-1), 0, IF(J25&gt;11, 1, $Q$2-J25)))/$Q$2,0)))</f>
-        <v>0.396050347222222</v>
-      </c>
-      <c r="N25" s="142" t="n">
-        <f aca="false">(K25-L25)*E25+(L25-M25)*E25*2+M25*E25*3</f>
-        <v>1.83767361111111</v>
-      </c>
-      <c r="P25" s="138"/>
-      <c r="Q25" s="138"/>
-      <c r="R25" s="138"/>
-      <c r="S25" s="138"/>
-      <c r="T25" s="143"/>
-    </row>
-    <row r="26" s="113" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="104" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="105" t="n">
-        <v>2</v>
-      </c>
-      <c r="C26" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="105" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="116" t="s">
-        <v>272</v>
-      </c>
-      <c r="H26" s="105" t="s">
-        <v>241</v>
-      </c>
-      <c r="I26" s="144" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C26-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J26" s="105" t="s">
+      <c r="I27" s="139" t="n">
+        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-12))/144,0)/$Q$2)</f>
+        <v>0.356481481481481</v>
+      </c>
+      <c r="J27" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="105" t="s">
+      <c r="K27" s="141" t="s">
         <v>213</v>
       </c>
-      <c r="L26" s="105" t="s">
+      <c r="L27" s="141" t="s">
         <v>213</v>
       </c>
-      <c r="M26" s="105" t="s">
+      <c r="M27" s="141" t="s">
         <v>213</v>
       </c>
-      <c r="N26" s="105" t="s">
+      <c r="N27" s="140" t="s">
         <v>213</v>
       </c>
-      <c r="O26" s="85"/>
-      <c r="P26" s="105"/>
-      <c r="Q26" s="105"/>
-      <c r="R26" s="105"/>
-      <c r="S26" s="105"/>
-      <c r="T26" s="112"/>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="145" t="s">
-        <v>201</v>
-      </c>
-      <c r="B27" s="146" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" s="146" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="146" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="146" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="146" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" s="147" t="s">
-        <v>273</v>
-      </c>
-      <c r="H27" s="146" t="s">
-        <v>241</v>
-      </c>
-      <c r="I27" s="148" t="n">
-        <f aca="false">IF($Q$2&lt;1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27))/144, IF($Q$2&gt;=1,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-1))/144,0)/$Q$2 + IF($Q$2&gt;=2,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-2))/144,0)/$Q$2 + IF($Q$2&gt;=3,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-3))/144,0)/$Q$2 + IF($Q$2&gt;=4,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-4))/144,0)/$Q$2 + IF($Q$2&gt;=5,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-5))/144,0)/$Q$2 + IF($Q$2&gt;=6,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-6))/144,0)/$Q$2 + IF($Q$2&gt;=7,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-7))/144,0)/$Q$2 + IF($Q$2&gt;=8,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-8))/144,0)/$Q$2 + IF($Q$2&gt;=9,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-9))/144,0)/$Q$2 + IF($Q$2&gt;=10,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-10))/144,0)/$Q$2 + IF($Q$2&gt;=11,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-11))/144,0)/$Q$2 + IF($Q$2&gt;=12,COUNTIF(Sheet5!$B$2:$M$13, "&gt;="&amp;($S$2+1-$P$2-C27-12))/144,0)/$Q$2)</f>
-        <v>0.760416666666667</v>
-      </c>
-      <c r="J27" s="149" t="s">
-        <v>213</v>
-      </c>
-      <c r="K27" s="149" t="s">
-        <v>213</v>
-      </c>
-      <c r="L27" s="149" t="s">
-        <v>213</v>
-      </c>
-      <c r="M27" s="149" t="s">
-        <v>213</v>
-      </c>
-      <c r="N27" s="149" t="s">
-        <v>213</v>
-      </c>
-      <c r="O27" s="150"/>
-      <c r="P27" s="146"/>
-      <c r="Q27" s="146"/>
-      <c r="R27" s="146"/>
-      <c r="S27" s="146"/>
-      <c r="T27" s="151"/>
+      <c r="O27" s="142"/>
+      <c r="P27" s="137"/>
+      <c r="Q27" s="137"/>
+      <c r="R27" s="137"/>
+      <c r="S27" s="137"/>
+      <c r="T27" s="143"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G36" s="152"/>
-      <c r="J36" s="153"/>
+      <c r="G36" s="144"/>
+      <c r="J36" s="145"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="154"/>
+      <c r="E38" s="146"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -14636,20 +14654,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
@@ -14866,7 +14884,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>146</v>
+        <v>280</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
@@ -15012,7 +15030,7 @@
         <v>109</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>-4</v>
@@ -15044,7 +15062,7 @@
         <v>109</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>-4</v>
@@ -15076,7 +15094,7 @@
         <v>109</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>-4</v>
@@ -15108,7 +15126,7 @@
         <v>109</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>-4</v>
@@ -15121,6 +15139,152 @@
       </c>
       <c r="J14" s="0" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G18" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>-3</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>-4</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -15141,11 +15305,11 @@
   </sheetPr>
   <dimension ref="B1:Y27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -17679,13 +17843,113 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="147" width="81.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="19.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="D1" s="147" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="147" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="148" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="147" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" s="147" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="148"/>
+      <c r="B3" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="147" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" s="147" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="148"/>
+      <c r="B4" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="147" t="s">
+        <v>302</v>
+      </c>
+      <c r="E4" s="147" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="148"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.73046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="3.71"/>
   </cols>
@@ -18083,18 +18347,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="2.99"/>
   </cols>
@@ -18648,11 +18912,11 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -20537,11 +20801,11 @@
   </sheetPr>
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.59765625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="4.14"/>
@@ -22870,11 +23134,11 @@
   </sheetPr>
   <dimension ref="B1:W22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="3.57"/>
@@ -24758,11 +25022,11 @@
   </sheetPr>
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.57"/>
@@ -24774,7 +25038,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="2" width="40.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -27180,13 +27444,13 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
@@ -27551,14 +27815,14 @@
   </sheetPr>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="9" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.71"/>
@@ -27566,7 +27830,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="2" width="40.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="2" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -30138,15 +30402,15 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.7"/>

</xml_diff>